<commit_message>
Modified parameters Excel file to account for preeclampsia possible earlier.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
+++ b/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DCEDF3-C1B1-BA46-BEB3-6FA42F4E537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F63E440-46C6-B443-963C-DC38B503308C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="6" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="5" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParameters" sheetId="8" r:id="rId1"/>
@@ -214,7 +214,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={DE156160-DAE5-104A-97C4-22BCF8A70901}</author>
+    <author>tc={54CFE3A7-0706-054E-8B1D-6AB0EB9EF138}</author>
     <author>tc={D8EDDA08-EBB1-6B4B-AA6D-B87645FA66A1}</author>
+    <author>tc={2EC934E8-F0EE-2145-80F2-BC5392BF3766}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{DE156160-DAE5-104A-97C4-22BCF8A70901}">
@@ -229,12 +231,28 @@
     If they don’t have a fetal death, then they have a live birth, so not worth having the live birth column here</t>
       </text>
     </comment>
-    <comment ref="C20" authorId="1" shapeId="0" xr:uid="{D8EDDA08-EBB1-6B4B-AA6D-B87645FA66A1}">
+    <comment ref="C19" authorId="1" shapeId="0" xr:uid="{54CFE3A7-0706-054E-8B1D-6AB0EB9EF138}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Think more on these values and Kim’s comment surrounding preeclampsia and termination early in pregnancy</t>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="2" shapeId="0" xr:uid="{D8EDDA08-EBB1-6B4B-AA6D-B87645FA66A1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Think more on these values and Kim’s comment surrounding preeclampsia and termination early in pregnancy</t>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="3" shapeId="0" xr:uid="{2EC934E8-F0EE-2145-80F2-BC5392BF3766}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
       </text>
     </comment>
   </commentList>
@@ -681,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,11 +716,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,8 +1122,14 @@
   <threadedComment ref="C1" dT="2024-04-19T18:28:34.76" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D8219667-F635-1340-8294-FDDDE70A7E71}" parentId="{DE156160-DAE5-104A-97C4-22BCF8A70901}">
     <text>If they don’t have a fetal death, then they have a live birth, so not worth having the live birth column here</text>
   </threadedComment>
+  <threadedComment ref="C19" dT="2024-04-19T18:26:41.97" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{54CFE3A7-0706-054E-8B1D-6AB0EB9EF138}">
+    <text>Think more on these values and Kim’s comment surrounding preeclampsia and termination early in pregnancy</text>
+  </threadedComment>
   <threadedComment ref="C20" dT="2024-04-19T18:26:41.97" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{D8EDDA08-EBB1-6B4B-AA6D-B87645FA66A1}">
     <text>Think more on these values and Kim’s comment surrounding preeclampsia and termination early in pregnancy</text>
+  </threadedComment>
+  <threadedComment ref="F37" dT="2023-10-20T20:29:33.53" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2EC934E8-F0EE-2145-80F2-BC5392BF3766}">
+    <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2876,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7588,8 +7609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870C18B-8ADE-814A-BF98-16981C435EF7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D124"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7613,14 +7634,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
         <v>0</v>
       </c>
       <c r="D2" s="6">
@@ -7628,14 +7649,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <v>0</v>
       </c>
       <c r="D3" s="6">
@@ -7643,14 +7664,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
         <v>0</v>
       </c>
       <c r="D4" s="6">
@@ -7658,14 +7679,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="6">
         <v>0</v>
       </c>
       <c r="D5" s="6">
@@ -7673,14 +7694,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="6">
         <v>0</v>
       </c>
       <c r="D6" s="6">
@@ -7688,14 +7709,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="6">
         <v>0</v>
       </c>
       <c r="D7" s="6">
@@ -7703,14 +7724,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="6">
         <v>0</v>
       </c>
       <c r="D8" s="6">
@@ -7718,14 +7739,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="6">
         <v>0</v>
       </c>
       <c r="D9" s="6">
@@ -7733,14 +7754,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>0</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="6">
         <v>0</v>
       </c>
       <c r="D10" s="6">
@@ -7748,14 +7769,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>0</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="6">
         <v>0</v>
       </c>
       <c r="D11" s="6">
@@ -7763,14 +7784,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="6">
         <v>0</v>
       </c>
       <c r="D12" s="6">
@@ -7778,14 +7799,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>0</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="6">
         <v>0</v>
       </c>
       <c r="D13" s="6">
@@ -7793,14 +7814,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="6">
         <v>0</v>
       </c>
       <c r="D14" s="6">
@@ -7808,14 +7829,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="6">
         <v>0</v>
       </c>
       <c r="D15" s="6">
@@ -7823,14 +7844,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="6">
         <v>0</v>
       </c>
       <c r="D16" s="6">
@@ -7838,14 +7859,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="6">
         <v>0</v>
       </c>
       <c r="D17" s="6">
@@ -7853,14 +7874,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="6">
         <v>16</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="6">
         <v>0</v>
       </c>
       <c r="D18" s="6">
@@ -7868,29 +7889,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>0</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="14">
-        <v>0</v>
+      <c r="C19" s="6">
+        <v>1E-4</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>0</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="6">
         <v>1E-4</v>
       </c>
       <c r="D20" s="6">
@@ -7898,14 +7919,14 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>0</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="6">
         <v>1E-4</v>
       </c>
       <c r="D21" s="6">
@@ -7913,14 +7934,14 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>0</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="6">
         <v>20</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="6">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="D22" s="6">
@@ -7928,14 +7949,14 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>0</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="6">
         <v>21</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="6">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="D23" s="6">
@@ -7943,14 +7964,14 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="6">
         <v>22</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="D24" s="6">
@@ -7958,14 +7979,14 @@
         <v>2.9999999999999996E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="6">
         <v>23</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="D25" s="6">
@@ -8509,11 +8530,11 @@
       </c>
       <c r="C60" s="7">
         <f>C19*SimParameters!$B$15</f>
-        <v>0</v>
+        <v>1.1000000000000002E-4</v>
       </c>
       <c r="D60" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1000000000000003E-3</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -9165,11 +9186,11 @@
       </c>
       <c r="C101" s="8">
         <f>C19*SimParameters!$B$16</f>
-        <v>0</v>
+        <v>1.2E-4</v>
       </c>
       <c r="D101" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2000000000000001E-3</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -9550,7 +9571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBCDA1E-E196-5243-A50A-855DF45BB886}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -9575,14 +9596,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
         <f>potential_preec_untrt!C2*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9591,14 +9612,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <f>potential_preec_untrt!C3*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9607,14 +9628,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
         <f>potential_preec_untrt!C4*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9623,14 +9644,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="6">
         <f>potential_preec_untrt!C5*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9639,14 +9660,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="6">
         <f>potential_preec_untrt!C6*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9655,14 +9676,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="6">
         <f>potential_preec_untrt!C7*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9671,14 +9692,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="6">
         <f>potential_preec_untrt!C8*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9687,14 +9708,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="6">
         <f>potential_preec_untrt!C9*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9703,14 +9724,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>0</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="6">
         <f>potential_preec_untrt!C10*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9719,14 +9740,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>0</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="6">
         <f>potential_preec_untrt!C11*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9735,14 +9756,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="6">
         <f>potential_preec_untrt!C12*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9751,14 +9772,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>0</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="6">
         <f>potential_preec_untrt!C13*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9767,14 +9788,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="6">
         <f>potential_preec_untrt!C14*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9783,14 +9804,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="6">
         <f>potential_preec_untrt!C15*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9799,14 +9820,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="6">
         <f>potential_preec_untrt!C16*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9815,14 +9836,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="6">
         <f>potential_preec_untrt!C17*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9831,14 +9852,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="6">
         <v>16</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="6">
         <f>potential_preec_untrt!C18*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -9847,30 +9868,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>0</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="6">
         <f>potential_preec_untrt!C19*SimParameters!$B$4</f>
-        <v>0</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>0</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="6">
         <f>potential_preec_untrt!C20*SimParameters!$B$4</f>
         <v>8.0000000000000007E-5</v>
       </c>
@@ -9879,14 +9900,14 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>0</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="6">
         <f>potential_preec_untrt!C21*SimParameters!$B$4</f>
         <v>8.0000000000000007E-5</v>
       </c>
@@ -9895,14 +9916,14 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>0</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="6">
         <v>20</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="6">
         <f>potential_preec_untrt!C22*SimParameters!$B$4</f>
         <v>1.6000000000000001E-4</v>
       </c>
@@ -9911,14 +9932,14 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>0</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="6">
         <v>21</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="6">
         <f>potential_preec_untrt!C23*SimParameters!$B$4</f>
         <v>1.6000000000000001E-4</v>
       </c>
@@ -9927,14 +9948,14 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="6">
         <v>22</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="6">
         <f>potential_preec_untrt!C24*SimParameters!$B$4</f>
         <v>2.3999999999999998E-4</v>
       </c>
@@ -9943,14 +9964,14 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="6">
         <v>23</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="6">
         <f>potential_preec_untrt!C25*SimParameters!$B$4</f>
         <v>2.3999999999999998E-4</v>
       </c>
@@ -9966,7 +9987,7 @@
       <c r="B26" s="6">
         <v>24</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="6">
         <f>potential_preec_untrt!C26*SimParameters!$B$4</f>
         <v>3.2000000000000003E-4</v>
       </c>
@@ -9982,7 +10003,7 @@
       <c r="B27" s="6">
         <v>25</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="6">
         <f>potential_preec_untrt!C27*SimParameters!$B$4</f>
         <v>3.2000000000000003E-4</v>
       </c>
@@ -9998,7 +10019,7 @@
       <c r="B28" s="6">
         <v>26</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="6">
         <f>potential_preec_untrt!C28*SimParameters!$B$4</f>
         <v>4.0000000000000002E-4</v>
       </c>
@@ -10014,7 +10035,7 @@
       <c r="B29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="6">
         <f>potential_preec_untrt!C29*SimParameters!$B$4</f>
         <v>4.7999999999999996E-4</v>
       </c>
@@ -10030,7 +10051,7 @@
       <c r="B30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="6">
         <f>potential_preec_untrt!C30*SimParameters!$B$4</f>
         <v>5.6000000000000006E-4</v>
       </c>
@@ -10046,7 +10067,7 @@
       <c r="B31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="6">
         <f>potential_preec_untrt!C31*SimParameters!$B$4</f>
         <v>6.4000000000000005E-4</v>
       </c>
@@ -10062,7 +10083,7 @@
       <c r="B32" s="6">
         <v>30</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="6">
         <f>potential_preec_untrt!C32*SimParameters!$B$4</f>
         <v>7.2000000000000005E-4</v>
       </c>
@@ -10078,7 +10099,7 @@
       <c r="B33" s="6">
         <v>31</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="6">
         <f>potential_preec_untrt!C33*SimParameters!$B$4</f>
         <v>8.0000000000000004E-4</v>
       </c>
@@ -10094,7 +10115,7 @@
       <c r="B34" s="6">
         <v>32</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="6">
         <f>potential_preec_untrt!C34*SimParameters!$B$4</f>
         <v>1.4400000000000001E-3</v>
       </c>
@@ -10110,7 +10131,7 @@
       <c r="B35" s="6">
         <v>33</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="6">
         <f>potential_preec_untrt!C35*SimParameters!$B$4</f>
         <v>1.6000000000000001E-3</v>
       </c>
@@ -10126,7 +10147,7 @@
       <c r="B36" s="6">
         <v>34</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="6">
         <f>potential_preec_untrt!C36*SimParameters!$B$4</f>
         <v>3.2000000000000002E-3</v>
       </c>
@@ -10142,7 +10163,7 @@
       <c r="B37" s="6">
         <v>35</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="6">
         <f>potential_preec_untrt!C37*SimParameters!$B$4</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -10158,7 +10179,7 @@
       <c r="B38" s="6">
         <v>36</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="6">
         <f>potential_preec_untrt!C38*SimParameters!$B$4</f>
         <v>5.6000000000000008E-3</v>
       </c>
@@ -10174,7 +10195,7 @@
       <c r="B39" s="6">
         <v>37</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="6">
         <f>potential_preec_untrt!C39*SimParameters!$B$4</f>
         <v>6.4000000000000003E-3</v>
       </c>
@@ -10190,7 +10211,7 @@
       <c r="B40" s="6">
         <v>38</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="6">
         <f>potential_preec_untrt!C40*SimParameters!$B$4</f>
         <v>7.2000000000000005E-4</v>
       </c>
@@ -10206,7 +10227,7 @@
       <c r="B41" s="6">
         <v>39</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="6">
         <f>potential_preec_untrt!C41*SimParameters!$B$4</f>
         <v>8.8000000000000005E-3</v>
       </c>
@@ -10222,7 +10243,7 @@
       <c r="B42" s="6">
         <v>40</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="6">
         <f>potential_preec_untrt!C42*SimParameters!$B$4</f>
         <v>1.1200000000000002E-2</v>
       </c>
@@ -10238,7 +10259,7 @@
       <c r="B43" s="7">
         <v>0</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="7">
         <f>potential_preec_untrt!C43*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10254,7 +10275,7 @@
       <c r="B44" s="7">
         <v>1</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="7">
         <f>potential_preec_untrt!C44*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10270,7 +10291,7 @@
       <c r="B45" s="7">
         <v>2</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="7">
         <f>potential_preec_untrt!C45*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10286,7 +10307,7 @@
       <c r="B46" s="7">
         <v>3</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="7">
         <f>potential_preec_untrt!C46*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10302,7 +10323,7 @@
       <c r="B47" s="7">
         <v>4</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="7">
         <f>potential_preec_untrt!C47*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10318,7 +10339,7 @@
       <c r="B48" s="7">
         <v>5</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="7">
         <f>potential_preec_untrt!C48*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10334,7 +10355,7 @@
       <c r="B49" s="7">
         <v>6</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="7">
         <f>potential_preec_untrt!C49*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10350,7 +10371,7 @@
       <c r="B50" s="7">
         <v>7</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="7">
         <f>potential_preec_untrt!C50*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10366,7 +10387,7 @@
       <c r="B51" s="7">
         <v>8</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="7">
         <f>potential_preec_untrt!C51*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10382,7 +10403,7 @@
       <c r="B52" s="7">
         <v>9</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="7">
         <f>potential_preec_untrt!C52*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10398,7 +10419,7 @@
       <c r="B53" s="7">
         <v>10</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="7">
         <f>potential_preec_untrt!C53*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10414,7 +10435,7 @@
       <c r="B54" s="7">
         <v>11</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="7">
         <f>potential_preec_untrt!C54*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10430,7 +10451,7 @@
       <c r="B55" s="7">
         <v>12</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="7">
         <f>potential_preec_untrt!C55*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10446,7 +10467,7 @@
       <c r="B56" s="7">
         <v>13</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="7">
         <f>potential_preec_untrt!C56*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10462,7 +10483,7 @@
       <c r="B57" s="7">
         <v>14</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C57" s="7">
         <f>potential_preec_untrt!C57*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10478,7 +10499,7 @@
       <c r="B58" s="7">
         <v>15</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="7">
         <f>potential_preec_untrt!C58*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10494,7 +10515,7 @@
       <c r="B59" s="7">
         <v>16</v>
       </c>
-      <c r="C59" s="15">
+      <c r="C59" s="7">
         <f>potential_preec_untrt!C59*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10510,13 +10531,13 @@
       <c r="B60" s="7">
         <v>17</v>
       </c>
-      <c r="C60" s="15">
+      <c r="C60" s="7">
         <f>potential_preec_untrt!C60*SimParameters!$B$4</f>
-        <v>0</v>
+        <v>8.8000000000000025E-5</v>
       </c>
       <c r="D60" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.8000000000000025E-4</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -10526,7 +10547,7 @@
       <c r="B61" s="7">
         <v>18</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="7">
         <f>potential_preec_untrt!C61*SimParameters!$B$4</f>
         <v>8.8000000000000025E-5</v>
       </c>
@@ -10542,7 +10563,7 @@
       <c r="B62" s="7">
         <v>19</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="7">
         <f>potential_preec_untrt!C62*SimParameters!$B$4</f>
         <v>8.8000000000000025E-5</v>
       </c>
@@ -10558,7 +10579,7 @@
       <c r="B63" s="7">
         <v>20</v>
       </c>
-      <c r="C63" s="15">
+      <c r="C63" s="7">
         <f>potential_preec_untrt!C63*SimParameters!$B$4</f>
         <v>1.7600000000000005E-4</v>
       </c>
@@ -10574,7 +10595,7 @@
       <c r="B64" s="7">
         <v>21</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="7">
         <f>potential_preec_untrt!C64*SimParameters!$B$4</f>
         <v>1.7600000000000005E-4</v>
       </c>
@@ -10590,7 +10611,7 @@
       <c r="B65" s="7">
         <v>22</v>
       </c>
-      <c r="C65" s="15">
+      <c r="C65" s="7">
         <f>potential_preec_untrt!C65*SimParameters!$B$4</f>
         <v>2.6400000000000002E-4</v>
       </c>
@@ -10606,7 +10627,7 @@
       <c r="B66" s="7">
         <v>23</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="7">
         <f>potential_preec_untrt!C66*SimParameters!$B$4</f>
         <v>2.6400000000000002E-4</v>
       </c>
@@ -10622,7 +10643,7 @@
       <c r="B67" s="7">
         <v>24</v>
       </c>
-      <c r="C67" s="15">
+      <c r="C67" s="7">
         <f>potential_preec_untrt!C67*SimParameters!$B$4</f>
         <v>3.520000000000001E-4</v>
       </c>
@@ -10638,7 +10659,7 @@
       <c r="B68" s="7">
         <v>25</v>
       </c>
-      <c r="C68" s="15">
+      <c r="C68" s="7">
         <f>potential_preec_untrt!C68*SimParameters!$B$4</f>
         <v>3.520000000000001E-4</v>
       </c>
@@ -10654,7 +10675,7 @@
       <c r="B69" s="7">
         <v>26</v>
       </c>
-      <c r="C69" s="15">
+      <c r="C69" s="7">
         <f>potential_preec_untrt!C69*SimParameters!$B$4</f>
         <v>4.4000000000000007E-4</v>
       </c>
@@ -10670,7 +10691,7 @@
       <c r="B70" s="7">
         <v>27</v>
       </c>
-      <c r="C70" s="15">
+      <c r="C70" s="7">
         <f>potential_preec_untrt!C70*SimParameters!$B$4</f>
         <v>5.2800000000000004E-4</v>
       </c>
@@ -10686,7 +10707,7 @@
       <c r="B71" s="7">
         <v>28</v>
       </c>
-      <c r="C71" s="15">
+      <c r="C71" s="7">
         <f>potential_preec_untrt!C71*SimParameters!$B$4</f>
         <v>6.1600000000000012E-4</v>
       </c>
@@ -10702,7 +10723,7 @@
       <c r="B72" s="7">
         <v>29</v>
       </c>
-      <c r="C72" s="15">
+      <c r="C72" s="7">
         <f>potential_preec_untrt!C72*SimParameters!$B$4</f>
         <v>7.040000000000002E-4</v>
       </c>
@@ -10718,7 +10739,7 @@
       <c r="B73" s="7">
         <v>30</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="7">
         <f>potential_preec_untrt!C73*SimParameters!$B$4</f>
         <v>7.9200000000000006E-4</v>
       </c>
@@ -10734,7 +10755,7 @@
       <c r="B74" s="7">
         <v>31</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="7">
         <f>potential_preec_untrt!C74*SimParameters!$B$4</f>
         <v>8.8000000000000014E-4</v>
       </c>
@@ -10750,7 +10771,7 @@
       <c r="B75" s="7">
         <v>32</v>
       </c>
-      <c r="C75" s="15">
+      <c r="C75" s="7">
         <f>potential_preec_untrt!C75*SimParameters!$B$4</f>
         <v>1.5840000000000001E-3</v>
       </c>
@@ -10766,7 +10787,7 @@
       <c r="B76" s="7">
         <v>33</v>
       </c>
-      <c r="C76" s="15">
+      <c r="C76" s="7">
         <f>potential_preec_untrt!C76*SimParameters!$B$4</f>
         <v>1.7600000000000003E-3</v>
       </c>
@@ -10782,7 +10803,7 @@
       <c r="B77" s="7">
         <v>34</v>
       </c>
-      <c r="C77" s="15">
+      <c r="C77" s="7">
         <f>potential_preec_untrt!C77*SimParameters!$B$4</f>
         <v>3.5200000000000006E-3</v>
       </c>
@@ -10798,7 +10819,7 @@
       <c r="B78" s="7">
         <v>35</v>
       </c>
-      <c r="C78" s="15">
+      <c r="C78" s="7">
         <f>potential_preec_untrt!C78*SimParameters!$B$4</f>
         <v>4.4000000000000003E-3</v>
       </c>
@@ -10814,7 +10835,7 @@
       <c r="B79" s="7">
         <v>36</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="7">
         <f>potential_preec_untrt!C79*SimParameters!$B$4</f>
         <v>6.1600000000000014E-3</v>
       </c>
@@ -10830,7 +10851,7 @@
       <c r="B80" s="7">
         <v>37</v>
       </c>
-      <c r="C80" s="15">
+      <c r="C80" s="7">
         <f>potential_preec_untrt!C80*SimParameters!$B$4</f>
         <v>7.0400000000000011E-3</v>
       </c>
@@ -10846,7 +10867,7 @@
       <c r="B81" s="7">
         <v>38</v>
       </c>
-      <c r="C81" s="15">
+      <c r="C81" s="7">
         <f>potential_preec_untrt!C81*SimParameters!$B$4</f>
         <v>7.9200000000000006E-4</v>
       </c>
@@ -10862,7 +10883,7 @@
       <c r="B82" s="7">
         <v>39</v>
       </c>
-      <c r="C82" s="15">
+      <c r="C82" s="7">
         <f>potential_preec_untrt!C82*SimParameters!$B$4</f>
         <v>9.6800000000000011E-3</v>
       </c>
@@ -10878,7 +10899,7 @@
       <c r="B83" s="7">
         <v>40</v>
       </c>
-      <c r="C83" s="15">
+      <c r="C83" s="7">
         <f>potential_preec_untrt!C83*SimParameters!$B$4</f>
         <v>1.2320000000000003E-2</v>
       </c>
@@ -10894,7 +10915,7 @@
       <c r="B84" s="8">
         <v>0</v>
       </c>
-      <c r="C84" s="16">
+      <c r="C84" s="8">
         <f>potential_preec_untrt!C84*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10910,7 +10931,7 @@
       <c r="B85" s="8">
         <v>1</v>
       </c>
-      <c r="C85" s="16">
+      <c r="C85" s="8">
         <f>potential_preec_untrt!C85*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10926,7 +10947,7 @@
       <c r="B86" s="8">
         <v>2</v>
       </c>
-      <c r="C86" s="16">
+      <c r="C86" s="8">
         <f>potential_preec_untrt!C86*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10942,7 +10963,7 @@
       <c r="B87" s="8">
         <v>3</v>
       </c>
-      <c r="C87" s="16">
+      <c r="C87" s="8">
         <f>potential_preec_untrt!C87*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10958,7 +10979,7 @@
       <c r="B88" s="8">
         <v>4</v>
       </c>
-      <c r="C88" s="16">
+      <c r="C88" s="8">
         <f>potential_preec_untrt!C88*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10974,7 +10995,7 @@
       <c r="B89" s="8">
         <v>5</v>
       </c>
-      <c r="C89" s="16">
+      <c r="C89" s="8">
         <f>potential_preec_untrt!C89*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -10990,7 +11011,7 @@
       <c r="B90" s="8">
         <v>6</v>
       </c>
-      <c r="C90" s="16">
+      <c r="C90" s="8">
         <f>potential_preec_untrt!C90*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11006,7 +11027,7 @@
       <c r="B91" s="8">
         <v>7</v>
       </c>
-      <c r="C91" s="16">
+      <c r="C91" s="8">
         <f>potential_preec_untrt!C91*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11022,7 +11043,7 @@
       <c r="B92" s="8">
         <v>8</v>
       </c>
-      <c r="C92" s="16">
+      <c r="C92" s="8">
         <f>potential_preec_untrt!C92*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11038,7 +11059,7 @@
       <c r="B93" s="8">
         <v>9</v>
       </c>
-      <c r="C93" s="16">
+      <c r="C93" s="8">
         <f>potential_preec_untrt!C93*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11054,7 +11075,7 @@
       <c r="B94" s="8">
         <v>10</v>
       </c>
-      <c r="C94" s="16">
+      <c r="C94" s="8">
         <f>potential_preec_untrt!C94*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11070,7 +11091,7 @@
       <c r="B95" s="8">
         <v>11</v>
       </c>
-      <c r="C95" s="16">
+      <c r="C95" s="8">
         <f>potential_preec_untrt!C95*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11086,7 +11107,7 @@
       <c r="B96" s="8">
         <v>12</v>
       </c>
-      <c r="C96" s="16">
+      <c r="C96" s="8">
         <f>potential_preec_untrt!C96*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11102,7 +11123,7 @@
       <c r="B97" s="8">
         <v>13</v>
       </c>
-      <c r="C97" s="16">
+      <c r="C97" s="8">
         <f>potential_preec_untrt!C97*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11118,7 +11139,7 @@
       <c r="B98" s="8">
         <v>14</v>
       </c>
-      <c r="C98" s="16">
+      <c r="C98" s="8">
         <f>potential_preec_untrt!C98*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11134,7 +11155,7 @@
       <c r="B99" s="8">
         <v>15</v>
       </c>
-      <c r="C99" s="16">
+      <c r="C99" s="8">
         <f>potential_preec_untrt!C99*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11150,7 +11171,7 @@
       <c r="B100" s="8">
         <v>16</v>
       </c>
-      <c r="C100" s="16">
+      <c r="C100" s="8">
         <f>potential_preec_untrt!C100*SimParameters!$B$4</f>
         <v>0</v>
       </c>
@@ -11166,13 +11187,13 @@
       <c r="B101" s="8">
         <v>17</v>
       </c>
-      <c r="C101" s="16">
+      <c r="C101" s="8">
         <f>potential_preec_untrt!C101*SimParameters!$B$4</f>
-        <v>0</v>
+        <v>9.6000000000000002E-5</v>
       </c>
       <c r="D101" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.6000000000000002E-4</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -11182,7 +11203,7 @@
       <c r="B102" s="8">
         <v>18</v>
       </c>
-      <c r="C102" s="16">
+      <c r="C102" s="8">
         <f>potential_preec_untrt!C102*SimParameters!$B$4</f>
         <v>9.6000000000000002E-5</v>
       </c>
@@ -11198,7 +11219,7 @@
       <c r="B103" s="8">
         <v>19</v>
       </c>
-      <c r="C103" s="16">
+      <c r="C103" s="8">
         <f>potential_preec_untrt!C103*SimParameters!$B$4</f>
         <v>9.6000000000000002E-5</v>
       </c>
@@ -11214,7 +11235,7 @@
       <c r="B104" s="8">
         <v>20</v>
       </c>
-      <c r="C104" s="16">
+      <c r="C104" s="8">
         <f>potential_preec_untrt!C104*SimParameters!$B$4</f>
         <v>1.92E-4</v>
       </c>
@@ -11230,7 +11251,7 @@
       <c r="B105" s="8">
         <v>21</v>
       </c>
-      <c r="C105" s="16">
+      <c r="C105" s="8">
         <f>potential_preec_untrt!C105*SimParameters!$B$4</f>
         <v>1.92E-4</v>
       </c>
@@ -11246,7 +11267,7 @@
       <c r="B106" s="8">
         <v>22</v>
       </c>
-      <c r="C106" s="16">
+      <c r="C106" s="8">
         <f>potential_preec_untrt!C106*SimParameters!$B$4</f>
         <v>2.8800000000000001E-4</v>
       </c>
@@ -11262,7 +11283,7 @@
       <c r="B107" s="8">
         <v>23</v>
       </c>
-      <c r="C107" s="16">
+      <c r="C107" s="8">
         <f>potential_preec_untrt!C107*SimParameters!$B$4</f>
         <v>2.8800000000000001E-4</v>
       </c>
@@ -11278,7 +11299,7 @@
       <c r="B108" s="8">
         <v>24</v>
       </c>
-      <c r="C108" s="16">
+      <c r="C108" s="8">
         <f>potential_preec_untrt!C108*SimParameters!$B$4</f>
         <v>3.8400000000000001E-4</v>
       </c>
@@ -11294,7 +11315,7 @@
       <c r="B109" s="8">
         <v>25</v>
       </c>
-      <c r="C109" s="16">
+      <c r="C109" s="8">
         <f>potential_preec_untrt!C109*SimParameters!$B$4</f>
         <v>3.8400000000000001E-4</v>
       </c>
@@ -11310,7 +11331,7 @@
       <c r="B110" s="8">
         <v>26</v>
       </c>
-      <c r="C110" s="16">
+      <c r="C110" s="8">
         <f>potential_preec_untrt!C110*SimParameters!$B$4</f>
         <v>4.7999999999999996E-4</v>
       </c>
@@ -11326,7 +11347,7 @@
       <c r="B111" s="8">
         <v>27</v>
       </c>
-      <c r="C111" s="16">
+      <c r="C111" s="8">
         <f>potential_preec_untrt!C111*SimParameters!$B$4</f>
         <v>5.7600000000000001E-4</v>
       </c>
@@ -11342,7 +11363,7 @@
       <c r="B112" s="8">
         <v>28</v>
       </c>
-      <c r="C112" s="16">
+      <c r="C112" s="8">
         <f>potential_preec_untrt!C112*SimParameters!$B$4</f>
         <v>6.7199999999999996E-4</v>
       </c>
@@ -11358,7 +11379,7 @@
       <c r="B113" s="8">
         <v>29</v>
       </c>
-      <c r="C113" s="16">
+      <c r="C113" s="8">
         <f>potential_preec_untrt!C113*SimParameters!$B$4</f>
         <v>7.6800000000000002E-4</v>
       </c>
@@ -11374,7 +11395,7 @@
       <c r="B114" s="8">
         <v>30</v>
       </c>
-      <c r="C114" s="16">
+      <c r="C114" s="8">
         <f>potential_preec_untrt!C114*SimParameters!$B$4</f>
         <v>8.6400000000000008E-4</v>
       </c>
@@ -11390,7 +11411,7 @@
       <c r="B115" s="8">
         <v>31</v>
       </c>
-      <c r="C115" s="16">
+      <c r="C115" s="8">
         <f>potential_preec_untrt!C115*SimParameters!$B$4</f>
         <v>9.5999999999999992E-4</v>
       </c>
@@ -11406,7 +11427,7 @@
       <c r="B116" s="8">
         <v>32</v>
       </c>
-      <c r="C116" s="16">
+      <c r="C116" s="8">
         <f>potential_preec_untrt!C116*SimParameters!$B$4</f>
         <v>1.7280000000000002E-3</v>
       </c>
@@ -11422,7 +11443,7 @@
       <c r="B117" s="8">
         <v>33</v>
       </c>
-      <c r="C117" s="16">
+      <c r="C117" s="8">
         <f>potential_preec_untrt!C117*SimParameters!$B$4</f>
         <v>1.9199999999999998E-3</v>
       </c>
@@ -11438,7 +11459,7 @@
       <c r="B118" s="8">
         <v>34</v>
       </c>
-      <c r="C118" s="16">
+      <c r="C118" s="8">
         <f>potential_preec_untrt!C118*SimParameters!$B$4</f>
         <v>3.8399999999999997E-3</v>
       </c>
@@ -11454,7 +11475,7 @@
       <c r="B119" s="8">
         <v>35</v>
       </c>
-      <c r="C119" s="16">
+      <c r="C119" s="8">
         <f>potential_preec_untrt!C119*SimParameters!$B$4</f>
         <v>4.8000000000000004E-3</v>
       </c>
@@ -11470,7 +11491,7 @@
       <c r="B120" s="8">
         <v>36</v>
       </c>
-      <c r="C120" s="16">
+      <c r="C120" s="8">
         <f>potential_preec_untrt!C120*SimParameters!$B$4</f>
         <v>6.7200000000000003E-3</v>
       </c>
@@ -11486,7 +11507,7 @@
       <c r="B121" s="8">
         <v>37</v>
       </c>
-      <c r="C121" s="16">
+      <c r="C121" s="8">
         <f>potential_preec_untrt!C121*SimParameters!$B$4</f>
         <v>7.6799999999999993E-3</v>
       </c>
@@ -11502,7 +11523,7 @@
       <c r="B122" s="8">
         <v>38</v>
       </c>
-      <c r="C122" s="16">
+      <c r="C122" s="8">
         <f>potential_preec_untrt!C122*SimParameters!$B$4</f>
         <v>8.6400000000000008E-4</v>
       </c>
@@ -11518,7 +11539,7 @@
       <c r="B123" s="8">
         <v>39</v>
       </c>
-      <c r="C123" s="16">
+      <c r="C123" s="8">
         <f>potential_preec_untrt!C123*SimParameters!$B$4</f>
         <v>1.056E-2</v>
       </c>
@@ -11534,7 +11555,7 @@
       <c r="B124" s="8">
         <v>40</v>
       </c>
-      <c r="C124" s="16">
+      <c r="C124" s="8">
         <f>potential_preec_untrt!C124*SimParameters!$B$4</f>
         <v>1.3440000000000001E-2</v>
       </c>
@@ -11550,191 +11571,195 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E248214-C639-FE41-8DE0-FF7112935623}">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>0</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>0</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>0</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="6">
         <v>0</v>
       </c>
     </row>
@@ -11742,10 +11767,10 @@
       <c r="A17" s="6">
         <v>0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="6">
         <v>0</v>
       </c>
     </row>
@@ -11753,10 +11778,10 @@
       <c r="A18" s="6">
         <v>0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="6">
         <v>16</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="6">
         <v>0</v>
       </c>
     </row>
@@ -11764,80 +11789,77 @@
       <c r="A19" s="6">
         <v>0</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>17</v>
       </c>
-      <c r="C19" s="14">
-        <v>0</v>
+      <c r="C19" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>0</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="14">
-        <v>0.6</v>
+      <c r="C20" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>0</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="14">
-        <v>0.55000000000000004</v>
+      <c r="C21" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>0</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="6">
         <v>20</v>
       </c>
-      <c r="C22" s="14">
-        <v>0.45</v>
+      <c r="C22" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>0</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="6">
         <v>21</v>
       </c>
       <c r="C23" s="6">
-        <f>potential_preg_untrt!C23*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="6">
         <v>22</v>
       </c>
       <c r="C24" s="6">
-        <f>potential_preg_untrt!C24*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="6">
         <v>23</v>
       </c>
       <c r="C25" s="6">
-        <f>potential_preg_untrt!C25*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -11924,7 +11946,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>0</v>
       </c>
@@ -11936,7 +11958,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>0</v>
       </c>
@@ -11948,7 +11970,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>0</v>
       </c>
@@ -11960,7 +11982,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>0</v>
       </c>
@@ -11972,7 +11994,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>0</v>
       </c>
@@ -11984,7 +12006,7 @@
         <v>6.3000000000000003E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>0</v>
       </c>
@@ -11996,7 +12018,7 @@
         <v>8.0999999999999996E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>0</v>
       </c>
@@ -12008,7 +12030,7 @@
         <v>1.0499999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>0</v>
       </c>
@@ -12020,7 +12042,7 @@
         <v>1.2600000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>0</v>
       </c>
@@ -12032,7 +12054,7 @@
         <v>1.83E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>0</v>
       </c>
@@ -12044,7 +12066,7 @@
         <v>3.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>1</v>
       </c>
@@ -12056,7 +12078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>1</v>
       </c>
@@ -12068,7 +12090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>1</v>
       </c>
@@ -12080,7 +12102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>1</v>
       </c>
@@ -12092,7 +12114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>1</v>
       </c>
@@ -12104,7 +12126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>1</v>
       </c>
@@ -12256,8 +12278,8 @@
         <v>17</v>
       </c>
       <c r="C60" s="7">
-        <f>C19*SimParameters!$B$9</f>
-        <v>0</v>
+        <f>C19</f>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -12268,8 +12290,8 @@
         <v>18</v>
       </c>
       <c r="C61" s="7">
-        <f>C20*SimParameters!$B$9</f>
-        <v>0.66</v>
+        <f t="shared" ref="C61:C66" si="0">C20</f>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -12280,8 +12302,8 @@
         <v>19</v>
       </c>
       <c r="C62" s="7">
-        <f>C21*SimParameters!$B$9</f>
-        <v>0.60500000000000009</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -12292,8 +12314,8 @@
         <v>20</v>
       </c>
       <c r="C63" s="7">
-        <f>C22*SimParameters!$B$9</f>
-        <v>0.49500000000000005</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -12304,8 +12326,8 @@
         <v>21</v>
       </c>
       <c r="C64" s="7">
-        <f>C23*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -12316,8 +12338,8 @@
         <v>22</v>
       </c>
       <c r="C65" s="7">
-        <f>C24*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -12328,8 +12350,8 @@
         <v>23</v>
       </c>
       <c r="C66" s="7">
-        <f>C25*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -12748,8 +12770,8 @@
         <v>17</v>
       </c>
       <c r="C101" s="8">
-        <f>C19*SimParameters!$B$16</f>
-        <v>0</v>
+        <f>C19</f>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -12760,8 +12782,8 @@
         <v>18</v>
       </c>
       <c r="C102" s="8">
-        <f>C20*SimParameters!$B$16</f>
-        <v>0.72</v>
+        <f t="shared" ref="C102:C107" si="1">C20</f>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -12772,8 +12794,8 @@
         <v>19</v>
       </c>
       <c r="C103" s="8">
-        <f>C21*SimParameters!$B$16</f>
-        <v>0.66</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -12784,8 +12806,8 @@
         <v>20</v>
       </c>
       <c r="C104" s="8">
-        <f>C22*SimParameters!$B$16</f>
-        <v>0.54</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -12796,8 +12818,8 @@
         <v>21</v>
       </c>
       <c r="C105" s="8">
-        <f>C23*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -12808,8 +12830,8 @@
         <v>22</v>
       </c>
       <c r="C106" s="8">
-        <f>C24*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -12820,8 +12842,8 @@
         <v>23</v>
       </c>
       <c r="C107" s="8">
-        <f>C25*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -13038,8 +13060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B660230-52FE-B14B-96EF-BB7257C5F721}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:C124"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13072,7 +13094,7 @@
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
       <c r="C2" s="6">
@@ -13086,7 +13108,7 @@
       <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="6">
@@ -13097,7 +13119,7 @@
       <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="6">
@@ -13108,7 +13130,7 @@
       <c r="A5" s="6">
         <v>0</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="6">
@@ -13122,7 +13144,7 @@
       <c r="A6" s="6">
         <v>0</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
       <c r="C6" s="6">
@@ -13136,7 +13158,7 @@
       <c r="A7" s="6">
         <v>0</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="6">
@@ -13147,7 +13169,7 @@
       <c r="A8" s="6">
         <v>0</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
       <c r="C8" s="6">
@@ -13165,7 +13187,7 @@
       <c r="A9" s="6">
         <v>0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
       <c r="C9" s="6">
@@ -13179,7 +13201,7 @@
       <c r="A10" s="6">
         <v>0</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
       <c r="C10" s="6">
@@ -13190,7 +13212,7 @@
       <c r="A11" s="6">
         <v>0</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="6">
         <v>9</v>
       </c>
       <c r="C11" s="6">
@@ -13201,7 +13223,7 @@
       <c r="A12" s="6">
         <v>0</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
       <c r="C12" s="6">
@@ -13212,7 +13234,7 @@
       <c r="A13" s="6">
         <v>0</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
       <c r="C13" s="6">
@@ -13230,7 +13252,7 @@
       <c r="A14" s="6">
         <v>0</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
       <c r="C14" s="6">
@@ -13241,7 +13263,7 @@
       <c r="A15" s="6">
         <v>0</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
       <c r="C15" s="6">
@@ -13252,7 +13274,7 @@
       <c r="A16" s="6">
         <v>0</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
       <c r="C16" s="6">
@@ -13263,7 +13285,7 @@
       <c r="A17" s="6">
         <v>0</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
       <c r="C17" s="6">
@@ -13277,7 +13299,7 @@
       <c r="A18" s="6">
         <v>0</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="6">
         <v>16</v>
       </c>
       <c r="C18" s="6">
@@ -13291,7 +13313,7 @@
       <c r="A19" s="6">
         <v>0</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>17</v>
       </c>
       <c r="C19" s="6">
@@ -13302,7 +13324,7 @@
       <c r="A20" s="6">
         <v>0</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="6">
         <v>18</v>
       </c>
       <c r="C20" s="6">
@@ -13313,7 +13335,7 @@
       <c r="A21" s="6">
         <v>0</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="6">
         <v>19</v>
       </c>
       <c r="C21" s="6">
@@ -13331,7 +13353,7 @@
       <c r="A22" s="6">
         <v>0</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="6">
         <v>20</v>
       </c>
       <c r="C22" s="6">
@@ -13342,7 +13364,7 @@
       <c r="A23" s="6">
         <v>0</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="6">
         <v>21</v>
       </c>
       <c r="C23" s="6">
@@ -13353,7 +13375,7 @@
       <c r="A24" s="6">
         <v>0</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="6">
         <v>22</v>
       </c>
       <c r="C24" s="6">
@@ -13367,7 +13389,7 @@
       <c r="A25" s="6">
         <v>0</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="6">
         <v>23</v>
       </c>
       <c r="C25" s="6">
@@ -13590,7 +13612,7 @@
       <c r="A43" s="7">
         <v>1</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="7">
         <v>0</v>
       </c>
       <c r="C43" s="7">
@@ -13605,7 +13627,7 @@
       <c r="A44" s="7">
         <v>1</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="7">
         <v>1</v>
       </c>
       <c r="C44" s="7">
@@ -13617,7 +13639,7 @@
       <c r="A45" s="7">
         <v>1</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="7">
         <v>2</v>
       </c>
       <c r="C45" s="7">
@@ -13629,7 +13651,7 @@
       <c r="A46" s="7">
         <v>1</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="7">
         <v>3</v>
       </c>
       <c r="C46" s="7">
@@ -13641,7 +13663,7 @@
       <c r="A47" s="7">
         <v>1</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="7">
         <v>4</v>
       </c>
       <c r="C47" s="7">
@@ -13653,7 +13675,7 @@
       <c r="A48" s="7">
         <v>1</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="7">
         <v>5</v>
       </c>
       <c r="C48" s="7">
@@ -13665,7 +13687,7 @@
       <c r="A49" s="7">
         <v>1</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="7">
         <v>6</v>
       </c>
       <c r="C49" s="7">
@@ -13677,7 +13699,7 @@
       <c r="A50" s="7">
         <v>1</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="7">
         <v>7</v>
       </c>
       <c r="C50" s="7">
@@ -13689,7 +13711,7 @@
       <c r="A51" s="7">
         <v>1</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="7">
         <v>8</v>
       </c>
       <c r="C51" s="7">
@@ -13701,7 +13723,7 @@
       <c r="A52" s="7">
         <v>1</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="7">
         <v>9</v>
       </c>
       <c r="C52" s="7">
@@ -13713,7 +13735,7 @@
       <c r="A53" s="7">
         <v>1</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="7">
         <v>10</v>
       </c>
       <c r="C53" s="7">
@@ -13725,7 +13747,7 @@
       <c r="A54" s="7">
         <v>1</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="7">
         <v>11</v>
       </c>
       <c r="C54" s="7">
@@ -13737,7 +13759,7 @@
       <c r="A55" s="7">
         <v>1</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="7">
         <v>12</v>
       </c>
       <c r="C55" s="7">
@@ -13749,7 +13771,7 @@
       <c r="A56" s="7">
         <v>1</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="7">
         <v>13</v>
       </c>
       <c r="C56" s="7">
@@ -13761,7 +13783,7 @@
       <c r="A57" s="7">
         <v>1</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="7">
         <v>14</v>
       </c>
       <c r="C57" s="7">
@@ -13773,7 +13795,7 @@
       <c r="A58" s="7">
         <v>1</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="7">
         <v>15</v>
       </c>
       <c r="C58" s="7">
@@ -13785,7 +13807,7 @@
       <c r="A59" s="7">
         <v>1</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="7">
         <v>16</v>
       </c>
       <c r="C59" s="7">
@@ -13797,7 +13819,7 @@
       <c r="A60" s="7">
         <v>1</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="7">
         <v>17</v>
       </c>
       <c r="C60" s="7">
@@ -13809,7 +13831,7 @@
       <c r="A61" s="7">
         <v>1</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="7">
         <v>18</v>
       </c>
       <c r="C61" s="7">
@@ -13821,7 +13843,7 @@
       <c r="A62" s="7">
         <v>1</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="7">
         <v>19</v>
       </c>
       <c r="C62" s="7">
@@ -13833,7 +13855,7 @@
       <c r="A63" s="7">
         <v>1</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="7">
         <v>20</v>
       </c>
       <c r="C63" s="7">
@@ -13845,7 +13867,7 @@
       <c r="A64" s="7">
         <v>1</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B64" s="7">
         <v>21</v>
       </c>
       <c r="C64" s="7">
@@ -13857,7 +13879,7 @@
       <c r="A65" s="7">
         <v>1</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="7">
         <v>22</v>
       </c>
       <c r="C65" s="7">
@@ -13869,7 +13891,7 @@
       <c r="A66" s="7">
         <v>1</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="7">
         <v>23</v>
       </c>
       <c r="C66" s="7">
@@ -14085,7 +14107,7 @@
       <c r="A84" s="8">
         <v>2</v>
       </c>
-      <c r="B84" s="16">
+      <c r="B84" s="8">
         <v>0</v>
       </c>
       <c r="C84" s="8">
@@ -14100,7 +14122,7 @@
       <c r="A85" s="8">
         <v>2</v>
       </c>
-      <c r="B85" s="16">
+      <c r="B85" s="8">
         <v>1</v>
       </c>
       <c r="C85" s="8">
@@ -14112,7 +14134,7 @@
       <c r="A86" s="8">
         <v>2</v>
       </c>
-      <c r="B86" s="16">
+      <c r="B86" s="8">
         <v>2</v>
       </c>
       <c r="C86" s="8">
@@ -14124,7 +14146,7 @@
       <c r="A87" s="8">
         <v>2</v>
       </c>
-      <c r="B87" s="16">
+      <c r="B87" s="8">
         <v>3</v>
       </c>
       <c r="C87" s="8">
@@ -14136,7 +14158,7 @@
       <c r="A88" s="8">
         <v>2</v>
       </c>
-      <c r="B88" s="16">
+      <c r="B88" s="8">
         <v>4</v>
       </c>
       <c r="C88" s="8">
@@ -14148,7 +14170,7 @@
       <c r="A89" s="8">
         <v>2</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="8">
         <v>5</v>
       </c>
       <c r="C89" s="8">
@@ -14160,7 +14182,7 @@
       <c r="A90" s="8">
         <v>2</v>
       </c>
-      <c r="B90" s="16">
+      <c r="B90" s="8">
         <v>6</v>
       </c>
       <c r="C90" s="8">
@@ -14172,7 +14194,7 @@
       <c r="A91" s="8">
         <v>2</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="8">
         <v>7</v>
       </c>
       <c r="C91" s="8">
@@ -14184,7 +14206,7 @@
       <c r="A92" s="8">
         <v>2</v>
       </c>
-      <c r="B92" s="16">
+      <c r="B92" s="8">
         <v>8</v>
       </c>
       <c r="C92" s="8">
@@ -14196,7 +14218,7 @@
       <c r="A93" s="8">
         <v>2</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="8">
         <v>9</v>
       </c>
       <c r="C93" s="8">
@@ -14208,7 +14230,7 @@
       <c r="A94" s="8">
         <v>2</v>
       </c>
-      <c r="B94" s="16">
+      <c r="B94" s="8">
         <v>10</v>
       </c>
       <c r="C94" s="8">
@@ -14220,7 +14242,7 @@
       <c r="A95" s="8">
         <v>2</v>
       </c>
-      <c r="B95" s="16">
+      <c r="B95" s="8">
         <v>11</v>
       </c>
       <c r="C95" s="8">
@@ -14232,7 +14254,7 @@
       <c r="A96" s="8">
         <v>2</v>
       </c>
-      <c r="B96" s="16">
+      <c r="B96" s="8">
         <v>12</v>
       </c>
       <c r="C96" s="8">
@@ -14244,7 +14266,7 @@
       <c r="A97" s="8">
         <v>2</v>
       </c>
-      <c r="B97" s="16">
+      <c r="B97" s="8">
         <v>13</v>
       </c>
       <c r="C97" s="8">
@@ -14256,7 +14278,7 @@
       <c r="A98" s="8">
         <v>2</v>
       </c>
-      <c r="B98" s="16">
+      <c r="B98" s="8">
         <v>14</v>
       </c>
       <c r="C98" s="8">
@@ -14268,7 +14290,7 @@
       <c r="A99" s="8">
         <v>2</v>
       </c>
-      <c r="B99" s="16">
+      <c r="B99" s="8">
         <v>15</v>
       </c>
       <c r="C99" s="8">
@@ -14280,7 +14302,7 @@
       <c r="A100" s="8">
         <v>2</v>
       </c>
-      <c r="B100" s="16">
+      <c r="B100" s="8">
         <v>16</v>
       </c>
       <c r="C100" s="8">
@@ -14292,7 +14314,7 @@
       <c r="A101" s="8">
         <v>2</v>
       </c>
-      <c r="B101" s="16">
+      <c r="B101" s="8">
         <v>17</v>
       </c>
       <c r="C101" s="8">
@@ -14304,7 +14326,7 @@
       <c r="A102" s="8">
         <v>2</v>
       </c>
-      <c r="B102" s="16">
+      <c r="B102" s="8">
         <v>18</v>
       </c>
       <c r="C102" s="8">
@@ -14316,7 +14338,7 @@
       <c r="A103" s="8">
         <v>2</v>
       </c>
-      <c r="B103" s="16">
+      <c r="B103" s="8">
         <v>19</v>
       </c>
       <c r="C103" s="8">
@@ -14328,7 +14350,7 @@
       <c r="A104" s="8">
         <v>2</v>
       </c>
-      <c r="B104" s="16">
+      <c r="B104" s="8">
         <v>20</v>
       </c>
       <c r="C104" s="8">
@@ -14340,7 +14362,7 @@
       <c r="A105" s="8">
         <v>2</v>
       </c>
-      <c r="B105" s="16">
+      <c r="B105" s="8">
         <v>21</v>
       </c>
       <c r="C105" s="8">
@@ -14352,7 +14374,7 @@
       <c r="A106" s="8">
         <v>2</v>
       </c>
-      <c r="B106" s="16">
+      <c r="B106" s="8">
         <v>22</v>
       </c>
       <c r="C106" s="8">
@@ -14364,7 +14386,7 @@
       <c r="A107" s="8">
         <v>2</v>
       </c>
-      <c r="B107" s="16">
+      <c r="B107" s="8">
         <v>23</v>
       </c>
       <c r="C107" s="8">

</xml_diff>

<commit_message>
Modified parameter values for simulation.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
+++ b/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F63E440-46C6-B443-963C-DC38B503308C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E3305-9ED0-384D-9049-1FCB026A5D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" firstSheet="1" activeTab="5" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParameters" sheetId="8" r:id="rId1"/>
@@ -52,6 +52,7 @@
     <author>tc={35C57926-D2D1-1E4D-B53B-E5E2E4FD75E7}</author>
     <author>tc={9A5BA4F2-D71D-6E40-92FE-646A717AC649}</author>
     <author>tc={AA203F26-57EB-FD4D-96A8-1E3EC58078F0}</author>
+    <author>tc={2AA8F2D0-6E32-494D-B542-C416DAEFF657}</author>
     <author>tc={BA1965E4-CB1E-A446-858D-2C189AC85BC3}</author>
     <author>tc={73131F6C-4FDD-8242-81D0-C94D07ECA3E3}</author>
     <author>tc={F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}</author>
@@ -83,15 +84,27 @@
     Lowered this slightly from 0.2 to 0.1 to improve sample size.</t>
       </text>
     </comment>
-    <comment ref="C21" authorId="3" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+    <comment ref="C20" authorId="3" shapeId="0" xr:uid="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
+    All the 0.003s — https://stacks.cdc.gov/view/cdc/61387
+Reply:
+    This rate is per live births. Needs to be decreased. Halved</t>
       </text>
     </comment>
-    <comment ref="D26" authorId="4" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
+    <comment ref="C21" authorId="4" shapeId="0" xr:uid="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    All the 0.003s — https://stacks.cdc.gov/view/cdc/61387
+Reply:
+    This rate is per live births. Needs to be decreased. Halved</t>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="5" shapeId="0" xr:uid="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -99,7 +112,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
       </text>
     </comment>
-    <comment ref="C37" authorId="5" shapeId="0" xr:uid="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
+    <comment ref="C37" authorId="6" shapeId="0" xr:uid="{F0934731-78BA-194A-B9CD-EC5F1F6C9CE0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -107,7 +120,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
       </text>
     </comment>
-    <comment ref="D67" authorId="6" shapeId="0" xr:uid="{3BD33B62-4B89-784D-BCF9-57648E8A7B32}">
+    <comment ref="D67" authorId="7" shapeId="0" xr:uid="{3BD33B62-4B89-784D-BCF9-57648E8A7B32}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -115,7 +128,7 @@
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
       </text>
     </comment>
-    <comment ref="D108" authorId="7" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
+    <comment ref="D108" authorId="8" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -699,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -716,8 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,8 +1064,17 @@
   <threadedComment ref="C4" dT="2023-11-27T01:41:40.99" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{AA203F26-57EB-FD4D-96A8-1E3EC58078F0}">
     <text>Lowered this slightly from 0.2 to 0.1 to improve sample size.</text>
   </threadedComment>
+  <threadedComment ref="C20" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+    <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
+  </threadedComment>
+  <threadedComment ref="C20" dT="2024-06-19T20:53:57.65" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{044105F4-3C00-3246-A892-C3EC22945EE2}" parentId="{2AA8F2D0-6E32-494D-B542-C416DAEFF657}">
+    <text>This rate is per live births. Needs to be decreased. Halved</text>
+  </threadedComment>
   <threadedComment ref="C21" dT="2023-10-20T20:32:56.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
     <text>All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</text>
+  </threadedComment>
+  <threadedComment ref="C21" dT="2024-06-19T20:53:57.65" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E51787F8-0032-8642-96CF-65A3841E3202}" parentId="{BA1965E4-CB1E-A446-858D-2C189AC85BC3}">
+    <text>This rate is per live births. Needs to be decreased. Halved</text>
   </threadedComment>
   <threadedComment ref="D26" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{73131F6C-4FDD-8242-81D0-C94D07ECA3E3}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</text>
@@ -2897,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3258,14 +3278,14 @@
         <v>18</v>
       </c>
       <c r="C20" s="6">
-        <v>0.01</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3276,14 +3296,14 @@
         <v>19</v>
       </c>
       <c r="C21" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3294,14 +3314,14 @@
         <v>20</v>
       </c>
       <c r="C22" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D22" s="6">
         <v>0</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3312,14 +3332,14 @@
         <v>21</v>
       </c>
       <c r="C23" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D23" s="6">
         <v>0</v>
       </c>
       <c r="E23" s="6">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3330,14 +3350,14 @@
         <v>22</v>
       </c>
       <c r="C24" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D24" s="6">
         <v>0</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3348,14 +3368,14 @@
         <v>23</v>
       </c>
       <c r="C25" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D25" s="6">
         <v>0</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="0"/>
-        <v>0.997</v>
+        <v>0.99850000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3366,14 +3386,14 @@
         <v>24</v>
       </c>
       <c r="C26" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D26" s="6">
         <v>0.01</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="0"/>
-        <v>0.98699999999999999</v>
+        <v>0.98850000000000005</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3384,14 +3404,14 @@
         <v>25</v>
       </c>
       <c r="C27" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D27" s="6">
         <v>0.01</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" si="0"/>
-        <v>0.98699999999999999</v>
+        <v>0.98850000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3402,14 +3422,14 @@
         <v>26</v>
       </c>
       <c r="C28" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D28" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E28" s="6">
         <f t="shared" si="0"/>
-        <v>0.98199999999999998</v>
+        <v>0.98350000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3420,14 +3440,14 @@
         <v>27</v>
       </c>
       <c r="C29" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D29" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" si="0"/>
-        <v>0.98199999999999998</v>
+        <v>0.98350000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3438,14 +3458,14 @@
         <v>28</v>
       </c>
       <c r="C30" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D30" s="6">
         <v>0.02</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" si="0"/>
-        <v>0.97699999999999998</v>
+        <v>0.97850000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3456,14 +3476,14 @@
         <v>29</v>
       </c>
       <c r="C31" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D31" s="6">
         <v>0.02</v>
       </c>
       <c r="E31" s="6">
         <f t="shared" si="0"/>
-        <v>0.97699999999999998</v>
+        <v>0.97850000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -3474,14 +3494,14 @@
         <v>30</v>
       </c>
       <c r="C32" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D32" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E32" s="6">
         <f t="shared" si="0"/>
-        <v>0.97199999999999998</v>
+        <v>0.97350000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3492,14 +3512,14 @@
         <v>31</v>
       </c>
       <c r="C33" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D33" s="6">
         <v>0.03</v>
       </c>
       <c r="E33" s="6">
         <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
+        <v>0.96850000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3510,14 +3530,14 @@
         <v>32</v>
       </c>
       <c r="C34" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D34" s="6">
         <v>0.09</v>
       </c>
       <c r="E34" s="6">
         <f t="shared" si="0"/>
-        <v>0.90700000000000003</v>
+        <v>0.90850000000000009</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3528,14 +3548,14 @@
         <v>33</v>
       </c>
       <c r="C35" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D35" s="6">
         <v>0.09</v>
       </c>
       <c r="E35" s="6">
         <f t="shared" si="0"/>
-        <v>0.90700000000000003</v>
+        <v>0.90850000000000009</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3546,14 +3566,14 @@
         <v>34</v>
       </c>
       <c r="C36" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D36" s="6">
         <v>0.09</v>
       </c>
       <c r="E36" s="6">
         <f t="shared" si="0"/>
-        <v>0.90700000000000003</v>
+        <v>0.90850000000000009</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4016,14 +4036,14 @@
       </c>
       <c r="C61" s="7">
         <f>C20*SimParameters!B9</f>
-        <v>1.1000000000000001E-2</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D61" s="7">
         <v>0</v>
       </c>
       <c r="E61" s="7">
         <f t="shared" si="1"/>
-        <v>0.98899999999999999</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -4035,14 +4055,14 @@
       </c>
       <c r="C62" s="7">
         <f>C21*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D62" s="7">
         <v>0</v>
       </c>
       <c r="E62" s="7">
         <f t="shared" si="1"/>
-        <v>0.99670000000000003</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -4054,14 +4074,14 @@
       </c>
       <c r="C63" s="7">
         <f>C22*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D63" s="7">
         <v>0</v>
       </c>
       <c r="E63" s="7">
         <f t="shared" si="1"/>
-        <v>0.99670000000000003</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -4073,14 +4093,14 @@
       </c>
       <c r="C64" s="7">
         <f>C23*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D64" s="7">
         <v>0</v>
       </c>
       <c r="E64" s="7">
         <f t="shared" si="1"/>
-        <v>0.99670000000000003</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -4092,14 +4112,14 @@
       </c>
       <c r="C65" s="7">
         <f>C24*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D65" s="7">
         <v>0</v>
       </c>
       <c r="E65" s="7">
         <f t="shared" si="1"/>
-        <v>0.99670000000000003</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4111,14 +4131,14 @@
       </c>
       <c r="C66" s="7">
         <f>C25*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D66" s="7">
         <v>0</v>
       </c>
       <c r="E66" s="7">
         <f t="shared" si="1"/>
-        <v>0.99670000000000003</v>
+        <v>0.99834999999999996</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -4130,14 +4150,14 @@
       </c>
       <c r="C67" s="7">
         <f>C26*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D67" s="7">
         <v>0.01</v>
       </c>
       <c r="E67" s="7">
         <f t="shared" si="1"/>
-        <v>0.98670000000000002</v>
+        <v>0.98834999999999995</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -4149,14 +4169,14 @@
       </c>
       <c r="C68" s="7">
         <f>C27*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D68" s="7">
         <v>0.01</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="1"/>
-        <v>0.98670000000000002</v>
+        <v>0.98834999999999995</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -4168,14 +4188,14 @@
       </c>
       <c r="C69" s="7">
         <f>C28*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D69" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E69" s="7">
         <f t="shared" si="1"/>
-        <v>0.98170000000000002</v>
+        <v>0.98334999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4187,14 +4207,14 @@
       </c>
       <c r="C70" s="7">
         <f>C29*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D70" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="1"/>
-        <v>0.98170000000000002</v>
+        <v>0.98334999999999995</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -4206,14 +4226,14 @@
       </c>
       <c r="C71" s="7">
         <f>C30*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D71" s="7">
         <v>0.02</v>
       </c>
       <c r="E71" s="7">
         <f t="shared" si="1"/>
-        <v>0.97670000000000001</v>
+        <v>0.97834999999999994</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -4225,14 +4245,14 @@
       </c>
       <c r="C72" s="7">
         <f>C31*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D72" s="7">
         <v>0.02</v>
       </c>
       <c r="E72" s="7">
         <f t="shared" si="1"/>
-        <v>0.97670000000000001</v>
+        <v>0.97834999999999994</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -4244,14 +4264,14 @@
       </c>
       <c r="C73" s="7">
         <f>C32*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D73" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E73" s="7">
         <f t="shared" si="1"/>
-        <v>0.97170000000000001</v>
+        <v>0.97334999999999994</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -4263,14 +4283,14 @@
       </c>
       <c r="C74" s="7">
         <f>C33*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D74" s="7">
         <v>0.03</v>
       </c>
       <c r="E74" s="7">
         <f t="shared" si="1"/>
-        <v>0.9667</v>
+        <v>0.96834999999999993</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -4282,14 +4302,14 @@
       </c>
       <c r="C75" s="7">
         <f>C34*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D75" s="7">
         <v>0.09</v>
       </c>
       <c r="E75" s="7">
         <f t="shared" si="1"/>
-        <v>0.90670000000000006</v>
+        <v>0.90834999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -4301,14 +4321,14 @@
       </c>
       <c r="C76" s="7">
         <f>C35*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D76" s="7">
         <v>0.09</v>
       </c>
       <c r="E76" s="7">
         <f t="shared" si="1"/>
-        <v>0.90670000000000006</v>
+        <v>0.90834999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -4320,14 +4340,14 @@
       </c>
       <c r="C77" s="7">
         <f>C36*SimParameters!B9</f>
-        <v>3.3000000000000004E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D77" s="7">
         <v>0.09</v>
       </c>
       <c r="E77" s="7">
         <f t="shared" si="1"/>
-        <v>0.90670000000000006</v>
+        <v>0.90834999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -4795,14 +4815,14 @@
       </c>
       <c r="C102" s="8">
         <f>C20*SimParameters!B10</f>
-        <v>1.2E-2</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D102" s="8">
         <v>0</v>
       </c>
       <c r="E102" s="8">
         <f t="shared" si="2"/>
-        <v>0.98799999999999999</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -4814,14 +4834,14 @@
       </c>
       <c r="C103" s="8">
         <f>C21*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D103" s="8">
         <v>0</v>
       </c>
       <c r="E103" s="8">
         <f t="shared" si="2"/>
-        <v>0.99639999999999995</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -4833,14 +4853,14 @@
       </c>
       <c r="C104" s="8">
         <f>C22*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D104" s="8">
         <v>0</v>
       </c>
       <c r="E104" s="8">
         <f t="shared" si="2"/>
-        <v>0.99639999999999995</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -4852,14 +4872,14 @@
       </c>
       <c r="C105" s="8">
         <f>C23*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D105" s="8">
         <v>0</v>
       </c>
       <c r="E105" s="8">
         <f t="shared" si="2"/>
-        <v>0.99639999999999995</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -4871,14 +4891,14 @@
       </c>
       <c r="C106" s="8">
         <f>C24*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D106" s="8">
         <v>0</v>
       </c>
       <c r="E106" s="8">
         <f t="shared" si="2"/>
-        <v>0.99639999999999995</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -4890,14 +4910,14 @@
       </c>
       <c r="C107" s="8">
         <f>C25*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D107" s="8">
         <v>0</v>
       </c>
       <c r="E107" s="8">
         <f t="shared" si="2"/>
-        <v>0.99639999999999995</v>
+        <v>0.99819999999999998</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -4909,14 +4929,14 @@
       </c>
       <c r="C108" s="8">
         <f>C26*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D108" s="8">
         <v>0.01</v>
       </c>
       <c r="E108" s="8">
         <f t="shared" si="2"/>
-        <v>0.98639999999999994</v>
+        <v>0.98819999999999997</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -4928,14 +4948,14 @@
       </c>
       <c r="C109" s="8">
         <f>C27*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D109" s="8">
         <v>0.01</v>
       </c>
       <c r="E109" s="8">
         <f t="shared" si="2"/>
-        <v>0.98639999999999994</v>
+        <v>0.98819999999999997</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -4947,14 +4967,14 @@
       </c>
       <c r="C110" s="8">
         <f>C28*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D110" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E110" s="8">
         <f t="shared" si="2"/>
-        <v>0.98139999999999994</v>
+        <v>0.98319999999999996</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -4966,14 +4986,14 @@
       </c>
       <c r="C111" s="8">
         <f>C29*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D111" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E111" s="8">
         <f t="shared" si="2"/>
-        <v>0.98139999999999994</v>
+        <v>0.98319999999999996</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -4985,14 +5005,14 @@
       </c>
       <c r="C112" s="8">
         <f>C30*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D112" s="8">
         <v>0.02</v>
       </c>
       <c r="E112" s="8">
         <f t="shared" si="2"/>
-        <v>0.97639999999999993</v>
+        <v>0.97819999999999996</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -5004,14 +5024,14 @@
       </c>
       <c r="C113" s="8">
         <f>C31*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D113" s="8">
         <v>0.02</v>
       </c>
       <c r="E113" s="8">
         <f t="shared" si="2"/>
-        <v>0.97639999999999993</v>
+        <v>0.97819999999999996</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -5023,14 +5043,14 @@
       </c>
       <c r="C114" s="8">
         <f>C32*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D114" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E114" s="8">
         <f t="shared" si="2"/>
-        <v>0.97139999999999993</v>
+        <v>0.97319999999999995</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -5042,14 +5062,14 @@
       </c>
       <c r="C115" s="8">
         <f>C33*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D115" s="8">
         <v>0.03</v>
       </c>
       <c r="E115" s="8">
         <f t="shared" si="2"/>
-        <v>0.96639999999999993</v>
+        <v>0.96819999999999995</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -5061,14 +5081,14 @@
       </c>
       <c r="C116" s="8">
         <f>C34*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D116" s="8">
         <v>0.09</v>
       </c>
       <c r="E116" s="8">
         <f t="shared" si="2"/>
-        <v>0.90639999999999998</v>
+        <v>0.90820000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -5080,14 +5100,14 @@
       </c>
       <c r="C117" s="8">
         <f>C35*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D117" s="8">
         <v>0.09</v>
       </c>
       <c r="E117" s="8">
         <f t="shared" si="2"/>
-        <v>0.90639999999999998</v>
+        <v>0.90820000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -5099,14 +5119,14 @@
       </c>
       <c r="C118" s="8">
         <f>C36*SimParameters!B10</f>
-        <v>3.5999999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D118" s="8">
         <v>0.09</v>
       </c>
       <c r="E118" s="8">
         <f t="shared" si="2"/>
-        <v>0.90639999999999998</v>
+        <v>0.90820000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -5234,7 +5254,7 @@
   <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C84" sqref="C84:C124"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5613,14 +5633,14 @@
       </c>
       <c r="C20" s="6">
         <f>potential_preg_untrt!C20*SimParameters!B3</f>
-        <v>8.0000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
-        <v>0.99199999999999999</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -5632,14 +5652,14 @@
       </c>
       <c r="C21" s="6">
         <f>potential_preg_untrt!C21*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D21" s="6">
         <v>0</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
-        <v>0.99760000000000004</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -5651,14 +5671,14 @@
       </c>
       <c r="C22" s="6">
         <f>potential_preg_untrt!C22*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D22" s="6">
         <v>0</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>0.99760000000000004</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -5670,14 +5690,14 @@
       </c>
       <c r="C23" s="6">
         <f>potential_preg_untrt!C23*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D23" s="6">
         <v>0</v>
       </c>
       <c r="E23" s="6">
         <f t="shared" si="0"/>
-        <v>0.99760000000000004</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -5689,14 +5709,14 @@
       </c>
       <c r="C24" s="6">
         <f>potential_preg_untrt!C24*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D24" s="6">
         <v>0</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
-        <v>0.99760000000000004</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -5708,14 +5728,14 @@
       </c>
       <c r="C25" s="6">
         <f>potential_preg_untrt!C25*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D25" s="6">
         <v>0</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="0"/>
-        <v>0.99760000000000004</v>
+        <v>0.99880000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -5727,14 +5747,14 @@
       </c>
       <c r="C26" s="6">
         <f>potential_preg_untrt!C26*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D26" s="6">
         <v>0.01</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="0"/>
-        <v>0.98760000000000003</v>
+        <v>0.98880000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -5746,14 +5766,14 @@
       </c>
       <c r="C27" s="6">
         <f>potential_preg_untrt!C27*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D27" s="6">
         <v>0.01</v>
       </c>
       <c r="E27" s="6">
         <f t="shared" si="0"/>
-        <v>0.98760000000000003</v>
+        <v>0.98880000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -5765,14 +5785,14 @@
       </c>
       <c r="C28" s="6">
         <f>potential_preg_untrt!C28*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D28" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E28" s="6">
         <f t="shared" si="0"/>
-        <v>0.98260000000000003</v>
+        <v>0.98380000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -5784,14 +5804,14 @@
       </c>
       <c r="C29" s="6">
         <f>potential_preg_untrt!C29*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D29" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" si="0"/>
-        <v>0.98260000000000003</v>
+        <v>0.98380000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -5803,14 +5823,14 @@
       </c>
       <c r="C30" s="6">
         <f>potential_preg_untrt!C30*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D30" s="6">
         <v>0.02</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" si="0"/>
-        <v>0.97760000000000002</v>
+        <v>0.9788</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -5822,14 +5842,14 @@
       </c>
       <c r="C31" s="6">
         <f>potential_preg_untrt!C31*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D31" s="6">
         <v>0.02</v>
       </c>
       <c r="E31" s="6">
         <f t="shared" si="0"/>
-        <v>0.97760000000000002</v>
+        <v>0.9788</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -5841,14 +5861,14 @@
       </c>
       <c r="C32" s="6">
         <f>potential_preg_untrt!C32*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D32" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E32" s="6">
         <f t="shared" si="0"/>
-        <v>0.97260000000000002</v>
+        <v>0.9738</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -5860,14 +5880,14 @@
       </c>
       <c r="C33" s="6">
         <f>potential_preg_untrt!C33*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D33" s="6">
         <v>0.03</v>
       </c>
       <c r="E33" s="6">
         <f t="shared" si="0"/>
-        <v>0.96760000000000002</v>
+        <v>0.96879999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -5879,14 +5899,14 @@
       </c>
       <c r="C34" s="6">
         <f>potential_preg_untrt!C34*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D34" s="6">
         <v>0.09</v>
       </c>
       <c r="E34" s="6">
         <f t="shared" si="0"/>
-        <v>0.90760000000000007</v>
+        <v>0.90880000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -5898,14 +5918,14 @@
       </c>
       <c r="C35" s="6">
         <f>potential_preg_untrt!C35*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D35" s="6">
         <v>0.09</v>
       </c>
       <c r="E35" s="6">
         <f t="shared" si="0"/>
-        <v>0.90760000000000007</v>
+        <v>0.90880000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5917,14 +5937,14 @@
       </c>
       <c r="C36" s="6">
         <f>potential_preg_untrt!C36*SimParameters!B3</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D36" s="6">
         <v>0.09</v>
       </c>
       <c r="E36" s="6">
         <f t="shared" si="0"/>
-        <v>0.90760000000000007</v>
+        <v>0.90880000000000005</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -6392,14 +6412,14 @@
       </c>
       <c r="C61" s="7">
         <f>potential_preg_untrt!C61*SimParameters!$B$3</f>
-        <v>8.8000000000000005E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D61" s="7">
         <v>0</v>
       </c>
       <c r="E61" s="7">
         <f t="shared" si="1"/>
-        <v>0.99119999999999997</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -6411,14 +6431,14 @@
       </c>
       <c r="C62" s="7">
         <f>potential_preg_untrt!C62*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D62" s="7">
         <v>0</v>
       </c>
       <c r="E62" s="7">
         <f t="shared" si="1"/>
-        <v>0.99736000000000002</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -6430,14 +6450,14 @@
       </c>
       <c r="C63" s="7">
         <f>potential_preg_untrt!C63*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D63" s="7">
         <v>0</v>
       </c>
       <c r="E63" s="7">
         <f t="shared" si="1"/>
-        <v>0.99736000000000002</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -6449,14 +6469,14 @@
       </c>
       <c r="C64" s="7">
         <f>potential_preg_untrt!C64*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D64" s="7">
         <v>0</v>
       </c>
       <c r="E64" s="7">
         <f t="shared" si="1"/>
-        <v>0.99736000000000002</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -6468,14 +6488,14 @@
       </c>
       <c r="C65" s="7">
         <f>potential_preg_untrt!C65*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D65" s="7">
         <v>0</v>
       </c>
       <c r="E65" s="7">
         <f t="shared" si="1"/>
-        <v>0.99736000000000002</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -6487,14 +6507,14 @@
       </c>
       <c r="C66" s="7">
         <f>potential_preg_untrt!C66*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D66" s="7">
         <v>0</v>
       </c>
       <c r="E66" s="7">
         <f t="shared" si="1"/>
-        <v>0.99736000000000002</v>
+        <v>0.99868000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -6506,14 +6526,14 @@
       </c>
       <c r="C67" s="7">
         <f>potential_preg_untrt!C67*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D67" s="7">
         <v>0.01</v>
       </c>
       <c r="E67" s="7">
         <f t="shared" si="1"/>
-        <v>0.98736000000000002</v>
+        <v>0.98868</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -6525,14 +6545,14 @@
       </c>
       <c r="C68" s="7">
         <f>potential_preg_untrt!C68*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D68" s="7">
         <v>0.01</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="1"/>
-        <v>0.98736000000000002</v>
+        <v>0.98868</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -6544,14 +6564,14 @@
       </c>
       <c r="C69" s="7">
         <f>potential_preg_untrt!C69*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D69" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E69" s="7">
         <f t="shared" si="1"/>
-        <v>0.98236000000000001</v>
+        <v>0.98368</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -6563,14 +6583,14 @@
       </c>
       <c r="C70" s="7">
         <f>potential_preg_untrt!C70*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D70" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="1"/>
-        <v>0.98236000000000001</v>
+        <v>0.98368</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -6582,14 +6602,14 @@
       </c>
       <c r="C71" s="7">
         <f>potential_preg_untrt!C71*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D71" s="7">
         <v>0.02</v>
       </c>
       <c r="E71" s="7">
         <f t="shared" si="1"/>
-        <v>0.97736000000000001</v>
+        <v>0.97867999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -6601,14 +6621,14 @@
       </c>
       <c r="C72" s="7">
         <f>potential_preg_untrt!C72*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D72" s="7">
         <v>0.02</v>
       </c>
       <c r="E72" s="7">
         <f t="shared" si="1"/>
-        <v>0.97736000000000001</v>
+        <v>0.97867999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -6620,14 +6640,14 @@
       </c>
       <c r="C73" s="7">
         <f>potential_preg_untrt!C73*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D73" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E73" s="7">
         <f t="shared" si="1"/>
-        <v>0.97236</v>
+        <v>0.97367999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -6639,14 +6659,14 @@
       </c>
       <c r="C74" s="7">
         <f>potential_preg_untrt!C74*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D74" s="7">
         <v>0.03</v>
       </c>
       <c r="E74" s="7">
         <f t="shared" si="1"/>
-        <v>0.96736</v>
+        <v>0.96867999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -6658,14 +6678,14 @@
       </c>
       <c r="C75" s="7">
         <f>potential_preg_untrt!C75*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D75" s="7">
         <v>0.09</v>
       </c>
       <c r="E75" s="7">
         <f t="shared" si="1"/>
-        <v>0.90736000000000006</v>
+        <v>0.90868000000000004</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -6677,14 +6697,14 @@
       </c>
       <c r="C76" s="7">
         <f>potential_preg_untrt!C76*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D76" s="7">
         <v>0.09</v>
       </c>
       <c r="E76" s="7">
         <f t="shared" si="1"/>
-        <v>0.90736000000000006</v>
+        <v>0.90868000000000004</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -6696,14 +6716,14 @@
       </c>
       <c r="C77" s="7">
         <f>potential_preg_untrt!C77*SimParameters!$B$3</f>
-        <v>2.6400000000000004E-3</v>
+        <v>1.3200000000000002E-3</v>
       </c>
       <c r="D77" s="7">
         <v>0.09</v>
       </c>
       <c r="E77" s="7">
         <f t="shared" si="1"/>
-        <v>0.90736000000000006</v>
+        <v>0.90868000000000004</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -7171,14 +7191,14 @@
       </c>
       <c r="C102" s="8">
         <f>potential_preg_untrt!C102*SimParameters!$B$3</f>
-        <v>9.6000000000000009E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D102" s="8">
         <v>0</v>
       </c>
       <c r="E102" s="8">
         <f t="shared" si="2"/>
-        <v>0.99039999999999995</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -7190,14 +7210,14 @@
       </c>
       <c r="C103" s="8">
         <f>potential_preg_untrt!C103*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D103" s="8">
         <v>0</v>
       </c>
       <c r="E103" s="8">
         <f t="shared" si="2"/>
-        <v>0.99712000000000001</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -7209,14 +7229,14 @@
       </c>
       <c r="C104" s="8">
         <f>potential_preg_untrt!C104*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D104" s="8">
         <v>0</v>
       </c>
       <c r="E104" s="8">
         <f t="shared" si="2"/>
-        <v>0.99712000000000001</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -7228,14 +7248,14 @@
       </c>
       <c r="C105" s="8">
         <f>potential_preg_untrt!C105*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D105" s="8">
         <v>0</v>
       </c>
       <c r="E105" s="8">
         <f t="shared" si="2"/>
-        <v>0.99712000000000001</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -7247,14 +7267,14 @@
       </c>
       <c r="C106" s="8">
         <f>potential_preg_untrt!C106*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D106" s="8">
         <v>0</v>
       </c>
       <c r="E106" s="8">
         <f t="shared" si="2"/>
-        <v>0.99712000000000001</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -7266,14 +7286,14 @@
       </c>
       <c r="C107" s="8">
         <f>potential_preg_untrt!C107*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D107" s="8">
         <v>0</v>
       </c>
       <c r="E107" s="8">
         <f t="shared" si="2"/>
-        <v>0.99712000000000001</v>
+        <v>0.99856</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -7285,14 +7305,14 @@
       </c>
       <c r="C108" s="8">
         <f>potential_preg_untrt!C108*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D108" s="8">
         <v>0.01</v>
       </c>
       <c r="E108" s="8">
         <f t="shared" si="2"/>
-        <v>0.98712</v>
+        <v>0.98855999999999999</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -7304,14 +7324,14 @@
       </c>
       <c r="C109" s="8">
         <f>potential_preg_untrt!C109*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D109" s="8">
         <v>0.01</v>
       </c>
       <c r="E109" s="8">
         <f t="shared" si="2"/>
-        <v>0.98712</v>
+        <v>0.98855999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -7323,14 +7343,14 @@
       </c>
       <c r="C110" s="8">
         <f>potential_preg_untrt!C110*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D110" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E110" s="8">
         <f t="shared" si="2"/>
-        <v>0.98211999999999999</v>
+        <v>0.98355999999999999</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -7342,14 +7362,14 @@
       </c>
       <c r="C111" s="8">
         <f>potential_preg_untrt!C111*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D111" s="8">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E111" s="8">
         <f t="shared" si="2"/>
-        <v>0.98211999999999999</v>
+        <v>0.98355999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -7361,14 +7381,14 @@
       </c>
       <c r="C112" s="8">
         <f>potential_preg_untrt!C112*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D112" s="8">
         <v>0.02</v>
       </c>
       <c r="E112" s="8">
         <f t="shared" si="2"/>
-        <v>0.97711999999999999</v>
+        <v>0.97855999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -7380,14 +7400,14 @@
       </c>
       <c r="C113" s="8">
         <f>potential_preg_untrt!C113*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D113" s="8">
         <v>0.02</v>
       </c>
       <c r="E113" s="8">
         <f t="shared" si="2"/>
-        <v>0.97711999999999999</v>
+        <v>0.97855999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -7399,14 +7419,14 @@
       </c>
       <c r="C114" s="8">
         <f>potential_preg_untrt!C114*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D114" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E114" s="8">
         <f t="shared" si="2"/>
-        <v>0.97211999999999998</v>
+        <v>0.97355999999999998</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -7418,14 +7438,14 @@
       </c>
       <c r="C115" s="8">
         <f>potential_preg_untrt!C115*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D115" s="8">
         <v>0.03</v>
       </c>
       <c r="E115" s="8">
         <f t="shared" si="2"/>
-        <v>0.96711999999999998</v>
+        <v>0.96855999999999998</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -7437,14 +7457,14 @@
       </c>
       <c r="C116" s="8">
         <f>potential_preg_untrt!C116*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D116" s="8">
         <v>0.09</v>
       </c>
       <c r="E116" s="8">
         <f t="shared" si="2"/>
-        <v>0.90712000000000004</v>
+        <v>0.90856000000000003</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -7456,14 +7476,14 @@
       </c>
       <c r="C117" s="8">
         <f>potential_preg_untrt!C117*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D117" s="8">
         <v>0.09</v>
       </c>
       <c r="E117" s="8">
         <f t="shared" si="2"/>
-        <v>0.90712000000000004</v>
+        <v>0.90856000000000003</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -7475,14 +7495,14 @@
       </c>
       <c r="C118" s="8">
         <f>potential_preg_untrt!C118*SimParameters!$B$3</f>
-        <v>2.8800000000000002E-3</v>
+        <v>1.4400000000000001E-3</v>
       </c>
       <c r="D118" s="8">
         <v>0.09</v>
       </c>
       <c r="E118" s="8">
         <f t="shared" si="2"/>
-        <v>0.90712000000000004</v>
+        <v>0.90856000000000003</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -7609,7 +7629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870C18B-8ADE-814A-BF98-16981C435EF7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -9571,7 +9591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBCDA1E-E196-5243-A50A-855DF45BB886}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -11573,15 +11593,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E248214-C639-FE41-8DE0-FF7112935623}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -11594,9 +11613,9 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
@@ -11871,7 +11890,7 @@
       </c>
       <c r="C26" s="6">
         <f>potential_preg_untrt!C26*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -11883,7 +11902,7 @@
       </c>
       <c r="C27" s="6">
         <f>potential_preg_untrt!C27*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -11895,7 +11914,7 @@
       </c>
       <c r="C28" s="6">
         <f>potential_preg_untrt!C28*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -11907,7 +11926,7 @@
       </c>
       <c r="C29" s="6">
         <f>potential_preg_untrt!C29*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -11919,7 +11938,7 @@
       </c>
       <c r="C30" s="6">
         <f>potential_preg_untrt!C30*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -11931,7 +11950,7 @@
       </c>
       <c r="C31" s="6">
         <f>potential_preg_untrt!C31*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -11943,7 +11962,7 @@
       </c>
       <c r="C32" s="6">
         <f>potential_preg_untrt!C32*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -11955,7 +11974,7 @@
       </c>
       <c r="C33" s="6">
         <f>potential_preg_untrt!C33*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -11967,7 +11986,7 @@
       </c>
       <c r="C34" s="6">
         <f>potential_preg_untrt!C34*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -11979,7 +11998,7 @@
       </c>
       <c r="C35" s="6">
         <f>potential_preg_untrt!C35*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -11991,7 +12010,7 @@
       </c>
       <c r="C36" s="6">
         <f>potential_preg_untrt!C36*3</f>
-        <v>9.0000000000000011E-3</v>
+        <v>4.5000000000000005E-3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -12363,7 +12382,7 @@
       </c>
       <c r="C67" s="7">
         <f>C26*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -12375,7 +12394,7 @@
       </c>
       <c r="C68" s="7">
         <f>C27*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -12387,7 +12406,7 @@
       </c>
       <c r="C69" s="7">
         <f>C28*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -12399,7 +12418,7 @@
       </c>
       <c r="C70" s="7">
         <f>C29*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -12411,7 +12430,7 @@
       </c>
       <c r="C71" s="7">
         <f>C30*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -12423,7 +12442,7 @@
       </c>
       <c r="C72" s="7">
         <f>C31*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -12435,7 +12454,7 @@
       </c>
       <c r="C73" s="7">
         <f>C32*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -12447,7 +12466,7 @@
       </c>
       <c r="C74" s="7">
         <f>C33*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -12459,7 +12478,7 @@
       </c>
       <c r="C75" s="7">
         <f>C34*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -12471,7 +12490,7 @@
       </c>
       <c r="C76" s="7">
         <f>C35*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -12483,7 +12502,7 @@
       </c>
       <c r="C77" s="7">
         <f>C36*SimParameters!$B$9</f>
-        <v>9.9000000000000025E-3</v>
+        <v>4.9500000000000013E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -12855,7 +12874,7 @@
       </c>
       <c r="C108" s="8">
         <f>C26*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -12867,7 +12886,7 @@
       </c>
       <c r="C109" s="8">
         <f>C27*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -12879,7 +12898,7 @@
       </c>
       <c r="C110" s="8">
         <f>C28*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -12891,7 +12910,7 @@
       </c>
       <c r="C111" s="8">
         <f>C29*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -12903,7 +12922,7 @@
       </c>
       <c r="C112" s="8">
         <f>C30*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -12915,7 +12934,7 @@
       </c>
       <c r="C113" s="8">
         <f>C31*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -12927,7 +12946,7 @@
       </c>
       <c r="C114" s="8">
         <f>C32*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -12939,7 +12958,7 @@
       </c>
       <c r="C115" s="8">
         <f>C33*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -12951,7 +12970,7 @@
       </c>
       <c r="C116" s="8">
         <f>C34*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -12963,7 +12982,7 @@
       </c>
       <c r="C117" s="8">
         <f>C35*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -12975,7 +12994,7 @@
       </c>
       <c r="C118" s="8">
         <f>C36*SimParameters!$B$16</f>
-        <v>1.0800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -15779,15 +15798,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -16012,15 +16022,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16037,4 +16048,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Downloaded renv package and reorganized files. Worked on distribution of pregnancy outcomes after discussion with clinician.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
+++ b/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2246A5-FDC6-D347-AB3C-09FD1DFDEA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07511BA-05BA-9542-A266-75995B83137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -273,7 +273,9 @@
 Reply:
     Previously 0.06
 Reply:
-    Previously 0.035</t>
+    Previously 0.035
+Reply:
+    Previously 0.15</t>
       </text>
     </comment>
     <comment ref="D35" authorId="23" shapeId="0" xr:uid="{96162AFE-BCF7-FF46-8327-A20C0FF6288B}">
@@ -281,7 +283,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Previously 0.06</t>
+    Previously 0.06
+Reply:
+    Previously 0.03</t>
       </text>
     </comment>
     <comment ref="D36" authorId="24" shapeId="0" xr:uid="{DB8D7BF8-7A77-C548-93AC-920263C47AE7}">
@@ -307,7 +311,9 @@
 Comment:
     Previously 0.3
 Reply:
-    Previously 0.12</t>
+    Previously 0.12
+Reply:
+    Previously 0.05</t>
       </text>
     </comment>
     <comment ref="D38" authorId="27" shapeId="0" xr:uid="{22732877-B594-3A44-BC45-02143C03F17F}">
@@ -399,6 +405,9 @@
   <authors>
     <author>tc={E213A8AF-362C-3249-8F32-5816963215D6}</author>
     <author>tc={29763DF1-A92A-BB44-B75E-A2C031E5A1DB}</author>
+    <author>tc={43C05DFE-3F99-2340-BC5C-ABCDE3AE0F7E}</author>
+    <author>tc={49F4C65F-40DD-5044-B5CC-CB04F634A42A}</author>
+    <author>tc={49444082-D094-F245-B3DE-77B68C1DD127}</author>
     <author>tc={F4A2424B-F409-B04F-B010-E79913C4F818}</author>
     <author>tc={1670A8BD-D7C8-874C-97A9-38556A273CCF}</author>
   </authors>
@@ -426,7 +435,31 @@
 </t>
       </text>
     </comment>
-    <comment ref="C41" authorId="2" shapeId="0" xr:uid="{F4A2424B-F409-B04F-B010-E79913C4F818}">
+    <comment ref="C29" authorId="2" shapeId="0" xr:uid="{43C05DFE-3F99-2340-BC5C-ABCDE3AE0F7E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.0001</t>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="3" shapeId="0" xr:uid="{49F4C65F-40DD-5044-B5CC-CB04F634A42A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.0004</t>
+      </text>
+    </comment>
+    <comment ref="C31" authorId="4" shapeId="0" xr:uid="{49444082-D094-F245-B3DE-77B68C1DD127}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.0005</t>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="5" shapeId="0" xr:uid="{F4A2424B-F409-B04F-B010-E79913C4F818}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -434,7 +467,7 @@
     Was 0.011</t>
       </text>
     </comment>
-    <comment ref="C42" authorId="3" shapeId="0" xr:uid="{1670A8BD-D7C8-874C-97A9-38556A273CCF}">
+    <comment ref="C42" authorId="6" shapeId="0" xr:uid="{1670A8BD-D7C8-874C-97A9-38556A273CCF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1065,7 +1098,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1116,6 +1149,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1664,8 +1703,14 @@
   <threadedComment ref="D34" dT="2024-07-06T23:46:35.55" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{66C098C2-0D77-3140-AB53-07109FBBBDB1}" parentId="{CCDC8F71-8200-9641-AEEF-2B20BAD612FE}">
     <text>Previously 0.035</text>
   </threadedComment>
+  <threadedComment ref="D34" dT="2024-07-12T13:50:09.92" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{C86BDAF5-9C01-C84C-933C-0BA61D71043A}" parentId="{CCDC8F71-8200-9641-AEEF-2B20BAD612FE}">
+    <text>Previously 0.15</text>
+  </threadedComment>
   <threadedComment ref="D35" dT="2024-06-21T18:22:01.97" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{96162AFE-BCF7-FF46-8327-A20C0FF6288B}">
     <text>Previously 0.06</text>
+  </threadedComment>
+  <threadedComment ref="D35" dT="2024-07-12T13:49:46.98" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{02D44866-621F-B34E-8FE2-8998FD60ED7D}" parentId="{96162AFE-BCF7-FF46-8327-A20C0FF6288B}">
+    <text>Previously 0.03</text>
   </threadedComment>
   <threadedComment ref="D36" dT="2024-06-21T18:22:13.45" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{DB8D7BF8-7A77-C548-93AC-920263C47AE7}">
     <text>Previously 0.06</text>
@@ -1678,6 +1723,9 @@
   </threadedComment>
   <threadedComment ref="D37" dT="2024-06-21T18:22:26.56" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{A2113B5B-E003-8D40-B7DC-CA7AD96B0FC2}" parentId="{97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}">
     <text>Previously 0.12</text>
+  </threadedComment>
+  <threadedComment ref="D37" dT="2024-07-12T13:50:56.67" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{9DCA148F-50FB-0949-9EF8-E60CF9728C79}" parentId="{97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}">
+    <text>Previously 0.05</text>
   </threadedComment>
   <threadedComment ref="D38" dT="2024-06-21T18:00:19.51" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{22732877-B594-3A44-BC45-02143C03F17F}">
     <text>Previously 0.35</text>
@@ -1737,6 +1785,15 @@
   <threadedComment ref="F1" dT="2024-06-21T19:39:03.42" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{FF188301-AAA9-9842-B50B-708EBB96FFC0}" parentId="{29763DF1-A92A-BB44-B75E-A2C031E5A1DB}">
     <text xml:space="preserve">Transformed this to logit function as opposed to multiplying directly. Risks were going out of bounds
 </text>
+  </threadedComment>
+  <threadedComment ref="C29" dT="2024-07-12T13:56:38.50" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{43C05DFE-3F99-2340-BC5C-ABCDE3AE0F7E}">
+    <text>Previously 0.0001</text>
+  </threadedComment>
+  <threadedComment ref="C30" dT="2024-07-12T13:57:20.72" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{49F4C65F-40DD-5044-B5CC-CB04F634A42A}">
+    <text>Previously 0.0004</text>
+  </threadedComment>
+  <threadedComment ref="C31" dT="2024-07-12T13:58:31.15" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{49444082-D094-F245-B3DE-77B68C1DD127}">
+    <text>Previously 0.0005</text>
   </threadedComment>
   <threadedComment ref="C41" dT="2024-06-21T19:31:37.84" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{F4A2424B-F409-B04F-B010-E79913C4F818}">
     <text>Was 0.011</text>
@@ -1953,7 +2010,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,7 +2037,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2101,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2714,14 +2771,14 @@
         <v>32</v>
       </c>
       <c r="C34" s="8">
-        <v>1.4999999999999999E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D34" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>0.98485</v>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2732,14 +2789,14 @@
         <v>33</v>
       </c>
       <c r="C35" s="8">
-        <v>1.4999999999999999E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D35" s="8">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>0.96984999999999999</v>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2750,14 +2807,14 @@
         <v>34</v>
       </c>
       <c r="C36" s="8">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D36" s="8">
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="0"/>
-        <v>0.95919999999999994</v>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2768,14 +2825,14 @@
         <v>35</v>
       </c>
       <c r="C37" s="8">
-        <v>1.1999999999999999E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D37" s="8">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="0"/>
-        <v>0.94879999999999998</v>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3517,15 +3574,15 @@
       </c>
       <c r="C75" s="3">
         <f>C34*SimParameters!B9</f>
-        <v>1.65E-4</v>
+        <v>3.8500000000000003E-4</v>
       </c>
       <c r="D75" s="3">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="2"/>
-        <v>0.98483500000000002</v>
+        <v>0.94961499999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -3537,15 +3594,15 @@
       </c>
       <c r="C76" s="3">
         <f>C35*SimParameters!B9</f>
-        <v>1.65E-4</v>
+        <v>6.0500000000000007E-4</v>
       </c>
       <c r="D76" s="3">
         <f t="shared" si="1"/>
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="2"/>
-        <v>0.969835</v>
+        <v>0.91939500000000007</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -3557,15 +3614,15 @@
       </c>
       <c r="C77" s="3">
         <f>C36*SimParameters!B9</f>
-        <v>8.8000000000000014E-4</v>
+        <v>3.8500000000000006E-3</v>
       </c>
       <c r="D77" s="3">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="2"/>
-        <v>0.95911999999999997</v>
+        <v>0.64615</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -3577,15 +3634,15 @@
       </c>
       <c r="C78" s="3">
         <f>C37*SimParameters!B9</f>
-        <v>1.32E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D78" s="3">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="2"/>
-        <v>0.94867999999999997</v>
+        <v>0.59834999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -4336,15 +4393,15 @@
       </c>
       <c r="C116" s="4">
         <f>C34*SimParameters!B10</f>
-        <v>1.7999999999999998E-4</v>
+        <v>4.1999999999999996E-4</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E116" s="4">
         <f t="shared" si="4"/>
-        <v>0.98482000000000003</v>
+        <v>0.94957999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -4356,15 +4413,15 @@
       </c>
       <c r="C117" s="4">
         <f>C35*SimParameters!B10</f>
-        <v>1.7999999999999998E-4</v>
+        <v>6.6E-4</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E117" s="4">
         <f t="shared" si="4"/>
-        <v>0.96982000000000002</v>
+        <v>0.91934000000000005</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -4376,15 +4433,15 @@
       </c>
       <c r="C118" s="4">
         <f>C36*SimParameters!B10</f>
-        <v>9.6000000000000002E-4</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E118" s="4">
         <f t="shared" si="4"/>
-        <v>0.95904</v>
+        <v>0.64580000000000004</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -4396,15 +4453,15 @@
       </c>
       <c r="C119" s="4">
         <f>C37*SimParameters!B10</f>
-        <v>1.4399999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="3"/>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E119" s="4">
         <f t="shared" si="4"/>
-        <v>0.94855999999999996</v>
+        <v>0.59819999999999995</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -4554,7 +4611,7 @@
       </c>
       <c r="C2" s="2">
         <f>potential_preg_untrt!C2*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D2" s="2">
         <f>potential_preg_untrt!D2</f>
@@ -4562,7 +4619,7 @@
       </c>
       <c r="E2" s="2">
         <f>1-D2-C2</f>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4574,7 +4631,7 @@
       </c>
       <c r="C3" s="2">
         <f>potential_preg_untrt!C3*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D3" s="2">
         <f>potential_preg_untrt!D3</f>
@@ -4582,7 +4639,7 @@
       </c>
       <c r="E3" s="2">
         <f>1-D3-C3</f>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4594,7 +4651,7 @@
       </c>
       <c r="C4" s="2">
         <f>potential_preg_untrt!C4*SimParameters!B3</f>
-        <v>0.1</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="D4" s="2">
         <f>potential_preg_untrt!D4</f>
@@ -4602,7 +4659,7 @@
       </c>
       <c r="E4" s="2">
         <f>1-D4-C4</f>
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4614,7 +4671,7 @@
       </c>
       <c r="C5" s="2">
         <f>potential_preg_untrt!C5*SimParameters!B3</f>
-        <v>0.1</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="D5" s="2">
         <f>potential_preg_untrt!D5</f>
@@ -4622,7 +4679,7 @@
       </c>
       <c r="E5" s="2">
         <f>1-D5-C5</f>
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -4634,7 +4691,7 @@
       </c>
       <c r="C6" s="2">
         <f>potential_preg_untrt!C6*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D6" s="2">
         <f>potential_preg_untrt!D6</f>
@@ -4642,7 +4699,7 @@
       </c>
       <c r="E6" s="2">
         <f>1-D6-C6</f>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4654,7 +4711,7 @@
       </c>
       <c r="C7" s="2">
         <f>potential_preg_untrt!C7*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D7" s="2">
         <f>potential_preg_untrt!D7</f>
@@ -4662,7 +4719,7 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" ref="E7:E41" si="0">1-C7-D7</f>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -4674,7 +4731,7 @@
       </c>
       <c r="C8" s="2">
         <f>potential_preg_untrt!C8*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D8" s="2">
         <f>potential_preg_untrt!D8</f>
@@ -4682,7 +4739,7 @@
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4694,7 +4751,7 @@
       </c>
       <c r="C9" s="2">
         <f>potential_preg_untrt!C9*SimParameters!B3</f>
-        <v>0.2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="D9" s="2">
         <f>potential_preg_untrt!D9</f>
@@ -4702,7 +4759,7 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -4714,7 +4771,7 @@
       </c>
       <c r="C10" s="2">
         <f>potential_preg_untrt!C10*SimParameters!B3</f>
-        <v>0.04</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D10" s="2">
         <f>potential_preg_untrt!D10</f>
@@ -4722,7 +4779,7 @@
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -4734,7 +4791,7 @@
       </c>
       <c r="C11" s="2">
         <f>potential_preg_untrt!C11*SimParameters!B3</f>
-        <v>0.04</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D11" s="2">
         <f>potential_preg_untrt!D11</f>
@@ -4742,7 +4799,7 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -4754,7 +4811,7 @@
       </c>
       <c r="C12" s="2">
         <f>potential_preg_untrt!C12*SimParameters!B3</f>
-        <v>0.04</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D12" s="2">
         <f>potential_preg_untrt!D12</f>
@@ -4762,7 +4819,7 @@
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -4774,7 +4831,7 @@
       </c>
       <c r="C13" s="2">
         <f>potential_preg_untrt!C13*SimParameters!B3</f>
-        <v>0.04</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D13" s="2">
         <f>potential_preg_untrt!D13</f>
@@ -4782,7 +4839,7 @@
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4794,7 +4851,7 @@
       </c>
       <c r="C14" s="2">
         <f>potential_preg_untrt!C14*SimParameters!B3</f>
-        <v>0.02</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D14" s="2">
         <f>potential_preg_untrt!D14</f>
@@ -4802,7 +4859,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4814,7 +4871,7 @@
       </c>
       <c r="C15" s="2">
         <f>potential_preg_untrt!C15*SimParameters!B3</f>
-        <v>0.02</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D15" s="2">
         <f>potential_preg_untrt!D15</f>
@@ -4822,7 +4879,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4834,7 +4891,7 @@
       </c>
       <c r="C16" s="2">
         <f>potential_preg_untrt!C16*SimParameters!B3</f>
-        <v>0.02</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D16" s="2">
         <f>potential_preg_untrt!D16</f>
@@ -4842,7 +4899,7 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -4854,7 +4911,7 @@
       </c>
       <c r="C17" s="2">
         <f>potential_preg_untrt!C17*SimParameters!B3</f>
-        <v>0.02</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D17" s="2">
         <f>potential_preg_untrt!D17</f>
@@ -4862,7 +4919,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0.99199999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -4874,7 +4931,7 @@
       </c>
       <c r="C18" s="2">
         <f>potential_preg_untrt!C18*SimParameters!B3</f>
-        <v>1.6000000000000001E-3</v>
+        <v>6.4000000000000005E-4</v>
       </c>
       <c r="D18" s="2">
         <f>potential_preg_untrt!D18</f>
@@ -4882,7 +4939,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>0.99839999999999995</v>
+        <v>0.99936000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -5194,15 +5251,15 @@
       </c>
       <c r="C34" s="2">
         <f>potential_preg_untrt!C34</f>
-        <v>1.4999999999999999E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D34" s="2">
         <f>potential_preg_untrt!D34</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>0.98485</v>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -5214,15 +5271,15 @@
       </c>
       <c r="C35" s="2">
         <f>potential_preg_untrt!C35</f>
-        <v>1.4999999999999999E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D35" s="2">
         <f>potential_preg_untrt!D35</f>
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>0.96984999999999999</v>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5234,15 +5291,15 @@
       </c>
       <c r="C36" s="2">
         <f>potential_preg_untrt!C36</f>
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D36" s="2">
         <f>potential_preg_untrt!D36</f>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="0"/>
-        <v>0.95919999999999994</v>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -5254,15 +5311,15 @@
       </c>
       <c r="C37" s="2">
         <f>potential_preg_untrt!C37</f>
-        <v>1.1999999999999999E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D37" s="2">
         <f>potential_preg_untrt!D37</f>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="0"/>
-        <v>0.94879999999999998</v>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -5373,7 +5430,7 @@
       </c>
       <c r="C43" s="3">
         <f>potential_preg_untrt!C43*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D43" s="3">
         <f>potential_preg_untrt!D43</f>
@@ -5381,7 +5438,7 @@
       </c>
       <c r="E43" s="3">
         <f>1-D43-C43</f>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5393,7 +5450,7 @@
       </c>
       <c r="C44" s="3">
         <f>potential_preg_untrt!C44*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D44" s="3">
         <f>potential_preg_untrt!D44</f>
@@ -5401,7 +5458,7 @@
       </c>
       <c r="E44" s="3">
         <f>1-D44-C44</f>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5413,7 +5470,7 @@
       </c>
       <c r="C45" s="3">
         <f>potential_preg_untrt!C45*SimParameters!$B$3</f>
-        <v>0.11000000000000001</v>
+        <v>4.4000000000000011E-2</v>
       </c>
       <c r="D45" s="3">
         <f>potential_preg_untrt!D45</f>
@@ -5421,7 +5478,7 @@
       </c>
       <c r="E45" s="3">
         <f>1-D45-C45</f>
-        <v>0.89</v>
+        <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5433,7 +5490,7 @@
       </c>
       <c r="C46" s="3">
         <f>potential_preg_untrt!C46*SimParameters!$B$3</f>
-        <v>0.11000000000000001</v>
+        <v>4.4000000000000011E-2</v>
       </c>
       <c r="D46" s="3">
         <f>potential_preg_untrt!D46</f>
@@ -5441,7 +5498,7 @@
       </c>
       <c r="E46" s="3">
         <f>1-D46-C46</f>
-        <v>0.89</v>
+        <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5453,7 +5510,7 @@
       </c>
       <c r="C47" s="3">
         <f>potential_preg_untrt!C47*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D47" s="3">
         <f>potential_preg_untrt!D47</f>
@@ -5461,7 +5518,7 @@
       </c>
       <c r="E47" s="3">
         <f>1-D47-C47</f>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5473,7 +5530,7 @@
       </c>
       <c r="C48" s="3">
         <f>potential_preg_untrt!C48*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D48" s="3">
         <f>potential_preg_untrt!D48</f>
@@ -5481,7 +5538,7 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" ref="E48:E82" si="1">1-C48-D48</f>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -5493,7 +5550,7 @@
       </c>
       <c r="C49" s="3">
         <f>potential_preg_untrt!C49*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D49" s="3">
         <f>potential_preg_untrt!D49</f>
@@ -5501,7 +5558,7 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="1"/>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -5513,7 +5570,7 @@
       </c>
       <c r="C50" s="3">
         <f>potential_preg_untrt!C50*SimParameters!$B$3</f>
-        <v>0.22000000000000003</v>
+        <v>8.8000000000000023E-2</v>
       </c>
       <c r="D50" s="3">
         <f>potential_preg_untrt!D50</f>
@@ -5521,7 +5578,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="1"/>
-        <v>0.78</v>
+        <v>0.91199999999999992</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -5533,7 +5590,7 @@
       </c>
       <c r="C51" s="3">
         <f>potential_preg_untrt!C51*SimParameters!$B$3</f>
-        <v>4.4000000000000004E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="D51" s="3">
         <f>potential_preg_untrt!D51</f>
@@ -5541,7 +5598,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="1"/>
-        <v>0.95599999999999996</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -5553,7 +5610,7 @@
       </c>
       <c r="C52" s="3">
         <f>potential_preg_untrt!C52*SimParameters!$B$3</f>
-        <v>4.4000000000000004E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="D52" s="3">
         <f>potential_preg_untrt!D52</f>
@@ -5561,7 +5618,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="1"/>
-        <v>0.95599999999999996</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -5573,7 +5630,7 @@
       </c>
       <c r="C53" s="3">
         <f>potential_preg_untrt!C53*SimParameters!$B$3</f>
-        <v>4.4000000000000004E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="D53" s="3">
         <f>potential_preg_untrt!D53</f>
@@ -5581,7 +5638,7 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="1"/>
-        <v>0.95599999999999996</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -5593,7 +5650,7 @@
       </c>
       <c r="C54" s="3">
         <f>potential_preg_untrt!C54*SimParameters!$B$3</f>
-        <v>4.4000000000000004E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="D54" s="3">
         <f>potential_preg_untrt!D54</f>
@@ -5601,7 +5658,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="1"/>
-        <v>0.95599999999999996</v>
+        <v>0.98240000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -5613,7 +5670,7 @@
       </c>
       <c r="C55" s="3">
         <f>potential_preg_untrt!C55*SimParameters!$B$3</f>
-        <v>2.2000000000000002E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D55" s="3">
         <f>potential_preg_untrt!D55</f>
@@ -5621,7 +5678,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="1"/>
-        <v>0.97799999999999998</v>
+        <v>0.99119999999999997</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5633,7 +5690,7 @@
       </c>
       <c r="C56" s="3">
         <f>potential_preg_untrt!C56*SimParameters!$B$3</f>
-        <v>2.2000000000000002E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D56" s="3">
         <f>potential_preg_untrt!D56</f>
@@ -5641,7 +5698,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="1"/>
-        <v>0.97799999999999998</v>
+        <v>0.99119999999999997</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5653,7 +5710,7 @@
       </c>
       <c r="C57" s="3">
         <f>potential_preg_untrt!C57*SimParameters!$B$3</f>
-        <v>2.2000000000000002E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D57" s="3">
         <f>potential_preg_untrt!D57</f>
@@ -5661,7 +5718,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="1"/>
-        <v>0.97799999999999998</v>
+        <v>0.99119999999999997</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5673,7 +5730,7 @@
       </c>
       <c r="C58" s="3">
         <f>potential_preg_untrt!C58*SimParameters!$B$3</f>
-        <v>2.2000000000000002E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D58" s="3">
         <f>potential_preg_untrt!D58</f>
@@ -5681,7 +5738,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="1"/>
-        <v>0.97799999999999998</v>
+        <v>0.99119999999999997</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5693,7 +5750,7 @@
       </c>
       <c r="C59" s="3">
         <f>potential_preg_untrt!C59*SimParameters!$B$3</f>
-        <v>1.7600000000000003E-3</v>
+        <v>7.040000000000002E-4</v>
       </c>
       <c r="D59" s="3">
         <f>potential_preg_untrt!D59</f>
@@ -5701,7 +5758,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="1"/>
-        <v>0.99824000000000002</v>
+        <v>0.99929599999999996</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -6013,15 +6070,15 @@
       </c>
       <c r="C75" s="3">
         <f>potential_preg_untrt!C75</f>
-        <v>1.65E-4</v>
+        <v>3.8500000000000003E-4</v>
       </c>
       <c r="D75" s="3">
         <f>potential_preg_untrt!D75</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="1"/>
-        <v>0.98483500000000002</v>
+        <v>0.94961499999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -6033,15 +6090,15 @@
       </c>
       <c r="C76" s="3">
         <f>potential_preg_untrt!C76</f>
-        <v>1.65E-4</v>
+        <v>6.0500000000000007E-4</v>
       </c>
       <c r="D76" s="3">
         <f>potential_preg_untrt!D76</f>
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="1"/>
-        <v>0.969835</v>
+        <v>0.91939500000000007</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -6053,15 +6110,15 @@
       </c>
       <c r="C77" s="3">
         <f>potential_preg_untrt!C77</f>
-        <v>8.8000000000000014E-4</v>
+        <v>3.8500000000000006E-3</v>
       </c>
       <c r="D77" s="3">
         <f>potential_preg_untrt!D77</f>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="1"/>
-        <v>0.95911999999999997</v>
+        <v>0.64615</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -6073,15 +6130,15 @@
       </c>
       <c r="C78" s="3">
         <f>potential_preg_untrt!C78</f>
-        <v>1.32E-3</v>
+        <v>1.6500000000000002E-3</v>
       </c>
       <c r="D78" s="3">
         <f>potential_preg_untrt!D78</f>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="1"/>
-        <v>0.94867999999999997</v>
+        <v>0.59834999999999994</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -6192,7 +6249,7 @@
       </c>
       <c r="C84" s="4">
         <f>potential_preg_untrt!C84*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D84" s="4">
         <f>potential_preg_untrt!D84</f>
@@ -6200,7 +6257,7 @@
       </c>
       <c r="E84" s="4">
         <f>1-D84-C84</f>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -6212,7 +6269,7 @@
       </c>
       <c r="C85" s="4">
         <f>potential_preg_untrt!C85*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D85" s="4">
         <f>potential_preg_untrt!D85</f>
@@ -6220,7 +6277,7 @@
       </c>
       <c r="E85" s="4">
         <f>1-D85-C85</f>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -6232,7 +6289,7 @@
       </c>
       <c r="C86" s="4">
         <f>potential_preg_untrt!C86*SimParameters!$B$3</f>
-        <v>0.12</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D86" s="4">
         <f>potential_preg_untrt!D86</f>
@@ -6240,7 +6297,7 @@
       </c>
       <c r="E86" s="4">
         <f>1-D86-C86</f>
-        <v>0.88</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -6252,7 +6309,7 @@
       </c>
       <c r="C87" s="4">
         <f>potential_preg_untrt!C87*SimParameters!$B$3</f>
-        <v>0.12</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D87" s="4">
         <f>potential_preg_untrt!D87</f>
@@ -6260,7 +6317,7 @@
       </c>
       <c r="E87" s="4">
         <f>1-D87-C87</f>
-        <v>0.88</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -6272,7 +6329,7 @@
       </c>
       <c r="C88" s="4">
         <f>potential_preg_untrt!C88*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D88" s="4">
         <f>potential_preg_untrt!D88</f>
@@ -6280,7 +6337,7 @@
       </c>
       <c r="E88" s="4">
         <f>1-D88-C88</f>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -6292,7 +6349,7 @@
       </c>
       <c r="C89" s="4">
         <f>potential_preg_untrt!C89*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D89" s="4">
         <f>potential_preg_untrt!D89</f>
@@ -6300,7 +6357,7 @@
       </c>
       <c r="E89" s="4">
         <f t="shared" ref="E89:E123" si="2">1-C89-D89</f>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -6312,7 +6369,7 @@
       </c>
       <c r="C90" s="4">
         <f>potential_preg_untrt!C90*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D90" s="4">
         <f>potential_preg_untrt!D90</f>
@@ -6320,7 +6377,7 @@
       </c>
       <c r="E90" s="4">
         <f t="shared" si="2"/>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -6332,7 +6389,7 @@
       </c>
       <c r="C91" s="4">
         <f>potential_preg_untrt!C91*SimParameters!$B$3</f>
-        <v>0.24</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -6340,7 +6397,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.76</v>
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -6352,7 +6409,7 @@
       </c>
       <c r="C92" s="4">
         <f>potential_preg_untrt!C92*SimParameters!$B$3</f>
-        <v>4.8000000000000001E-2</v>
+        <v>1.9200000000000002E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -6360,7 +6417,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -6372,7 +6429,7 @@
       </c>
       <c r="C93" s="4">
         <f>potential_preg_untrt!C93*SimParameters!$B$3</f>
-        <v>4.8000000000000001E-2</v>
+        <v>1.9200000000000002E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -6380,7 +6437,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -6392,7 +6449,7 @@
       </c>
       <c r="C94" s="4">
         <f>potential_preg_untrt!C94*SimParameters!$B$3</f>
-        <v>4.8000000000000001E-2</v>
+        <v>1.9200000000000002E-2</v>
       </c>
       <c r="D94" s="4">
         <f>potential_preg_untrt!D94</f>
@@ -6400,7 +6457,7 @@
       </c>
       <c r="E94" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -6412,7 +6469,7 @@
       </c>
       <c r="C95" s="4">
         <f>potential_preg_untrt!C95*SimParameters!$B$3</f>
-        <v>4.8000000000000001E-2</v>
+        <v>1.9200000000000002E-2</v>
       </c>
       <c r="D95" s="4">
         <f>potential_preg_untrt!D95</f>
@@ -6420,7 +6477,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="2"/>
-        <v>0.95199999999999996</v>
+        <v>0.98080000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -6432,7 +6489,7 @@
       </c>
       <c r="C96" s="4">
         <f>potential_preg_untrt!C96*SimParameters!$B$3</f>
-        <v>2.4E-2</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D96" s="4">
         <f>potential_preg_untrt!D96</f>
@@ -6440,7 +6497,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="2"/>
-        <v>0.97599999999999998</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -6452,7 +6509,7 @@
       </c>
       <c r="C97" s="4">
         <f>potential_preg_untrt!C97*SimParameters!$B$3</f>
-        <v>2.4E-2</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D97" s="4">
         <f>potential_preg_untrt!D97</f>
@@ -6460,7 +6517,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="2"/>
-        <v>0.97599999999999998</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -6472,7 +6529,7 @@
       </c>
       <c r="C98" s="4">
         <f>potential_preg_untrt!C98*SimParameters!$B$3</f>
-        <v>2.4E-2</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -6480,7 +6537,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.97599999999999998</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -6492,7 +6549,7 @@
       </c>
       <c r="C99" s="4">
         <f>potential_preg_untrt!C99*SimParameters!$B$3</f>
-        <v>2.4E-2</v>
+        <v>9.6000000000000009E-3</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -6500,7 +6557,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.97599999999999998</v>
+        <v>0.99039999999999995</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -6512,7 +6569,7 @@
       </c>
       <c r="C100" s="4">
         <f>potential_preg_untrt!C100*SimParameters!$B$3</f>
-        <v>1.92E-3</v>
+        <v>7.6800000000000002E-4</v>
       </c>
       <c r="D100" s="4">
         <f>potential_preg_untrt!D100</f>
@@ -6520,7 +6577,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="2"/>
-        <v>0.99807999999999997</v>
+        <v>0.99923200000000001</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -6832,15 +6889,15 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preg_untrt!C116</f>
-        <v>1.7999999999999998E-4</v>
+        <v>4.1999999999999996E-4</v>
       </c>
       <c r="D116" s="4">
         <f>potential_preg_untrt!D116</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E116" s="4">
         <f t="shared" si="2"/>
-        <v>0.98482000000000003</v>
+        <v>0.94957999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -6852,15 +6909,15 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preg_untrt!C117</f>
-        <v>1.7999999999999998E-4</v>
+        <v>6.6E-4</v>
       </c>
       <c r="D117" s="4">
         <f>potential_preg_untrt!D117</f>
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E117" s="4">
         <f t="shared" si="2"/>
-        <v>0.96982000000000002</v>
+        <v>0.91934000000000005</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -6872,15 +6929,15 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preg_untrt!C118</f>
-        <v>9.6000000000000002E-4</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="D118" s="4">
         <f>potential_preg_untrt!D118</f>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="E118" s="4">
         <f t="shared" si="2"/>
-        <v>0.95904</v>
+        <v>0.64580000000000004</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -6892,15 +6949,15 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preg_untrt!C119</f>
-        <v>1.4399999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="D119" s="4">
         <f>potential_preg_untrt!D119</f>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E119" s="4">
         <f t="shared" si="2"/>
-        <v>0.94855999999999996</v>
+        <v>0.59819999999999995</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -7012,8 +7069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870C18B-8ADE-814A-BF98-16981C435EF7}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7572,19 +7629,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="8">
-        <v>1E-4</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="D29" s="15">
         <f t="shared" si="1"/>
-        <v>-3.9999565683801923</v>
+        <v>-4.6989613183595207</v>
       </c>
       <c r="E29" s="15">
         <f>D29+LOG(SimParameters!$B$19)</f>
-        <v>-4.6989265727162106</v>
+        <v>-5.3979313226955394</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>9.0228916237305098E-3</v>
+        <v>4.5055421756067648E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -7595,19 +7652,19 @@
         <v>28</v>
       </c>
       <c r="C30" s="8">
-        <v>4.0000000000000002E-4</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="D30" s="15">
         <f t="shared" si="1"/>
-        <v>-3.3977662561264501</v>
+        <v>-4.3979226365453163</v>
       </c>
       <c r="E30" s="15">
         <f>D30+LOG(SimParameters!$B$19)</f>
-        <v>-4.0967362604624693</v>
+        <v>-5.0968926408813351</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>1.6354921785067249E-2</v>
+        <v>6.0785461201715348E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -7618,19 +7675,19 @@
         <v>29</v>
       </c>
       <c r="C31" s="8">
-        <v>5.0000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D31" s="15">
         <f t="shared" si="1"/>
-        <v>-3.3008127941181171</v>
+        <v>-3.6988831367525901</v>
       </c>
       <c r="E31" s="15">
         <f>D31+LOG(SimParameters!$B$19)</f>
-        <v>-3.9997827984541359</v>
+        <v>-4.3978531410886088</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>1.7990046730857353E-2</v>
+        <v>1.2154184181940421E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -7641,19 +7698,19 @@
         <v>30</v>
       </c>
       <c r="C32" s="8">
-        <v>8.0000000000000004E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="D32" s="15">
         <f t="shared" si="1"/>
-        <v>-3.0965624383741357</v>
+        <v>-3.2215880947229243</v>
       </c>
       <c r="E32" s="15">
         <f>D32+LOG(SimParameters!$B$19)</f>
-        <v>-3.7955324427101544</v>
+        <v>-3.920558099058943</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>2.1977092262942803E-2</v>
+        <v>1.9444440799320156E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -7664,19 +7721,19 @@
         <v>31</v>
       </c>
       <c r="C33" s="8">
-        <v>1.1999999999999999E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D33" s="15">
         <f t="shared" si="1"/>
-        <v>-2.9202972876316853</v>
+        <v>-2.9995654882259823</v>
       </c>
       <c r="E33" s="15">
         <f>D33+LOG(SimParameters!$B$19)</f>
-        <v>-3.619267291967704</v>
+        <v>-3.6985354925620011</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="2"/>
-        <v>2.6102695103414991E-2</v>
+        <v>2.4161527152488677E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -7687,19 +7744,19 @@
         <v>32</v>
       </c>
       <c r="C34" s="8">
-        <v>1.8E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" si="1"/>
-        <v>-2.7439450604267974</v>
+        <v>-2.9202972876316853</v>
       </c>
       <c r="E34" s="15">
         <f>D34+LOG(SimParameters!$B$19)</f>
-        <v>-3.4429150647628162</v>
+        <v>-3.619267291967704</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>3.0980851137979604E-2</v>
+        <v>2.6102695103414991E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -7710,19 +7767,19 @@
         <v>33</v>
       </c>
       <c r="C35" s="8">
-        <v>5.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="D35" s="15">
         <f t="shared" si="1"/>
-        <v>-2.2988530764097068</v>
+        <v>-1.5096504795465824</v>
       </c>
       <c r="E35" s="15">
         <f>D35+LOG(SimParameters!$B$19)</f>
-        <v>-2.9978230807457256</v>
+        <v>-2.2086204838826013</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>4.7524316066742761E-2</v>
+        <v>9.8979033395933586E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -7733,19 +7790,19 @@
         <v>34</v>
       </c>
       <c r="C36" s="8">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" si="1"/>
-        <v>-1.9956351945975499</v>
+        <v>-1.3802112417116059</v>
       </c>
       <c r="E36" s="15">
         <f>D36+LOG(SimParameters!$B$19)</f>
-        <v>-2.6946051989335684</v>
+        <v>-2.0791812460476247</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>6.3292442454347467E-2</v>
+        <v>0.11113682192415951</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -7756,19 +7813,19 @@
         <v>35</v>
       </c>
       <c r="C37" s="8">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" si="1"/>
-        <v>-1.6901960800285136</v>
+        <v>-1.2787536009528289</v>
       </c>
       <c r="E37" s="15">
         <f>D37+LOG(SimParameters!$B$19)</f>
-        <v>-2.3891660843645326</v>
+        <v>-1.9777236052888476</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>8.4002576233824053E-2</v>
+        <v>0.12156171214195612</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -7779,19 +7836,19 @@
         <v>36</v>
       </c>
       <c r="C38" s="8">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="D38" s="15">
         <f t="shared" si="1"/>
-        <v>-1.6901960800285136</v>
+        <v>-1.1949766032160551</v>
       </c>
       <c r="E38" s="15">
         <f>D38+LOG(SimParameters!$B$19)</f>
-        <v>-2.3891660843645326</v>
+        <v>-1.8939466075520739</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>8.4002576233824053E-2</v>
+        <v>0.13079513429212816</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -8441,19 +8498,19 @@
       </c>
       <c r="C70" s="3">
         <f>C29*SimParameters!$B$15</f>
-        <v>1.1000000000000002E-4</v>
+        <v>2.2000000000000003E-5</v>
       </c>
       <c r="D70" s="14">
         <f t="shared" si="1"/>
-        <v>-3.9585595398210911</v>
+        <v>-4.6575677645940914</v>
       </c>
       <c r="E70" s="14">
         <f>D70+LOG(SimParameters!$B$19)</f>
-        <v>-4.6575295441571098</v>
+        <v>-5.3565377689301101</v>
       </c>
       <c r="F70" s="14">
         <f t="shared" si="2"/>
-        <v>9.4006666131868435E-3</v>
+        <v>4.6950623435460994E-3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -8465,19 +8522,19 @@
       </c>
       <c r="C71" s="3">
         <f>C30*SimParameters!$B$15</f>
-        <v>4.4000000000000007E-4</v>
+        <v>4.4000000000000006E-5</v>
       </c>
       <c r="D71" s="14">
         <f t="shared" si="1"/>
-        <v>-3.3563561918897333</v>
+        <v>-4.3565282141361994</v>
       </c>
       <c r="E71" s="14">
         <f>D71+LOG(SimParameters!$B$19)</f>
-        <v>-4.0553261962257521</v>
+        <v>-5.0554982184722181</v>
       </c>
       <c r="F71" s="14">
         <f t="shared" si="2"/>
-        <v>1.7034619342510351E-2</v>
+        <v>6.333817275568066E-3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -8489,19 +8546,19 @@
       </c>
       <c r="C72" s="3">
         <f>C31*SimParameters!$B$15</f>
-        <v>5.5000000000000003E-4</v>
+        <v>2.2000000000000003E-4</v>
       </c>
       <c r="D72" s="14">
         <f t="shared" si="1"/>
-        <v>-3.2593983828295738</v>
+        <v>-3.6574817638803068</v>
       </c>
       <c r="E72" s="14">
         <f>D72+LOG(SimParameters!$B$19)</f>
-        <v>-3.9583683871655926</v>
+        <v>-4.356451768216326</v>
       </c>
       <c r="F72" s="14">
         <f t="shared" si="2"/>
-        <v>1.8736484311822035E-2</v>
+        <v>1.2661440966665547E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -8513,19 +8570,19 @@
       </c>
       <c r="C73" s="3">
         <f>C32*SimParameters!$B$15</f>
-        <v>8.8000000000000014E-4</v>
+        <v>6.6E-4</v>
       </c>
       <c r="D73" s="14">
         <f t="shared" si="1"/>
-        <v>-3.0551349804482149</v>
+        <v>-3.1801693354690972</v>
       </c>
       <c r="E73" s="14">
         <f>D73+LOG(SimParameters!$B$19)</f>
-        <v>-3.7541049847842336</v>
+        <v>-3.8791393398051159</v>
       </c>
       <c r="F73" s="14">
         <f t="shared" si="2"/>
-        <v>2.2885395652437045E-2</v>
+        <v>2.0250065545743406E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -8537,19 +8594,19 @@
       </c>
       <c r="C74" s="3">
         <f>C33*SimParameters!$B$15</f>
-        <v>1.32E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D74" s="14">
         <f t="shared" si="1"/>
-        <v>-2.8788524213874007</v>
+        <v>-2.9581293279706786</v>
       </c>
       <c r="E74" s="14">
         <f>D74+LOG(SimParameters!$B$19)</f>
-        <v>-3.5778224257234195</v>
+        <v>-3.6570993323066974</v>
       </c>
       <c r="F74" s="14">
         <f t="shared" si="2"/>
-        <v>2.717723004012558E-2</v>
+        <v>2.5158003356518917E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -8561,19 +8618,19 @@
       </c>
       <c r="C75" s="3">
         <f>C34*SimParameters!$B$15</f>
-        <v>1.98E-3</v>
+        <v>1.32E-3</v>
       </c>
       <c r="D75" s="14">
         <f t="shared" si="1"/>
-        <v>-2.7024740542348642</v>
+        <v>-2.8788524213874007</v>
       </c>
       <c r="E75" s="14">
         <f>D75+LOG(SimParameters!$B$19)</f>
-        <v>-3.4014440585708829</v>
+        <v>-3.5778224257234195</v>
       </c>
       <c r="F75" s="14">
         <f t="shared" si="2"/>
-        <v>3.2250364772667045E-2</v>
+        <v>2.717723004012558E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -8585,19 +8642,19 @@
       </c>
       <c r="C76" s="3">
         <f>C35*SimParameters!$B$15</f>
-        <v>5.5000000000000005E-3</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="D76" s="14">
         <f t="shared" si="1"/>
-        <v>-2.2572420979662104</v>
+        <v>-1.4669125342051141</v>
       </c>
       <c r="E76" s="14">
         <f>D76+LOG(SimParameters!$B$19)</f>
-        <v>-2.9562121023022292</v>
+        <v>-2.1658825385411329</v>
       </c>
       <c r="F76" s="14">
         <f t="shared" si="2"/>
-        <v>4.9443730141344254E-2</v>
+        <v>0.10285635932288763</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -8609,19 +8666,19 @@
       </c>
       <c r="C77" s="3">
         <f>C36*SimParameters!$B$15</f>
-        <v>1.1000000000000001E-2</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="D77" s="14">
         <f t="shared" si="1"/>
-        <v>-1.9538036064389543</v>
+        <v>-1.3370052157899126</v>
       </c>
       <c r="E77" s="14">
         <f>D77+LOG(SimParameters!$B$19)</f>
-        <v>-2.6527736107749731</v>
+        <v>-2.0359752201259314</v>
       </c>
       <c r="F77" s="14">
         <f t="shared" si="2"/>
-        <v>6.5818265136210169E-2</v>
+        <v>0.11547719617364935</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -8633,19 +8690,19 @@
       </c>
       <c r="C78" s="3">
         <f>C37*SimParameters!$B$15</f>
-        <v>2.2000000000000002E-2</v>
+        <v>5.5000000000000007E-2</v>
       </c>
       <c r="D78" s="14">
         <f t="shared" si="1"/>
-        <v>-1.6479161739653951</v>
+        <v>-1.2350691190150189</v>
       </c>
       <c r="E78" s="14">
         <f>D78+LOG(SimParameters!$B$19)</f>
-        <v>-2.3468861783014141</v>
+        <v>-1.9340391233510377</v>
       </c>
       <c r="F78" s="14">
         <f t="shared" si="2"/>
-        <v>8.7313594015583307E-2</v>
+        <v>0.12630418387093481</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -8657,19 +8714,19 @@
       </c>
       <c r="C79" s="3">
         <f>C38*SimParameters!$B$15</f>
-        <v>2.2000000000000002E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="D79" s="14">
         <f t="shared" si="1"/>
-        <v>-1.6479161739653951</v>
+        <v>-1.1508029406882248</v>
       </c>
       <c r="E79" s="14">
         <f>D79+LOG(SimParameters!$B$19)</f>
-        <v>-2.3468861783014141</v>
+        <v>-1.8497729450242435</v>
       </c>
       <c r="F79" s="14">
         <f t="shared" si="2"/>
-        <v>8.7313594015583307E-2</v>
+        <v>0.13589955806781698</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -9323,19 +9380,19 @@
       </c>
       <c r="C111" s="4">
         <f>C29*SimParameters!$B$16</f>
-        <v>1.2E-4</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="D111" s="13">
         <f t="shared" si="5"/>
-        <v>-3.9207666354873765</v>
+        <v>-4.6197783350957495</v>
       </c>
       <c r="E111" s="13">
         <f>D111+LOG(SimParameters!$B$19)</f>
-        <v>-4.6197366398233957</v>
+        <v>-5.3187483394317683</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="6"/>
-        <v>9.7592104003560946E-3</v>
+        <v>4.874999580500021E-3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -9347,19 +9404,19 @@
       </c>
       <c r="C112" s="4">
         <f>C30*SimParameters!$B$16</f>
-        <v>4.8000000000000001E-4</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="D112" s="13">
         <f t="shared" si="5"/>
-        <v>-3.3185502512263594</v>
+        <v>-4.3187379159889581</v>
       </c>
       <c r="E112" s="13">
         <f>D112+LOG(SimParameters!$B$19)</f>
-        <v>-4.0175202555623777</v>
+        <v>-5.0177079203249768</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="6"/>
-        <v>1.7679354083987433E-2</v>
+        <v>6.5761501489709634E-3</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -9371,19 +9428,19 @@
       </c>
       <c r="C113" s="4">
         <f>C31*SimParameters!$B$16</f>
-        <v>5.9999999999999995E-4</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="D113" s="13">
         <f t="shared" si="5"/>
-        <v>-3.2215880947229243</v>
+        <v>-3.6196845151030543</v>
       </c>
       <c r="E113" s="13">
         <f>D113+LOG(SimParameters!$B$19)</f>
-        <v>-3.920558099058943</v>
+        <v>-4.3186545194390735</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="6"/>
-        <v>1.9444440799320156E-2</v>
+        <v>1.3142757828126333E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -9395,19 +9452,19 @@
       </c>
       <c r="C114" s="4">
         <f>C32*SimParameters!$B$16</f>
-        <v>9.6000000000000002E-4</v>
+        <v>7.1999999999999994E-4</v>
       </c>
       <c r="D114" s="13">
         <f t="shared" si="5"/>
-        <v>-3.0173116440067362</v>
+        <v>-3.1423546989185689</v>
       </c>
       <c r="E114" s="13">
         <f>D114+LOG(SimParameters!$B$19)</f>
-        <v>-3.716281648342755</v>
+        <v>-3.8413247032545876</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="6"/>
-        <v>2.3746627197533426E-2</v>
+        <v>2.1014077282474689E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -9419,19 +9476,19 @@
       </c>
       <c r="C115" s="4">
         <f>C33*SimParameters!$B$16</f>
-        <v>1.4399999999999999E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="D115" s="13">
         <f t="shared" si="5"/>
-        <v>-2.841011673141558</v>
+        <v>-2.9202972876316853</v>
       </c>
       <c r="E115" s="13">
         <f>D115+LOG(SimParameters!$B$19)</f>
-        <v>-3.5399816774775767</v>
+        <v>-3.619267291967704</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="6"/>
-        <v>2.8195790017344867E-2</v>
+        <v>2.6102695103414991E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -9443,19 +9500,19 @@
       </c>
       <c r="C116" s="4">
         <f>C34*SimParameters!$B$16</f>
-        <v>2.16E-3</v>
+        <v>1.4399999999999999E-3</v>
       </c>
       <c r="D116" s="13">
         <f t="shared" si="5"/>
-        <v>-2.6646071581847273</v>
+        <v>-2.841011673141558</v>
       </c>
       <c r="E116" s="13">
         <f>D116+LOG(SimParameters!$B$19)</f>
-        <v>-3.363577162520746</v>
+        <v>-3.5399816774775767</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="6"/>
-        <v>3.3453365225185473E-2</v>
+        <v>2.8195790017344867E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -9467,19 +9524,19 @@
       </c>
       <c r="C117" s="4">
         <f>C35*SimParameters!$B$16</f>
-        <v>6.0000000000000001E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D117" s="13">
         <f t="shared" si="5"/>
-        <v>-2.2192351340136698</v>
+        <v>-1.4277745331355436</v>
       </c>
       <c r="E117" s="13">
         <f>D117+LOG(SimParameters!$B$19)</f>
-        <v>-2.9182051383496885</v>
+        <v>-2.1267445374715623</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="6"/>
-        <v>5.1260920579713251E-2</v>
+        <v>0.10652444011971599</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -9491,19 +9548,19 @@
       </c>
       <c r="C118" s="4">
         <f>C36*SimParameters!$B$16</f>
-        <v>1.2E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D118" s="13">
         <f t="shared" si="5"/>
-        <v>-1.9155756985400032</v>
+        <v>-1.2973957110088872</v>
       </c>
       <c r="E118" s="13">
         <f>D118+LOG(SimParameters!$B$19)</f>
-        <v>-2.6145457028760219</v>
+        <v>-1.9963657153449059</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="6"/>
-        <v>6.8208130347300028E-2</v>
+        <v>0.11958502698246047</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -9515,19 +9572,19 @@
       </c>
       <c r="C119" s="4">
         <f>C37*SimParameters!$B$16</f>
-        <v>2.4E-2</v>
+        <v>0.06</v>
       </c>
       <c r="D119" s="13">
         <f t="shared" si="5"/>
-        <v>-1.6092385759550858</v>
+        <v>-1.1949766032160551</v>
       </c>
       <c r="E119" s="13">
         <f>D119+LOG(SimParameters!$B$19)</f>
-        <v>-2.3082085802911045</v>
+        <v>-1.8939466075520739</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="6"/>
-        <v>9.044540782581055E-2</v>
+        <v>0.13079513429212816</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -9539,19 +9596,19 @@
       </c>
       <c r="C120" s="4">
         <f>C38*SimParameters!$B$16</f>
-        <v>2.4E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D120" s="13">
         <f t="shared" si="5"/>
-        <v>-1.6092385759550858</v>
+        <v>-1.1102154797875936</v>
       </c>
       <c r="E120" s="13">
         <f>D120+LOG(SimParameters!$B$19)</f>
-        <v>-2.3082085802911045</v>
+        <v>-1.8091854841236124</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="6"/>
-        <v>9.044540782581055E-2</v>
+        <v>0.14073659616116271</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -10248,19 +10305,19 @@
       </c>
       <c r="C29" s="2">
         <f>potential_preec_untrt!C29*SimParameters!$B$4</f>
-        <v>8.0000000000000007E-5</v>
+        <v>1.6000000000000003E-5</v>
       </c>
       <c r="D29" s="15">
         <f t="shared" si="1"/>
-        <v>-4.096875268059688</v>
+        <v>-4.7958730685767748</v>
       </c>
       <c r="E29" s="15">
         <f>D29+LOG(SimParameters!$B$19)</f>
-        <v>-4.7958452723957068</v>
+        <v>-5.4948430729127935</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="2"/>
-        <v>8.1962764200181667E-3</v>
+        <v>4.0910952414538217E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -10272,19 +10329,19 @@
       </c>
       <c r="C30" s="2">
         <f>potential_preec_untrt!C30*SimParameters!$B$4</f>
-        <v>3.2000000000000003E-4</v>
+        <v>3.2000000000000005E-5</v>
       </c>
       <c r="D30" s="15">
         <f t="shared" si="1"/>
-        <v>-3.4947110252052624</v>
+        <v>-4.4948361240343093</v>
       </c>
       <c r="E30" s="15">
         <f>D30+LOG(SimParameters!$B$19)</f>
-        <v>-4.1936810295412812</v>
+        <v>-5.1938061283703281</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="2"/>
-        <v>1.4866291682698516E-2</v>
+        <v>5.5201976201283707E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -10296,19 +10353,19 @@
       </c>
       <c r="C31" s="2">
         <f>potential_preec_untrt!C31*SimParameters!$B$4</f>
-        <v>4.0000000000000002E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
       <c r="D31" s="15">
         <f t="shared" si="1"/>
-        <v>-3.3977662561264501</v>
+        <v>-3.7958105246674081</v>
       </c>
       <c r="E31" s="15">
         <f>D31+LOG(SimParameters!$B$19)</f>
-        <v>-4.0967362604624693</v>
+        <v>-4.4947805290034264</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="2"/>
-        <v>1.6354921785067249E-2</v>
+        <v>1.1043803603731542E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -10320,19 +10377,19 @@
       </c>
       <c r="C32" s="2">
         <f>potential_preec_untrt!C32*SimParameters!$B$4</f>
-        <v>6.4000000000000005E-4</v>
+        <v>4.7999999999999996E-4</v>
       </c>
       <c r="D32" s="15">
         <f t="shared" si="1"/>
-        <v>-3.1935419885662175</v>
+        <v>-3.3185502512263594</v>
       </c>
       <c r="E32" s="15">
         <f>D32+LOG(SimParameters!$B$19)</f>
-        <v>-3.8925119929022363</v>
+        <v>-4.0175202555623777</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="2"/>
-        <v>1.9986447282310034E-2</v>
+        <v>1.7679354083987433E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -10344,19 +10401,19 @@
       </c>
       <c r="C33" s="2">
         <f>potential_preec_untrt!C33*SimParameters!$B$4</f>
-        <v>9.5999999999999992E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D33" s="15">
         <f t="shared" si="1"/>
-        <v>-3.0173116440067362</v>
+        <v>-3.0965624383741357</v>
       </c>
       <c r="E33" s="15">
         <f>D33+LOG(SimParameters!$B$19)</f>
-        <v>-3.716281648342755</v>
+        <v>-3.7955324427101544</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="2"/>
-        <v>2.3746627197533426E-2</v>
+        <v>2.1977092262942803E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -10368,19 +10425,19 @@
       </c>
       <c r="C34" s="2">
         <f>potential_preec_untrt!C34*SimParameters!$B$4</f>
-        <v>1.4400000000000001E-3</v>
+        <v>9.5999999999999992E-4</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" si="1"/>
-        <v>-2.841011673141558</v>
+        <v>-3.0173116440067362</v>
       </c>
       <c r="E34" s="15">
         <f>D34+LOG(SimParameters!$B$19)</f>
-        <v>-3.5399816774775767</v>
+        <v>-3.716281648342755</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="2"/>
-        <v>2.8195790017344867E-2</v>
+        <v>2.3746627197533426E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -10392,19 +10449,19 @@
       </c>
       <c r="C35" s="2">
         <f>potential_preec_untrt!C35*SimParameters!$B$4</f>
-        <v>4.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D35" s="15">
         <f t="shared" si="1"/>
-        <v>-2.3961993470957363</v>
+        <v>-1.6092385759550858</v>
       </c>
       <c r="E35" s="15">
         <f>D35+LOG(SimParameters!$B$19)</f>
-        <v>-3.0951693514317551</v>
+        <v>-2.3082085802911045</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="2"/>
-        <v>4.3306954825074587E-2</v>
+        <v>9.044540782581055E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -10416,19 +10473,19 @@
       </c>
       <c r="C36" s="2">
         <f>potential_preec_untrt!C36*SimParameters!$B$4</f>
-        <v>8.0000000000000002E-3</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" si="1"/>
-        <v>-2.0934216851622351</v>
+        <v>-1.4807253789884878</v>
       </c>
       <c r="E36" s="15">
         <f>D36+LOG(SimParameters!$B$19)</f>
-        <v>-2.7923916894982539</v>
+        <v>-2.1796953833245065</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="2"/>
-        <v>5.7736702059241522E-2</v>
+        <v>0.10158872641769165</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -10440,19 +10497,19 @@
       </c>
       <c r="C37" s="2">
         <f>potential_preec_untrt!C37*SimParameters!$B$4</f>
-        <v>1.6E-2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" si="1"/>
-        <v>-1.7888751157754166</v>
+        <v>-1.3802112417116059</v>
       </c>
       <c r="E37" s="15">
         <f>D37+LOG(SimParameters!$B$19)</f>
-        <v>-2.4878451201114355</v>
+        <v>-2.0791812460476247</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="2"/>
-        <v>7.6714687362351444E-2</v>
+        <v>0.11113682192415951</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -10464,19 +10521,19 @@
       </c>
       <c r="C38" s="2">
         <f>potential_preec_untrt!C38*SimParameters!$B$4</f>
-        <v>1.6E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D38" s="15">
         <f t="shared" si="1"/>
-        <v>-1.7888751157754166</v>
+        <v>-1.2973957110088872</v>
       </c>
       <c r="E38" s="15">
         <f>D38+LOG(SimParameters!$B$19)</f>
-        <v>-2.4878451201114355</v>
+        <v>-1.9963657153449059</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="2"/>
-        <v>7.6714687362351444E-2</v>
+        <v>0.11958502698246047</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -11130,19 +11187,19 @@
       </c>
       <c r="C70" s="3">
         <f>potential_preec_untrt!C70*SimParameters!$B$4</f>
-        <v>8.8000000000000025E-5</v>
+        <v>1.7600000000000004E-5</v>
       </c>
       <c r="D70" s="14">
         <f t="shared" si="1"/>
-        <v>-4.0554791082537367</v>
+        <v>-4.7544796885357039</v>
       </c>
       <c r="E70" s="14">
         <f>D70+LOG(SimParameters!$B$19)</f>
-        <v>-4.7544491125897554</v>
+        <v>-5.4534496928717227</v>
       </c>
       <c r="F70" s="14">
         <f t="shared" si="2"/>
-        <v>8.5397331546595845E-3</v>
+        <v>4.2632561228359185E-3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -11154,19 +11211,19 @@
       </c>
       <c r="C71" s="3">
         <f>potential_preec_untrt!C71*SimParameters!$B$4</f>
-        <v>3.520000000000001E-4</v>
+        <v>3.5200000000000009E-5</v>
       </c>
       <c r="D71" s="14">
         <f t="shared" si="1"/>
-        <v>-3.4533044379525117</v>
+        <v>-4.4534420490870454</v>
       </c>
       <c r="E71" s="14">
         <f>D71+LOG(SimParameters!$B$19)</f>
-        <v>-4.1522744422885305</v>
+        <v>-5.1524120534230642</v>
       </c>
       <c r="F71" s="14">
         <f t="shared" si="2"/>
-        <v>1.5485043882038368E-2</v>
+        <v>5.7521544051882759E-3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -11178,19 +11235,19 @@
       </c>
       <c r="C72" s="3">
         <f>potential_preec_untrt!C72*SimParameters!$B$4</f>
-        <v>4.4000000000000007E-4</v>
+        <v>1.7600000000000005E-4</v>
       </c>
       <c r="D72" s="14">
         <f t="shared" si="1"/>
-        <v>-3.3563561918897333</v>
+        <v>-3.7544108896298929</v>
       </c>
       <c r="E72" s="14">
         <f>D72+LOG(SimParameters!$B$19)</f>
-        <v>-4.0553261962257521</v>
+        <v>-4.4533808939659121</v>
       </c>
       <c r="F72" s="14">
         <f t="shared" si="2"/>
-        <v>1.7034619342510351E-2</v>
+        <v>1.150523845220339E-2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -11202,19 +11259,19 @@
       </c>
       <c r="C73" s="3">
         <f>potential_preec_untrt!C73*SimParameters!$B$4</f>
-        <v>7.040000000000002E-4</v>
+        <v>5.2800000000000004E-4</v>
       </c>
       <c r="D73" s="14">
         <f t="shared" si="1"/>
-        <v>-3.1521214898704435</v>
+        <v>-3.2771367094212489</v>
       </c>
       <c r="E73" s="14">
         <f>D73+LOG(SimParameters!$B$19)</f>
-        <v>-3.8510914942064622</v>
+        <v>-3.9761067137572677</v>
       </c>
       <c r="F73" s="14">
         <f t="shared" si="2"/>
-        <v>2.0814087287952962E-2</v>
+        <v>1.841312649977285E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -11226,19 +11283,19 @@
       </c>
       <c r="C74" s="3">
         <f>potential_preec_untrt!C74*SimParameters!$B$4</f>
-        <v>1.0560000000000001E-3</v>
+        <v>8.8000000000000014E-4</v>
       </c>
       <c r="D74" s="14">
         <f t="shared" si="1"/>
-        <v>-2.9758772245100031</v>
+        <v>-3.0551349804482149</v>
       </c>
       <c r="E74" s="14">
         <f>D74+LOG(SimParameters!$B$19)</f>
-        <v>-3.6748472288460219</v>
+        <v>-3.7541049847842336</v>
       </c>
       <c r="F74" s="14">
         <f t="shared" si="2"/>
-        <v>2.4726383587674761E-2</v>
+        <v>2.2885395652437045E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -11250,19 +11307,19 @@
       </c>
       <c r="C75" s="3">
         <f>potential_preec_untrt!C75*SimParameters!$B$4</f>
-        <v>1.5840000000000001E-3</v>
+        <v>1.0560000000000001E-3</v>
       </c>
       <c r="D75" s="14">
         <f t="shared" si="1"/>
-        <v>-2.799556354876573</v>
+        <v>-2.9758772245100031</v>
       </c>
       <c r="E75" s="14">
         <f>D75+LOG(SimParameters!$B$19)</f>
-        <v>-3.4985263592125917</v>
+        <v>-3.6748472288460219</v>
       </c>
       <c r="F75" s="14">
         <f t="shared" si="2"/>
-        <v>2.9354189383821068E-2</v>
+        <v>2.4726383587674761E-2</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -11274,19 +11331,19 @@
       </c>
       <c r="C76" s="3">
         <f>potential_preec_untrt!C76*SimParameters!$B$4</f>
-        <v>4.4000000000000003E-3</v>
+        <v>2.6400000000000003E-2</v>
       </c>
       <c r="D76" s="14">
         <f t="shared" si="1"/>
-        <v>-2.3546322114503684</v>
+        <v>-1.5667766383521775</v>
       </c>
       <c r="E76" s="14">
         <f>D76+LOG(SimParameters!$B$19)</f>
-        <v>-3.0536022157863871</v>
+        <v>-2.265746642688196</v>
       </c>
       <c r="F76" s="14">
         <f t="shared" si="2"/>
-        <v>4.5062210072855845E-2</v>
+        <v>9.3999819544859392E-2</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -11298,19 +11355,19 @@
       </c>
       <c r="C77" s="3">
         <f>potential_preec_untrt!C77*SimParameters!$B$4</f>
-        <v>8.8000000000000005E-3</v>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="D77" s="14">
         <f t="shared" si="1"/>
-        <v>-2.0516786212178384</v>
+        <v>-1.437894631317945</v>
       </c>
       <c r="E77" s="14">
         <f>D77+LOG(SimParameters!$B$19)</f>
-        <v>-2.7506486255538571</v>
+        <v>-2.1368646356539638</v>
       </c>
       <c r="F77" s="14">
         <f t="shared" si="2"/>
-        <v>6.005002868936829E-2</v>
+        <v>0.10556506811727921</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -11322,19 +11379,19 @@
       </c>
       <c r="C78" s="3">
         <f>potential_preec_untrt!C78*SimParameters!$B$4</f>
-        <v>1.7600000000000001E-2</v>
+        <v>4.4000000000000011E-2</v>
       </c>
       <c r="D78" s="14">
         <f t="shared" si="1"/>
-        <v>-1.7467756859829426</v>
+        <v>-1.3370052157899126</v>
       </c>
       <c r="E78" s="14">
         <f>D78+LOG(SimParameters!$B$19)</f>
-        <v>-2.4457456903189616</v>
+        <v>-2.0359752201259314</v>
       </c>
       <c r="F78" s="14">
         <f t="shared" si="2"/>
-        <v>7.9750215786880879E-2</v>
+        <v>0.11547719617364935</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -11346,19 +11403,19 @@
       </c>
       <c r="C79" s="3">
         <f>potential_preec_untrt!C79*SimParameters!$B$4</f>
-        <v>1.7600000000000001E-2</v>
+        <v>5.2800000000000007E-2</v>
       </c>
       <c r="D79" s="14">
         <f t="shared" si="1"/>
-        <v>-1.7467756859829426</v>
+        <v>-1.2538077668450323</v>
       </c>
       <c r="E79" s="14">
         <f>D79+LOG(SimParameters!$B$19)</f>
-        <v>-2.4457456903189616</v>
+        <v>-1.952777771181051</v>
       </c>
       <c r="F79" s="14">
         <f t="shared" si="2"/>
-        <v>7.9750215786880879E-2</v>
+        <v>0.12425078626846925</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -12012,19 +12069,19 @@
       </c>
       <c r="C111" s="4">
         <f>potential_preec_untrt!C111*SimParameters!$B$4</f>
-        <v>9.6000000000000002E-5</v>
+        <v>1.9200000000000003E-5</v>
       </c>
       <c r="D111" s="13">
         <f t="shared" si="5"/>
-        <v>-4.0176870726888119</v>
+        <v>-4.7166904327623476</v>
       </c>
       <c r="E111" s="13">
         <f>D111+LOG(SimParameters!$B$19)</f>
-        <v>-4.7166570770248306</v>
+        <v>-5.4156604370983663</v>
       </c>
       <c r="F111" s="13">
         <f t="shared" si="6"/>
-        <v>8.8657269692349119E-3</v>
+        <v>4.426717318032041E-3</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -12036,19 +12093,19 @@
       </c>
       <c r="C112" s="4">
         <f>potential_preec_untrt!C112*SimParameters!$B$4</f>
-        <v>3.8400000000000001E-4</v>
+        <v>3.8400000000000005E-5</v>
       </c>
       <c r="D112" s="13">
         <f t="shared" si="5"/>
-        <v>-3.4155019745235555</v>
+        <v>-4.4156520984041592</v>
       </c>
       <c r="E112" s="13">
         <f>D112+LOG(SimParameters!$B$19)</f>
-        <v>-4.1144719788595747</v>
+        <v>-5.1146221027401779</v>
       </c>
       <c r="F112" s="13">
         <f t="shared" si="6"/>
-        <v>1.6072033481906906E-2</v>
+        <v>5.9723644596316877E-3</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -12060,19 +12117,19 @@
       </c>
       <c r="C113" s="4">
         <f>potential_preec_untrt!C113*SimParameters!$B$4</f>
-        <v>4.7999999999999996E-4</v>
+        <v>1.92E-4</v>
       </c>
       <c r="D113" s="13">
         <f t="shared" si="5"/>
-        <v>-3.3185502512263594</v>
+        <v>-3.7166153787499843</v>
       </c>
       <c r="E113" s="13">
         <f>D113+LOG(SimParameters!$B$19)</f>
-        <v>-4.0175202555623777</v>
+        <v>-4.415585383086003</v>
       </c>
       <c r="F113" s="13">
         <f t="shared" si="6"/>
-        <v>1.7679354083987433E-2</v>
+        <v>1.1943114140972667E-2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -12084,19 +12141,19 @@
       </c>
       <c r="C114" s="4">
         <f>potential_preec_untrt!C114*SimParameters!$B$4</f>
-        <v>7.6800000000000002E-4</v>
+        <v>5.7600000000000001E-4</v>
       </c>
       <c r="D114" s="13">
         <f t="shared" si="5"/>
-        <v>-3.1143051136621178</v>
+        <v>-3.2393272908832915</v>
       </c>
       <c r="E114" s="13">
         <f>D114+LOG(SimParameters!$B$19)</f>
-        <v>-3.8132751179981366</v>
+        <v>-3.9382972952193103</v>
       </c>
       <c r="F114" s="13">
         <f t="shared" si="6"/>
-        <v>2.1598946558741741E-2</v>
+        <v>1.9109086574313931E-2</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -12108,19 +12165,19 @@
       </c>
       <c r="C115" s="4">
         <f>potential_preec_untrt!C115*SimParameters!$B$4</f>
-        <v>1.152E-3</v>
+        <v>9.5999999999999992E-4</v>
       </c>
       <c r="D115" s="13">
         <f t="shared" si="5"/>
-        <v>-2.9380469252711707</v>
+        <v>-3.0173116440067362</v>
       </c>
       <c r="E115" s="13">
         <f>D115+LOG(SimParameters!$B$19)</f>
-        <v>-3.6370169296071895</v>
+        <v>-3.716281648342755</v>
       </c>
       <c r="F115" s="13">
         <f t="shared" si="6"/>
-        <v>2.5655250878529656E-2</v>
+        <v>2.3746627197533426E-2</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -12132,19 +12189,19 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preec_untrt!C116*SimParameters!$B$4</f>
-        <v>1.7280000000000002E-3</v>
+        <v>1.152E-3</v>
       </c>
       <c r="D116" s="13">
         <f t="shared" si="5"/>
-        <v>-2.7617051518462854</v>
+        <v>-2.9380469252711707</v>
       </c>
       <c r="E116" s="13">
         <f>D116+LOG(SimParameters!$B$19)</f>
-        <v>-3.4606751561823041</v>
+        <v>-3.6370169296071895</v>
       </c>
       <c r="F116" s="13">
         <f t="shared" si="6"/>
-        <v>3.0452093117645997E-2</v>
+        <v>2.5655250878529656E-2</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -12156,19 +12213,19 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preec_untrt!C117*SimParameters!$B$4</f>
-        <v>4.8000000000000004E-3</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="D117" s="13">
         <f t="shared" si="5"/>
-        <v>-2.3166691299711561</v>
+        <v>-1.5279161859719514</v>
       </c>
       <c r="E117" s="13">
         <f>D117+LOG(SimParameters!$B$19)</f>
-        <v>-3.0156391343071749</v>
+        <v>-2.2268861903079702</v>
       </c>
       <c r="F117" s="13">
         <f t="shared" si="6"/>
-        <v>4.6724329063534874E-2</v>
+        <v>9.7361947798738122E-2</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -12180,19 +12237,19 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preec_untrt!C118*SimParameters!$B$4</f>
-        <v>9.6000000000000009E-3</v>
+        <v>3.8400000000000004E-2</v>
       </c>
       <c r="D118" s="13">
         <f t="shared" si="5"/>
-        <v>-2.0135393986364742</v>
+        <v>-1.3986632302911335</v>
       </c>
       <c r="E118" s="13">
         <f>D118+LOG(SimParameters!$B$19)</f>
-        <v>-2.712509402972493</v>
+        <v>-2.0976332346271525</v>
       </c>
       <c r="F118" s="13">
         <f t="shared" si="6"/>
-        <v>6.2239227813195554E-2</v>
+        <v>0.10932707117165556</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -12204,19 +12261,19 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preec_untrt!C119*SimParameters!$B$4</f>
-        <v>1.9200000000000002E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D119" s="13">
         <f t="shared" si="5"/>
-        <v>-1.7082792284707902</v>
+        <v>-1.2973957110088872</v>
       </c>
       <c r="E119" s="13">
         <f>D119+LOG(SimParameters!$B$19)</f>
-        <v>-2.4072492328068087</v>
+        <v>-1.9963657153449059</v>
       </c>
       <c r="F119" s="13">
         <f t="shared" si="6"/>
-        <v>8.2621573981492086E-2</v>
+        <v>0.11958502698246047</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -12228,19 +12285,19 @@
       </c>
       <c r="C120" s="4">
         <f>potential_preec_untrt!C120*SimParameters!$B$4</f>
-        <v>1.9200000000000002E-2</v>
+        <v>5.7599999999999998E-2</v>
       </c>
       <c r="D120" s="13">
         <f t="shared" si="5"/>
-        <v>-1.7082792284707902</v>
+        <v>-1.2138127940198145</v>
       </c>
       <c r="E120" s="13">
         <f>D120+LOG(SimParameters!$B$19)</f>
-        <v>-2.4072492328068087</v>
+        <v>-1.9127827983558332</v>
       </c>
       <c r="F120" s="13">
         <f t="shared" si="6"/>
-        <v>8.2621573981492086E-2</v>
+        <v>0.1286685418969449</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -12742,7 +12799,7 @@
       </c>
       <c r="C34" s="2">
         <f>potential_preg_untrt!C34*SimParameters!$B$22</f>
-        <v>3.7499999999999995E-4</v>
+        <v>8.7500000000000002E-4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -12754,7 +12811,7 @@
       </c>
       <c r="C35" s="2">
         <f>potential_preg_untrt!C35*SimParameters!$B$22</f>
-        <v>3.7499999999999995E-4</v>
+        <v>1.3750000000000001E-3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -12766,7 +12823,7 @@
       </c>
       <c r="C36" s="2">
         <f>potential_preg_untrt!C36*SimParameters!$B$22</f>
-        <v>2E-3</v>
+        <v>8.7500000000000008E-3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -12778,7 +12835,7 @@
       </c>
       <c r="C37" s="2">
         <f>potential_preg_untrt!C37*SimParameters!$B$22</f>
-        <v>2.9999999999999996E-3</v>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -13234,7 +13291,7 @@
       </c>
       <c r="C75" s="3">
         <f>C34*SimParameters!$B$9</f>
-        <v>4.125E-4</v>
+        <v>9.6250000000000014E-4</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -13246,7 +13303,7 @@
       </c>
       <c r="C76" s="3">
         <f>C35*SimParameters!$B$9</f>
-        <v>4.125E-4</v>
+        <v>1.5125000000000002E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -13258,7 +13315,7 @@
       </c>
       <c r="C77" s="3">
         <f>C36*SimParameters!$B$9</f>
-        <v>2.2000000000000001E-3</v>
+        <v>9.6250000000000016E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -13270,7 +13327,7 @@
       </c>
       <c r="C78" s="3">
         <f>C37*SimParameters!$B$9</f>
-        <v>3.3E-3</v>
+        <v>4.1250000000000002E-3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -13726,7 +13783,7 @@
       </c>
       <c r="C116" s="4">
         <f>C34*SimParameters!$B$16</f>
-        <v>4.4999999999999993E-4</v>
+        <v>1.0499999999999999E-3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -13738,7 +13795,7 @@
       </c>
       <c r="C117" s="4">
         <f>C35*SimParameters!$B$16</f>
-        <v>4.4999999999999993E-4</v>
+        <v>1.6500000000000002E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -13750,7 +13807,7 @@
       </c>
       <c r="C118" s="4">
         <f>C36*SimParameters!$B$16</f>
-        <v>2.3999999999999998E-3</v>
+        <v>1.0500000000000001E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -13762,7 +13819,7 @@
       </c>
       <c r="C119" s="4">
         <f>C37*SimParameters!$B$16</f>
-        <v>3.5999999999999995E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finalized parameters for generating prenatal encounters.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
+++ b/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F022E8E-339C-ED44-B7B8-2E3E517A4C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E358ED3-2EE4-7F4D-B194-4EA59AB7A172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="-21000" windowWidth="33600" windowHeight="21000" activeTab="7" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="13680" yWindow="-20500" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -74,6 +74,7 @@
     <author>tc={97E3E9D9-E3D7-4F43-B515-8C34E1CF5817}</author>
     <author>tc={22732877-B594-3A44-BC45-02143C03F17F}</author>
     <author>tc={EA6C2EE4-5812-B246-9332-1DE9E5ED6A26}</author>
+    <author>tc={2C5EF934-2828-4B4A-9619-70709D64AE47}</author>
     <author>tc={7B3AA43D-BF71-F649-BE1E-473187DEA264}</author>
   </authors>
   <commentList>
@@ -334,7 +335,15 @@
     Previously 0.7</t>
       </text>
     </comment>
-    <comment ref="D108" authorId="29" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
+    <comment ref="C60" authorId="29" shapeId="0" xr:uid="{2C5EF934-2828-4B4A-9619-70709D64AE47}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This corresponds to the outcome observed at GA from LMP = 20</t>
+      </text>
+    </comment>
+    <comment ref="D108" authorId="30" shapeId="0" xr:uid="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -548,8 +557,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={1E63AE57-A890-3A48-BD1B-8B7A590497DA}</author>
-    <author>tc={07325BD5-DBD7-D345-91E1-9899E6E1E2F8}</author>
-    <author>tc={2623C7C6-39C8-A44D-90FA-D0272993273C}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1E63AE57-A890-3A48-BD1B-8B7A590497DA}">
@@ -560,28 +567,12 @@
     These will need to be modified/played around with.</t>
       </text>
     </comment>
-    <comment ref="E13" authorId="1" shapeId="0" xr:uid="{07325BD5-DBD7-D345-91E1-9899E6E1E2F8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Check this math</t>
-      </text>
-    </comment>
-    <comment ref="E22" authorId="2" shapeId="0" xr:uid="{2623C7C6-39C8-A44D-90FA-D0272993273C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Check this math</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>p_fetaldeath</t>
   </si>
@@ -647,9 +638,6 @@
   </si>
   <si>
     <t>MarginalProb</t>
-  </si>
-  <si>
-    <t>WeeklyProb</t>
   </si>
   <si>
     <t>Description</t>
@@ -1092,6 +1080,9 @@
   </si>
   <si>
     <t>Difference in the log-odds of preeclampsia from the baseline levels.</t>
+  </si>
+  <si>
+    <t>g+B21</t>
   </si>
 </sst>
 </file>
@@ -1736,6 +1727,9 @@
   <threadedComment ref="D40" dT="2024-06-21T18:24:58.18" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{EA6C2EE4-5812-B246-9332-1DE9E5ED6A26}">
     <text>Previously 0.7</text>
   </threadedComment>
+  <threadedComment ref="C60" dT="2024-07-12T18:29:36.90" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2C5EF934-2828-4B4A-9619-70709D64AE47}">
+    <text>This corresponds to the outcome observed at GA from LMP = 20</text>
+  </threadedComment>
   <threadedComment ref="D108" dT="2023-10-20T20:36:59.95" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{7B3AA43D-BF71-F649-BE1E-473187DEA264}">
     <text>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</text>
   </threadedComment>
@@ -1853,12 +1847,6 @@
   <threadedComment ref="C1" dT="2024-04-19T19:01:33.29" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{1E63AE57-A890-3A48-BD1B-8B7A590497DA}">
     <text>These will need to be modified/played around with.</text>
   </threadedComment>
-  <threadedComment ref="E13" dT="2024-04-19T18:46:15.87" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{07325BD5-DBD7-D345-91E1-9899E6E1E2F8}" done="1">
-    <text>Check this math</text>
-  </threadedComment>
-  <threadedComment ref="E22" dT="2024-04-19T18:46:15.87" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{2623C7C6-39C8-A44D-90FA-D0272993273C}" done="1">
-    <text>Check this math</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1878,126 +1866,126 @@
   <sheetData>
     <row r="2" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="85" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="119" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="102" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="85" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="136" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="136" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="68" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="102" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2010,7 +1998,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2126,7 +2114,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2136,7 +2124,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2158,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101:C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3273,8 +3261,8 @@
         <v>17</v>
       </c>
       <c r="C60" s="3">
-        <f>C19*SimParameters!B9</f>
-        <v>1E-3</v>
+        <f>C19</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D60" s="3">
         <f t="shared" si="1"/>
@@ -3282,7 +3270,7 @@
       </c>
       <c r="E60" s="3">
         <f t="shared" si="2"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3293,8 +3281,8 @@
         <v>18</v>
       </c>
       <c r="C61" s="3">
-        <f>C20*SimParameters!B9</f>
-        <v>1E-3</v>
+        <f t="shared" ref="C61:C83" si="3">C20</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" si="1"/>
@@ -3302,7 +3290,7 @@
       </c>
       <c r="E61" s="3">
         <f t="shared" si="2"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3313,8 +3301,8 @@
         <v>19</v>
       </c>
       <c r="C62" s="3">
-        <f>C21*SimParameters!B9</f>
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D62" s="3">
         <f t="shared" si="1"/>
@@ -3322,7 +3310,7 @@
       </c>
       <c r="E62" s="3">
         <f t="shared" si="2"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -3333,8 +3321,8 @@
         <v>20</v>
       </c>
       <c r="C63" s="3">
-        <f>C22*SimParameters!B9</f>
-        <v>3.1250000000000001E-5</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D63" s="3">
         <f t="shared" si="1"/>
@@ -3342,7 +3330,7 @@
       </c>
       <c r="E63" s="3">
         <f t="shared" si="2"/>
-        <v>0.99996874999999996</v>
+        <v>0.99997499999999995</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3353,8 +3341,8 @@
         <v>21</v>
       </c>
       <c r="C64" s="3">
-        <f>C23*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D64" s="3">
         <f t="shared" si="1"/>
@@ -3362,7 +3350,7 @@
       </c>
       <c r="E64" s="3">
         <f t="shared" si="2"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3373,8 +3361,8 @@
         <v>22</v>
       </c>
       <c r="C65" s="3">
-        <f>C24*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D65" s="3">
         <f t="shared" si="1"/>
@@ -3382,7 +3370,7 @@
       </c>
       <c r="E65" s="3">
         <f t="shared" si="2"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3393,8 +3381,8 @@
         <v>23</v>
       </c>
       <c r="C66" s="3">
-        <f>C25*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D66" s="3">
         <f t="shared" si="1"/>
@@ -3402,7 +3390,7 @@
       </c>
       <c r="E66" s="3">
         <f t="shared" si="2"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -3413,8 +3401,8 @@
         <v>24</v>
       </c>
       <c r="C67" s="3">
-        <f>C26*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D67" s="3">
         <f t="shared" si="1"/>
@@ -3422,7 +3410,7 @@
       </c>
       <c r="E67" s="3">
         <f t="shared" si="2"/>
-        <v>0.99899925000000001</v>
+        <v>0.99899939999999998</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -3433,8 +3421,8 @@
         <v>25</v>
       </c>
       <c r="C68" s="3">
-        <f>C27*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D68" s="3">
         <f t="shared" si="1"/>
@@ -3442,7 +3430,7 @@
       </c>
       <c r="E68" s="3">
         <f t="shared" si="2"/>
-        <v>0.99849925000000006</v>
+        <v>0.99849940000000004</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -3453,8 +3441,8 @@
         <v>26</v>
       </c>
       <c r="C69" s="3">
-        <f>C28*SimParameters!B9</f>
-        <v>7.5000000000000002E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D69" s="3">
         <f t="shared" si="1"/>
@@ -3462,7 +3450,7 @@
       </c>
       <c r="E69" s="3">
         <f t="shared" si="2"/>
-        <v>0.99819924999999998</v>
+        <v>0.99819939999999996</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -3473,8 +3461,8 @@
         <v>27</v>
       </c>
       <c r="C70" s="3">
-        <f>C29*SimParameters!B9</f>
-        <v>7.5000000000000002E-6</v>
+        <f t="shared" si="3"/>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="D70" s="3">
         <f t="shared" si="1"/>
@@ -3482,7 +3470,7 @@
       </c>
       <c r="E70" s="3">
         <f t="shared" si="2"/>
-        <v>0.99799249999999995</v>
+        <v>0.99799400000000005</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -3493,8 +3481,8 @@
         <v>28</v>
       </c>
       <c r="C71" s="3">
-        <f>C30*SimParameters!B9</f>
-        <v>3.1250000000000001E-5</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D71" s="3">
         <f t="shared" si="1"/>
@@ -3502,7 +3490,7 @@
       </c>
       <c r="E71" s="3">
         <f t="shared" si="2"/>
-        <v>0.99696874999999996</v>
+        <v>0.99697499999999994</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -3513,8 +3501,8 @@
         <v>29</v>
       </c>
       <c r="C72" s="3">
-        <f>C31*SimParameters!B9</f>
-        <v>3.1250000000000001E-5</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D72" s="3">
         <f t="shared" si="1"/>
@@ -3522,7 +3510,7 @@
       </c>
       <c r="E72" s="3">
         <f t="shared" si="2"/>
-        <v>0.99496874999999996</v>
+        <v>0.99497499999999994</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -3533,8 +3521,8 @@
         <v>30</v>
       </c>
       <c r="C73" s="3">
-        <f>C32*SimParameters!B9</f>
-        <v>3.1250000000000001E-5</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D73" s="3">
         <f t="shared" si="1"/>
@@ -3542,7 +3530,7 @@
       </c>
       <c r="E73" s="3">
         <f t="shared" si="2"/>
-        <v>0.99396874999999996</v>
+        <v>0.99397499999999994</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -3553,8 +3541,8 @@
         <v>31</v>
       </c>
       <c r="C74" s="3">
-        <f>C33*SimParameters!B9</f>
-        <v>1.8749999999999998E-4</v>
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D74" s="3">
         <f t="shared" si="1"/>
@@ -3562,7 +3550,7 @@
       </c>
       <c r="E74" s="3">
         <f t="shared" si="2"/>
-        <v>0.99181249999999999</v>
+        <v>0.99185000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -3573,8 +3561,8 @@
         <v>32</v>
       </c>
       <c r="C75" s="3">
-        <f>C34*SimParameters!B9</f>
-        <v>4.3750000000000001E-4</v>
+        <f t="shared" si="3"/>
+        <v>3.5E-4</v>
       </c>
       <c r="D75" s="3">
         <f t="shared" si="1"/>
@@ -3582,7 +3570,7 @@
       </c>
       <c r="E75" s="3">
         <f t="shared" si="2"/>
-        <v>0.94956249999999998</v>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -3593,8 +3581,8 @@
         <v>33</v>
       </c>
       <c r="C76" s="3">
-        <f>C35*SimParameters!B9</f>
-        <v>6.8750000000000007E-4</v>
+        <f t="shared" si="3"/>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D76" s="3">
         <f t="shared" si="1"/>
@@ -3602,7 +3590,7 @@
       </c>
       <c r="E76" s="3">
         <f t="shared" si="2"/>
-        <v>0.91931250000000009</v>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -3613,8 +3601,8 @@
         <v>34</v>
       </c>
       <c r="C77" s="3">
-        <f>C36*SimParameters!B9</f>
-        <v>4.3750000000000004E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D77" s="3">
         <f t="shared" si="1"/>
@@ -3622,7 +3610,7 @@
       </c>
       <c r="E77" s="3">
         <f t="shared" si="2"/>
-        <v>0.645625</v>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -3633,8 +3621,8 @@
         <v>35</v>
       </c>
       <c r="C78" s="3">
-        <f>C37*SimParameters!B9</f>
-        <v>1.8749999999999999E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.5E-3</v>
       </c>
       <c r="D78" s="3">
         <f t="shared" si="1"/>
@@ -3642,7 +3630,7 @@
       </c>
       <c r="E78" s="3">
         <f t="shared" si="2"/>
-        <v>0.59812500000000002</v>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -3653,8 +3641,8 @@
         <v>36</v>
       </c>
       <c r="C79" s="3">
-        <f>C38*SimParameters!B9</f>
-        <v>2E-3</v>
+        <f t="shared" si="3"/>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D79" s="3">
         <f t="shared" si="1"/>
@@ -3662,7 +3650,7 @@
       </c>
       <c r="E79" s="3">
         <f t="shared" si="2"/>
-        <v>0.29800000000000004</v>
+        <v>0.2984</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -3673,8 +3661,8 @@
         <v>37</v>
       </c>
       <c r="C80" s="3">
-        <f>C39*SimParameters!B9</f>
-        <v>7.4999999999999997E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D80" s="3">
         <f t="shared" si="1"/>
@@ -3682,7 +3670,7 @@
       </c>
       <c r="E80" s="3">
         <f t="shared" si="2"/>
-        <v>0.29250000000000009</v>
+        <v>0.29400000000000004</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -3693,8 +3681,8 @@
         <v>38</v>
       </c>
       <c r="C81" s="3">
-        <f>C40*SimParameters!B9</f>
-        <v>1.2500000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.01</v>
       </c>
       <c r="D81" s="3">
         <f t="shared" si="1"/>
@@ -3702,7 +3690,7 @@
       </c>
       <c r="E81" s="3">
         <f t="shared" si="2"/>
-        <v>0.13750000000000007</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -3713,8 +3701,8 @@
         <v>39</v>
       </c>
       <c r="C82" s="3">
-        <f>C41*SimParameters!B9</f>
-        <v>0.25</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="D82" s="3">
         <f t="shared" si="1"/>
@@ -3722,7 +3710,7 @@
       </c>
       <c r="E82" s="3">
         <f t="shared" si="2"/>
-        <v>5.0000000000000044E-2</v>
+        <v>0.10000000000000009</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -3733,8 +3721,8 @@
         <v>40</v>
       </c>
       <c r="C83" s="3">
-        <f>C42*SimParameters!B9</f>
-        <v>0.25</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="D83" s="3">
         <f t="shared" si="1"/>
@@ -3776,7 +3764,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="D85" s="4">
-        <f t="shared" ref="D85:D124" si="3">D3</f>
+        <f t="shared" ref="D85:D124" si="4">D3</f>
         <v>0</v>
       </c>
       <c r="E85" s="4">
@@ -3796,7 +3784,7 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="D86" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E86" s="4">
@@ -3816,7 +3804,7 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="D87" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E87" s="4">
@@ -3836,7 +3824,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="D88" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E88" s="4">
@@ -3856,11 +3844,11 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="D89" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E89" s="4">
-        <f t="shared" ref="E89:E123" si="4">1-C89-D89</f>
+        <f t="shared" ref="E89:E123" si="5">1-C89-D89</f>
         <v>0.85</v>
       </c>
     </row>
@@ -3876,11 +3864,11 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="D90" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E90" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.86499999999999999</v>
       </c>
     </row>
@@ -3896,11 +3884,11 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.86499999999999999</v>
       </c>
     </row>
@@ -3916,11 +3904,11 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D92" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97750000000000004</v>
       </c>
     </row>
@@ -3936,11 +3924,11 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D93" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97750000000000004</v>
       </c>
     </row>
@@ -3956,11 +3944,11 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D94" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97750000000000004</v>
       </c>
     </row>
@@ -3976,11 +3964,11 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D95" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.97750000000000004</v>
       </c>
     </row>
@@ -3996,11 +3984,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D96" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -4016,11 +4004,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D97" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -4036,11 +4024,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D98" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -4056,11 +4044,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D99" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -4076,11 +4064,11 @@
         <v>1.2000000000000001E-3</v>
       </c>
       <c r="D100" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.99880000000000002</v>
       </c>
     </row>
@@ -4092,16 +4080,16 @@
         <v>17</v>
       </c>
       <c r="C101" s="4">
-        <f>C19*SimParameters!B10</f>
-        <v>1.2000000000000001E-3</v>
+        <f>C19</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D101" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99880000000000002</v>
+        <f t="shared" si="5"/>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -4112,16 +4100,16 @@
         <v>18</v>
       </c>
       <c r="C102" s="4">
-        <f>C20*SimParameters!B10</f>
-        <v>1.2000000000000001E-3</v>
+        <f t="shared" ref="C102:C124" si="6">C20</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D102" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99880000000000002</v>
+        <f t="shared" si="5"/>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -4132,16 +4120,16 @@
         <v>19</v>
       </c>
       <c r="C103" s="4">
-        <f>C21*SimParameters!B10</f>
-        <v>1.2000000000000001E-3</v>
+        <f t="shared" si="6"/>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D103" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99880000000000002</v>
+        <f t="shared" si="5"/>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -4152,16 +4140,16 @@
         <v>20</v>
       </c>
       <c r="C104" s="4">
-        <f>C22*SimParameters!B10</f>
-        <v>3.7500000000000003E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D104" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99996249999999998</v>
+        <f t="shared" si="5"/>
+        <v>0.99997499999999995</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -4172,16 +4160,16 @@
         <v>21</v>
       </c>
       <c r="C105" s="4">
-        <f>C23*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D105" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99998910000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -4192,16 +4180,16 @@
         <v>22</v>
       </c>
       <c r="C106" s="4">
-        <f>C24*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D106" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99998910000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -4212,16 +4200,16 @@
         <v>23</v>
       </c>
       <c r="C107" s="4">
-        <f>C25*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D107" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99998910000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -4232,16 +4220,16 @@
         <v>24</v>
       </c>
       <c r="C108" s="4">
-        <f>C26*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D108" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1E-3</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99899910000000003</v>
+        <f t="shared" si="5"/>
+        <v>0.99899939999999998</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -4252,16 +4240,16 @@
         <v>25</v>
       </c>
       <c r="C109" s="4">
-        <f>C27*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D109" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5E-3</v>
       </c>
       <c r="E109" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99849910000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.99849940000000004</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -4272,16 +4260,16 @@
         <v>26</v>
       </c>
       <c r="C110" s="4">
-        <f>C28*SimParameters!B10</f>
-        <v>8.9999999999999996E-7</v>
+        <f t="shared" si="6"/>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D110" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.8E-3</v>
       </c>
       <c r="E110" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99819910000000001</v>
+        <f t="shared" si="5"/>
+        <v>0.99819939999999996</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -4292,16 +4280,16 @@
         <v>27</v>
       </c>
       <c r="C111" s="4">
-        <f>C29*SimParameters!B10</f>
-        <v>9.0000000000000002E-6</v>
+        <f t="shared" si="6"/>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="D111" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2E-3</v>
       </c>
       <c r="E111" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99799099999999996</v>
+        <f t="shared" si="5"/>
+        <v>0.99799400000000005</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -4312,16 +4300,16 @@
         <v>28</v>
       </c>
       <c r="C112" s="4">
-        <f>C30*SimParameters!B10</f>
-        <v>3.7500000000000003E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D112" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E112" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99696249999999997</v>
+        <f t="shared" si="5"/>
+        <v>0.99697499999999994</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -4332,16 +4320,16 @@
         <v>29</v>
       </c>
       <c r="C113" s="4">
-        <f>C31*SimParameters!B10</f>
-        <v>3.7500000000000003E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D113" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E113" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99496249999999997</v>
+        <f t="shared" si="5"/>
+        <v>0.99497499999999994</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -4352,16 +4340,16 @@
         <v>30</v>
       </c>
       <c r="C114" s="4">
-        <f>C32*SimParameters!B10</f>
-        <v>3.7500000000000003E-5</v>
+        <f t="shared" si="6"/>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D114" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="E114" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99396249999999997</v>
+        <f t="shared" si="5"/>
+        <v>0.99397499999999994</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -4372,16 +4360,16 @@
         <v>31</v>
       </c>
       <c r="C115" s="4">
-        <f>C33*SimParameters!B10</f>
-        <v>2.2499999999999999E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D115" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E115" s="4">
-        <f t="shared" si="4"/>
-        <v>0.99177499999999996</v>
+        <f t="shared" si="5"/>
+        <v>0.99185000000000001</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -4392,16 +4380,16 @@
         <v>32</v>
       </c>
       <c r="C116" s="4">
-        <f>C34*SimParameters!B10</f>
-        <v>5.2499999999999997E-4</v>
+        <f t="shared" si="6"/>
+        <v>3.5E-4</v>
       </c>
       <c r="D116" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="E116" s="4">
-        <f t="shared" si="4"/>
-        <v>0.94947499999999996</v>
+        <f t="shared" si="5"/>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -4412,16 +4400,16 @@
         <v>33</v>
       </c>
       <c r="C117" s="4">
-        <f>C35*SimParameters!B10</f>
-        <v>8.25E-4</v>
+        <f t="shared" si="6"/>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D117" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.08</v>
       </c>
       <c r="E117" s="4">
-        <f t="shared" si="4"/>
-        <v>0.91917500000000008</v>
+        <f t="shared" si="5"/>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -4432,16 +4420,16 @@
         <v>34</v>
       </c>
       <c r="C118" s="4">
-        <f>C36*SimParameters!B10</f>
-        <v>5.2500000000000003E-3</v>
+        <f t="shared" si="6"/>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D118" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.35</v>
       </c>
       <c r="E118" s="4">
-        <f t="shared" si="4"/>
-        <v>0.64475000000000005</v>
+        <f t="shared" si="5"/>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -4452,16 +4440,16 @@
         <v>35</v>
       </c>
       <c r="C119" s="4">
-        <f>C37*SimParameters!B10</f>
-        <v>2.2500000000000003E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.5E-3</v>
       </c>
       <c r="D119" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
       <c r="E119" s="4">
-        <f t="shared" si="4"/>
-        <v>0.59775</v>
+        <f t="shared" si="5"/>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -4472,16 +4460,16 @@
         <v>36</v>
       </c>
       <c r="C120" s="4">
-        <f>C38*SimParameters!B10</f>
-        <v>2.4000000000000002E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D120" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E120" s="4">
-        <f t="shared" si="4"/>
-        <v>0.29760000000000009</v>
+        <f t="shared" si="5"/>
+        <v>0.2984</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -4492,16 +4480,16 @@
         <v>37</v>
       </c>
       <c r="C121" s="4">
-        <f>C39*SimParameters!B10</f>
-        <v>9.0000000000000011E-3</v>
+        <f t="shared" si="6"/>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D121" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E121" s="4">
-        <f t="shared" si="4"/>
-        <v>0.29100000000000004</v>
+        <f t="shared" si="5"/>
+        <v>0.29400000000000004</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -4512,16 +4500,16 @@
         <v>38</v>
       </c>
       <c r="C122" s="4">
-        <f>C40*SimParameters!B10</f>
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.01</v>
       </c>
       <c r="D122" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.85</v>
       </c>
       <c r="E122" s="4">
-        <f t="shared" si="4"/>
-        <v>0.13500000000000001</v>
+        <f t="shared" si="5"/>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -4532,16 +4520,16 @@
         <v>39</v>
       </c>
       <c r="C123" s="4">
-        <f>C41*SimParameters!B10</f>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="6"/>
+        <v>0.2</v>
       </c>
       <c r="D123" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="E123" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.10000000000000009</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -4552,11 +4540,11 @@
         <v>40</v>
       </c>
       <c r="C124" s="4">
-        <f>C42*SimParameters!B10</f>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="6"/>
+        <v>0.2</v>
       </c>
       <c r="D124" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="E124" s="4">
@@ -4573,8 +4561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="I120" sqref="I120"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5770,7 +5758,7 @@
       </c>
       <c r="C60" s="3">
         <f>potential_preg_untrt!C60</f>
-        <v>1E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D60" s="3">
         <f>potential_preg_untrt!D60</f>
@@ -5778,7 +5766,7 @@
       </c>
       <c r="E60" s="3">
         <f t="shared" si="1"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -5790,7 +5778,7 @@
       </c>
       <c r="C61" s="3">
         <f>potential_preg_untrt!C61</f>
-        <v>1E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D61" s="3">
         <f>potential_preg_untrt!D61</f>
@@ -5798,7 +5786,7 @@
       </c>
       <c r="E61" s="3">
         <f t="shared" si="1"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -5810,7 +5798,7 @@
       </c>
       <c r="C62" s="3">
         <f>potential_preg_untrt!C62</f>
-        <v>1E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D62" s="3">
         <f>potential_preg_untrt!D62</f>
@@ -5818,7 +5806,7 @@
       </c>
       <c r="E62" s="3">
         <f t="shared" si="1"/>
-        <v>0.999</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -5830,7 +5818,7 @@
       </c>
       <c r="C63" s="3">
         <f>potential_preg_untrt!C63</f>
-        <v>3.1250000000000001E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D63" s="3">
         <f>potential_preg_untrt!D63</f>
@@ -5838,7 +5826,7 @@
       </c>
       <c r="E63" s="3">
         <f t="shared" si="1"/>
-        <v>0.99996874999999996</v>
+        <v>0.99997499999999995</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -5850,7 +5838,7 @@
       </c>
       <c r="C64" s="3">
         <f>potential_preg_untrt!C64</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D64" s="3">
         <f>potential_preg_untrt!D64</f>
@@ -5858,7 +5846,7 @@
       </c>
       <c r="E64" s="3">
         <f t="shared" si="1"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -5870,7 +5858,7 @@
       </c>
       <c r="C65" s="3">
         <f>potential_preg_untrt!C65</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D65" s="3">
         <f>potential_preg_untrt!D65</f>
@@ -5878,7 +5866,7 @@
       </c>
       <c r="E65" s="3">
         <f t="shared" si="1"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -5890,7 +5878,7 @@
       </c>
       <c r="C66" s="3">
         <f>potential_preg_untrt!C66</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D66" s="3">
         <f>potential_preg_untrt!D66</f>
@@ -5898,7 +5886,7 @@
       </c>
       <c r="E66" s="3">
         <f t="shared" si="1"/>
-        <v>0.99998925000000005</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -5910,7 +5898,7 @@
       </c>
       <c r="C67" s="3">
         <f>potential_preg_untrt!C67</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D67" s="3">
         <f>potential_preg_untrt!D67</f>
@@ -5918,7 +5906,7 @@
       </c>
       <c r="E67" s="3">
         <f t="shared" si="1"/>
-        <v>0.99899925000000001</v>
+        <v>0.99899939999999998</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -5930,7 +5918,7 @@
       </c>
       <c r="C68" s="3">
         <f>potential_preg_untrt!C68</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D68" s="3">
         <f>potential_preg_untrt!D68</f>
@@ -5938,7 +5926,7 @@
       </c>
       <c r="E68" s="3">
         <f t="shared" si="1"/>
-        <v>0.99849925000000006</v>
+        <v>0.99849940000000004</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -5950,7 +5938,7 @@
       </c>
       <c r="C69" s="3">
         <f>potential_preg_untrt!C69</f>
-        <v>7.5000000000000002E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D69" s="3">
         <f>potential_preg_untrt!D69</f>
@@ -5958,7 +5946,7 @@
       </c>
       <c r="E69" s="3">
         <f t="shared" si="1"/>
-        <v>0.99819924999999998</v>
+        <v>0.99819939999999996</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -5970,7 +5958,7 @@
       </c>
       <c r="C70" s="3">
         <f>potential_preg_untrt!C70</f>
-        <v>7.5000000000000002E-6</v>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="D70" s="3">
         <f>potential_preg_untrt!D70</f>
@@ -5978,7 +5966,7 @@
       </c>
       <c r="E70" s="3">
         <f t="shared" si="1"/>
-        <v>0.99799249999999995</v>
+        <v>0.99799400000000005</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -5990,7 +5978,7 @@
       </c>
       <c r="C71" s="3">
         <f>potential_preg_untrt!C71</f>
-        <v>3.1250000000000001E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D71" s="3">
         <f>potential_preg_untrt!D71</f>
@@ -5998,7 +5986,7 @@
       </c>
       <c r="E71" s="3">
         <f t="shared" si="1"/>
-        <v>0.99696874999999996</v>
+        <v>0.99697499999999994</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -6010,7 +5998,7 @@
       </c>
       <c r="C72" s="3">
         <f>potential_preg_untrt!C72</f>
-        <v>3.1250000000000001E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D72" s="3">
         <f>potential_preg_untrt!D72</f>
@@ -6018,7 +6006,7 @@
       </c>
       <c r="E72" s="3">
         <f t="shared" si="1"/>
-        <v>0.99496874999999996</v>
+        <v>0.99497499999999994</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -6030,7 +6018,7 @@
       </c>
       <c r="C73" s="3">
         <f>potential_preg_untrt!C73</f>
-        <v>3.1250000000000001E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D73" s="3">
         <f>potential_preg_untrt!D73</f>
@@ -6038,7 +6026,7 @@
       </c>
       <c r="E73" s="3">
         <f t="shared" si="1"/>
-        <v>0.99396874999999996</v>
+        <v>0.99397499999999994</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -6050,7 +6038,7 @@
       </c>
       <c r="C74" s="3">
         <f>potential_preg_untrt!C74</f>
-        <v>1.8749999999999998E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D74" s="3">
         <f>potential_preg_untrt!D74</f>
@@ -6058,7 +6046,7 @@
       </c>
       <c r="E74" s="3">
         <f t="shared" si="1"/>
-        <v>0.99181249999999999</v>
+        <v>0.99185000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -6070,7 +6058,7 @@
       </c>
       <c r="C75" s="3">
         <f>potential_preg_untrt!C75</f>
-        <v>4.3750000000000001E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D75" s="3">
         <f>potential_preg_untrt!D75</f>
@@ -6078,7 +6066,7 @@
       </c>
       <c r="E75" s="3">
         <f t="shared" si="1"/>
-        <v>0.94956249999999998</v>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -6090,7 +6078,7 @@
       </c>
       <c r="C76" s="3">
         <f>potential_preg_untrt!C76</f>
-        <v>6.8750000000000007E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D76" s="3">
         <f>potential_preg_untrt!D76</f>
@@ -6098,7 +6086,7 @@
       </c>
       <c r="E76" s="3">
         <f t="shared" si="1"/>
-        <v>0.91931250000000009</v>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -6110,7 +6098,7 @@
       </c>
       <c r="C77" s="3">
         <f>potential_preg_untrt!C77</f>
-        <v>4.3750000000000004E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D77" s="3">
         <f>potential_preg_untrt!D77</f>
@@ -6118,7 +6106,7 @@
       </c>
       <c r="E77" s="3">
         <f t="shared" si="1"/>
-        <v>0.645625</v>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -6130,7 +6118,7 @@
       </c>
       <c r="C78" s="3">
         <f>potential_preg_untrt!C78</f>
-        <v>1.8749999999999999E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D78" s="3">
         <f>potential_preg_untrt!D78</f>
@@ -6138,7 +6126,7 @@
       </c>
       <c r="E78" s="3">
         <f t="shared" si="1"/>
-        <v>0.59812500000000002</v>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -6150,7 +6138,7 @@
       </c>
       <c r="C79" s="3">
         <f>potential_preg_untrt!C79</f>
-        <v>2E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D79" s="3">
         <f>potential_preg_untrt!D79</f>
@@ -6158,7 +6146,7 @@
       </c>
       <c r="E79" s="3">
         <f t="shared" si="1"/>
-        <v>0.29800000000000004</v>
+        <v>0.2984</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -6170,7 +6158,7 @@
       </c>
       <c r="C80" s="3">
         <f>potential_preg_untrt!C80</f>
-        <v>7.4999999999999997E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D80" s="3">
         <f>potential_preg_untrt!D80</f>
@@ -6178,7 +6166,7 @@
       </c>
       <c r="E80" s="3">
         <f t="shared" si="1"/>
-        <v>0.29250000000000009</v>
+        <v>0.29400000000000004</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -6190,7 +6178,7 @@
       </c>
       <c r="C81" s="3">
         <f>potential_preg_untrt!C81</f>
-        <v>1.2500000000000001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D81" s="3">
         <f>potential_preg_untrt!D81</f>
@@ -6198,7 +6186,7 @@
       </c>
       <c r="E81" s="3">
         <f t="shared" si="1"/>
-        <v>0.13750000000000007</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -6210,7 +6198,7 @@
       </c>
       <c r="C82" s="3">
         <f>potential_preg_untrt!C82</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D82" s="3">
         <f>potential_preg_untrt!D82</f>
@@ -6218,7 +6206,7 @@
       </c>
       <c r="E82" s="3">
         <f t="shared" si="1"/>
-        <v>5.0000000000000044E-2</v>
+        <v>0.10000000000000009</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -6230,7 +6218,7 @@
       </c>
       <c r="C83" s="3">
         <f>potential_preg_untrt!C83</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D83" s="3">
         <f>potential_preg_untrt!D83</f>
@@ -6589,7 +6577,7 @@
       </c>
       <c r="C101" s="4">
         <f>potential_preg_untrt!C101</f>
-        <v>1.2000000000000001E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D101" s="4">
         <f>potential_preg_untrt!D101</f>
@@ -6597,7 +6585,7 @@
       </c>
       <c r="E101" s="4">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -6609,7 +6597,7 @@
       </c>
       <c r="C102" s="4">
         <f>potential_preg_untrt!C102</f>
-        <v>1.2000000000000001E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D102" s="4">
         <f>potential_preg_untrt!D102</f>
@@ -6617,7 +6605,7 @@
       </c>
       <c r="E102" s="4">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -6629,7 +6617,7 @@
       </c>
       <c r="C103" s="4">
         <f>potential_preg_untrt!C103</f>
-        <v>1.2000000000000001E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D103" s="4">
         <f>potential_preg_untrt!D103</f>
@@ -6637,7 +6625,7 @@
       </c>
       <c r="E103" s="4">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99919999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -6649,7 +6637,7 @@
       </c>
       <c r="C104" s="4">
         <f>potential_preg_untrt!C104</f>
-        <v>3.7500000000000003E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D104" s="4">
         <f>potential_preg_untrt!D104</f>
@@ -6657,7 +6645,7 @@
       </c>
       <c r="E104" s="4">
         <f t="shared" si="2"/>
-        <v>0.99996249999999998</v>
+        <v>0.99997499999999995</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -6669,7 +6657,7 @@
       </c>
       <c r="C105" s="4">
         <f>potential_preg_untrt!C105</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D105" s="4">
         <f>potential_preg_untrt!D105</f>
@@ -6677,7 +6665,7 @@
       </c>
       <c r="E105" s="4">
         <f t="shared" si="2"/>
-        <v>0.99998910000000008</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -6689,7 +6677,7 @@
       </c>
       <c r="C106" s="4">
         <f>potential_preg_untrt!C106</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D106" s="4">
         <f>potential_preg_untrt!D106</f>
@@ -6697,7 +6685,7 @@
       </c>
       <c r="E106" s="4">
         <f t="shared" si="2"/>
-        <v>0.99998910000000008</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -6709,7 +6697,7 @@
       </c>
       <c r="C107" s="4">
         <f>potential_preg_untrt!C107</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D107" s="4">
         <f>potential_preg_untrt!D107</f>
@@ -6717,7 +6705,7 @@
       </c>
       <c r="E107" s="4">
         <f t="shared" si="2"/>
-        <v>0.99998910000000008</v>
+        <v>0.99998940000000003</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -6729,7 +6717,7 @@
       </c>
       <c r="C108" s="4">
         <f>potential_preg_untrt!C108</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D108" s="4">
         <f>potential_preg_untrt!D108</f>
@@ -6737,7 +6725,7 @@
       </c>
       <c r="E108" s="4">
         <f t="shared" si="2"/>
-        <v>0.99899910000000003</v>
+        <v>0.99899939999999998</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -6749,7 +6737,7 @@
       </c>
       <c r="C109" s="4">
         <f>potential_preg_untrt!C109</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D109" s="4">
         <f>potential_preg_untrt!D109</f>
@@ -6757,7 +6745,7 @@
       </c>
       <c r="E109" s="4">
         <f t="shared" si="2"/>
-        <v>0.99849910000000008</v>
+        <v>0.99849940000000004</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -6769,7 +6757,7 @@
       </c>
       <c r="C110" s="4">
         <f>potential_preg_untrt!C110</f>
-        <v>8.9999999999999996E-7</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="D110" s="4">
         <f>potential_preg_untrt!D110</f>
@@ -6777,7 +6765,7 @@
       </c>
       <c r="E110" s="4">
         <f t="shared" si="2"/>
-        <v>0.99819910000000001</v>
+        <v>0.99819939999999996</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -6789,7 +6777,7 @@
       </c>
       <c r="C111" s="4">
         <f>potential_preg_untrt!C111</f>
-        <v>9.0000000000000002E-6</v>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="D111" s="4">
         <f>potential_preg_untrt!D111</f>
@@ -6797,7 +6785,7 @@
       </c>
       <c r="E111" s="4">
         <f t="shared" si="2"/>
-        <v>0.99799099999999996</v>
+        <v>0.99799400000000005</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -6809,7 +6797,7 @@
       </c>
       <c r="C112" s="4">
         <f>potential_preg_untrt!C112</f>
-        <v>3.7500000000000003E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D112" s="4">
         <f>potential_preg_untrt!D112</f>
@@ -6817,7 +6805,7 @@
       </c>
       <c r="E112" s="4">
         <f t="shared" si="2"/>
-        <v>0.99696249999999997</v>
+        <v>0.99697499999999994</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -6829,7 +6817,7 @@
       </c>
       <c r="C113" s="4">
         <f>potential_preg_untrt!C113</f>
-        <v>3.7500000000000003E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D113" s="4">
         <f>potential_preg_untrt!D113</f>
@@ -6837,7 +6825,7 @@
       </c>
       <c r="E113" s="4">
         <f t="shared" si="2"/>
-        <v>0.99496249999999997</v>
+        <v>0.99497499999999994</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -6849,7 +6837,7 @@
       </c>
       <c r="C114" s="4">
         <f>potential_preg_untrt!C114</f>
-        <v>3.7500000000000003E-5</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="D114" s="4">
         <f>potential_preg_untrt!D114</f>
@@ -6857,7 +6845,7 @@
       </c>
       <c r="E114" s="4">
         <f t="shared" si="2"/>
-        <v>0.99396249999999997</v>
+        <v>0.99397499999999994</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -6869,7 +6857,7 @@
       </c>
       <c r="C115" s="4">
         <f>potential_preg_untrt!C115</f>
-        <v>2.2499999999999999E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D115" s="4">
         <f>potential_preg_untrt!D115</f>
@@ -6877,7 +6865,7 @@
       </c>
       <c r="E115" s="4">
         <f t="shared" si="2"/>
-        <v>0.99177499999999996</v>
+        <v>0.99185000000000001</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -6889,7 +6877,7 @@
       </c>
       <c r="C116" s="4">
         <f>potential_preg_untrt!C116</f>
-        <v>5.2499999999999997E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D116" s="4">
         <f>potential_preg_untrt!D116</f>
@@ -6897,7 +6885,7 @@
       </c>
       <c r="E116" s="4">
         <f t="shared" si="2"/>
-        <v>0.94947499999999996</v>
+        <v>0.94964999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -6909,7 +6897,7 @@
       </c>
       <c r="C117" s="4">
         <f>potential_preg_untrt!C117</f>
-        <v>8.25E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D117" s="4">
         <f>potential_preg_untrt!D117</f>
@@ -6917,7 +6905,7 @@
       </c>
       <c r="E117" s="4">
         <f t="shared" si="2"/>
-        <v>0.91917500000000008</v>
+        <v>0.91944999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -6929,7 +6917,7 @@
       </c>
       <c r="C118" s="4">
         <f>potential_preg_untrt!C118</f>
-        <v>5.2500000000000003E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D118" s="4">
         <f>potential_preg_untrt!D118</f>
@@ -6937,7 +6925,7 @@
       </c>
       <c r="E118" s="4">
         <f t="shared" si="2"/>
-        <v>0.64475000000000005</v>
+        <v>0.64650000000000007</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -6949,7 +6937,7 @@
       </c>
       <c r="C119" s="4">
         <f>potential_preg_untrt!C119</f>
-        <v>2.2500000000000003E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D119" s="4">
         <f>potential_preg_untrt!D119</f>
@@ -6957,7 +6945,7 @@
       </c>
       <c r="E119" s="4">
         <f t="shared" si="2"/>
-        <v>0.59775</v>
+        <v>0.59850000000000003</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -6969,7 +6957,7 @@
       </c>
       <c r="C120" s="4">
         <f>potential_preg_untrt!C120</f>
-        <v>2.4000000000000002E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D120" s="4">
         <f>potential_preg_untrt!D120</f>
@@ -6977,7 +6965,7 @@
       </c>
       <c r="E120" s="4">
         <f t="shared" si="2"/>
-        <v>0.29760000000000009</v>
+        <v>0.2984</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -6989,7 +6977,7 @@
       </c>
       <c r="C121" s="4">
         <f>potential_preg_untrt!C121</f>
-        <v>9.0000000000000011E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D121" s="4">
         <f>potential_preg_untrt!D121</f>
@@ -6997,7 +6985,7 @@
       </c>
       <c r="E121" s="4">
         <f t="shared" si="2"/>
-        <v>0.29100000000000004</v>
+        <v>0.29400000000000004</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -7009,7 +6997,7 @@
       </c>
       <c r="C122" s="4">
         <f>potential_preg_untrt!C122</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D122" s="4">
         <f>potential_preg_untrt!D122</f>
@@ -7017,7 +7005,7 @@
       </c>
       <c r="E122" s="4">
         <f t="shared" si="2"/>
-        <v>0.13500000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -7029,7 +7017,7 @@
       </c>
       <c r="C123" s="4">
         <f>potential_preg_untrt!C123</f>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="D123" s="4">
         <f>potential_preg_untrt!D123</f>
@@ -7037,7 +7025,7 @@
       </c>
       <c r="E123" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -7049,7 +7037,7 @@
       </c>
       <c r="C124" s="4">
         <f>potential_preg_untrt!C124</f>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="D124" s="4">
         <f>potential_preg_untrt!D124</f>
@@ -7069,7 +7057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870C18B-8ADE-814A-BF98-16981C435EF7}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -7093,10 +7081,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -9717,8 +9705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBCDA1E-E196-5243-A50A-855DF45BB886}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9741,10 +9729,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -12406,8 +12394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E248214-C639-FE41-8DE0-FF7112935623}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12906,7 +12894,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="3">
-        <f>C2*SimParameters!$B$9</f>
+        <f>C2</f>
         <v>0</v>
       </c>
     </row>
@@ -12918,7 +12906,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="3">
-        <f>C3*SimParameters!$B$9</f>
+        <f t="shared" ref="C44:C63" si="0">C3</f>
         <v>0</v>
       </c>
     </row>
@@ -12930,7 +12918,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="3">
-        <f>C4*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12942,7 +12930,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="3">
-        <f>C5*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12954,7 +12942,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="3">
-        <f>C6*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12966,7 +12954,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="3">
-        <f>C7*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12978,7 +12966,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="3">
-        <f>C8*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -12990,7 +12978,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="3">
-        <f>C9*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13002,7 +12990,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="3">
-        <f>C10*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13014,7 +13002,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="3">
-        <f>C11*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13026,7 +13014,7 @@
         <v>10</v>
       </c>
       <c r="C53" s="3">
-        <f>C12*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13038,7 +13026,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="3">
-        <f>C13*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13050,7 +13038,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="3">
-        <f>C14*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13062,7 +13050,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="3">
-        <f>C15*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13074,7 +13062,7 @@
         <v>14</v>
       </c>
       <c r="C57" s="3">
-        <f>C16*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13086,7 +13074,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="3">
-        <f>C17*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13098,7 +13086,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="3">
-        <f>C18*SimParameters!$B$9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -13110,7 +13098,7 @@
         <v>17</v>
       </c>
       <c r="C60" s="3">
-        <f>C19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -13122,7 +13110,7 @@
         <v>18</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" ref="C61:C66" si="0">C20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -13158,7 +13146,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C61:C66" si="1">C23</f>
         <v>0.5</v>
       </c>
     </row>
@@ -13170,7 +13158,7 @@
         <v>22</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -13182,7 +13170,7 @@
         <v>23</v>
       </c>
       <c r="C66" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -13194,8 +13182,8 @@
         <v>24</v>
       </c>
       <c r="C67" s="3">
-        <f>C26*SimParameters!$B$9</f>
-        <v>1.875E-6</v>
+        <f>C26</f>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -13206,8 +13194,8 @@
         <v>25</v>
       </c>
       <c r="C68" s="3">
-        <f>C27*SimParameters!$B$9</f>
-        <v>1.875E-6</v>
+        <f t="shared" ref="C68:C83" si="2">C27</f>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -13218,8 +13206,8 @@
         <v>26</v>
       </c>
       <c r="C69" s="3">
-        <f>C28*SimParameters!$B$9</f>
-        <v>1.875E-6</v>
+        <f t="shared" si="2"/>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -13230,8 +13218,8 @@
         <v>27</v>
       </c>
       <c r="C70" s="3">
-        <f>C29*SimParameters!$B$9</f>
-        <v>1.8750000000000002E-5</v>
+        <f t="shared" si="2"/>
+        <v>1.5E-5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -13242,8 +13230,8 @@
         <v>28</v>
       </c>
       <c r="C71" s="3">
-        <f>C30*SimParameters!$B$9</f>
-        <v>7.8125000000000002E-5</v>
+        <f t="shared" si="2"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -13254,8 +13242,8 @@
         <v>29</v>
       </c>
       <c r="C72" s="3">
-        <f>C31*SimParameters!$B$9</f>
-        <v>7.8125000000000002E-5</v>
+        <f t="shared" si="2"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -13266,8 +13254,8 @@
         <v>30</v>
       </c>
       <c r="C73" s="3">
-        <f>C32*SimParameters!$B$9</f>
-        <v>7.8125000000000002E-5</v>
+        <f t="shared" si="2"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -13278,8 +13266,8 @@
         <v>31</v>
       </c>
       <c r="C74" s="3">
-        <f>C33*SimParameters!$B$9</f>
-        <v>4.6874999999999993E-4</v>
+        <f t="shared" si="2"/>
+        <v>3.7499999999999995E-4</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -13290,8 +13278,8 @@
         <v>32</v>
       </c>
       <c r="C75" s="3">
-        <f>C34*SimParameters!$B$9</f>
-        <v>1.0937500000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.7500000000000002E-4</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -13302,8 +13290,8 @@
         <v>33</v>
       </c>
       <c r="C76" s="3">
-        <f>C35*SimParameters!$B$9</f>
-        <v>1.7187500000000002E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.3750000000000001E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -13314,8 +13302,8 @@
         <v>34</v>
       </c>
       <c r="C77" s="3">
-        <f>C36*SimParameters!$B$9</f>
-        <v>1.0937500000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.7500000000000008E-3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -13326,8 +13314,8 @@
         <v>35</v>
       </c>
       <c r="C78" s="3">
-        <f>C37*SimParameters!$B$9</f>
-        <v>4.6874999999999998E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -13338,8 +13326,8 @@
         <v>36</v>
       </c>
       <c r="C79" s="3">
-        <f>C38*SimParameters!$B$9</f>
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -13350,8 +13338,8 @@
         <v>37</v>
       </c>
       <c r="C80" s="3">
-        <f>C39*SimParameters!$B$9</f>
-        <v>1.8749999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -13362,8 +13350,8 @@
         <v>38</v>
       </c>
       <c r="C81" s="3">
-        <f>C40*SimParameters!$B$9</f>
-        <v>3.125E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -13374,8 +13362,8 @@
         <v>39</v>
       </c>
       <c r="C82" s="3">
-        <f>C41*SimParameters!$B$9</f>
-        <v>0.625</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -13386,8 +13374,8 @@
         <v>40</v>
       </c>
       <c r="C83" s="3">
-        <f>C42*SimParameters!$B$9</f>
-        <v>0.625</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -13398,7 +13386,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="4">
-        <f>C2*SimParameters!$B$16</f>
+        <f>C2</f>
         <v>0</v>
       </c>
     </row>
@@ -13410,7 +13398,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="4">
-        <f>C3*SimParameters!$B$16</f>
+        <f t="shared" ref="C85:C104" si="3">C3</f>
         <v>0</v>
       </c>
     </row>
@@ -13422,7 +13410,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="4">
-        <f>C4*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13434,7 +13422,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="4">
-        <f>C5*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13446,7 +13434,7 @@
         <v>4</v>
       </c>
       <c r="C88" s="4">
-        <f>C6*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13458,7 +13446,7 @@
         <v>5</v>
       </c>
       <c r="C89" s="4">
-        <f>C7*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13470,7 +13458,7 @@
         <v>6</v>
       </c>
       <c r="C90" s="4">
-        <f>C8*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13482,7 +13470,7 @@
         <v>7</v>
       </c>
       <c r="C91" s="4">
-        <f>C9*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13494,7 +13482,7 @@
         <v>8</v>
       </c>
       <c r="C92" s="4">
-        <f>C10*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13506,7 +13494,7 @@
         <v>9</v>
       </c>
       <c r="C93" s="4">
-        <f>C11*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13518,7 +13506,7 @@
         <v>10</v>
       </c>
       <c r="C94" s="4">
-        <f>C12*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13530,7 +13518,7 @@
         <v>11</v>
       </c>
       <c r="C95" s="4">
-        <f>C13*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13542,7 +13530,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="4">
-        <f>C14*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13554,7 +13542,7 @@
         <v>13</v>
       </c>
       <c r="C97" s="4">
-        <f>C15*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13566,7 +13554,7 @@
         <v>14</v>
       </c>
       <c r="C98" s="4">
-        <f>C16*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13578,7 +13566,7 @@
         <v>15</v>
       </c>
       <c r="C99" s="4">
-        <f>C17*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13590,7 +13578,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="4">
-        <f>C18*SimParameters!$B$16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13602,7 +13590,7 @@
         <v>17</v>
       </c>
       <c r="C101" s="4">
-        <f>C19</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -13614,7 +13602,7 @@
         <v>18</v>
       </c>
       <c r="C102" s="4">
-        <f t="shared" ref="C102:C107" si="1">C20</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -13626,7 +13614,7 @@
         <v>19</v>
       </c>
       <c r="C103" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -13638,7 +13626,7 @@
         <v>20</v>
       </c>
       <c r="C104" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -13650,7 +13638,7 @@
         <v>21</v>
       </c>
       <c r="C105" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C102:C107" si="4">C23</f>
         <v>0.5</v>
       </c>
     </row>
@@ -13662,7 +13650,7 @@
         <v>22</v>
       </c>
       <c r="C106" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
@@ -13674,7 +13662,7 @@
         <v>23</v>
       </c>
       <c r="C107" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>
@@ -13686,8 +13674,8 @@
         <v>24</v>
       </c>
       <c r="C108" s="4">
-        <f>C26*SimParameters!$B$16</f>
-        <v>4.5000000000000001E-6</v>
+        <f>C26</f>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -13698,8 +13686,8 @@
         <v>25</v>
       </c>
       <c r="C109" s="4">
-        <f>C27*SimParameters!$B$16</f>
-        <v>4.5000000000000001E-6</v>
+        <f t="shared" ref="C109:C124" si="5">C27</f>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -13710,8 +13698,8 @@
         <v>26</v>
       </c>
       <c r="C110" s="4">
-        <f>C28*SimParameters!$B$16</f>
-        <v>4.5000000000000001E-6</v>
+        <f t="shared" si="5"/>
+        <v>1.5E-6</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -13722,8 +13710,8 @@
         <v>27</v>
       </c>
       <c r="C111" s="4">
-        <f>C29*SimParameters!$B$16</f>
-        <v>4.5000000000000003E-5</v>
+        <f t="shared" si="5"/>
+        <v>1.5E-5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -13734,8 +13722,8 @@
         <v>28</v>
       </c>
       <c r="C112" s="4">
-        <f>C30*SimParameters!$B$16</f>
-        <v>1.875E-4</v>
+        <f t="shared" si="5"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -13746,8 +13734,8 @@
         <v>29</v>
       </c>
       <c r="C113" s="4">
-        <f>C31*SimParameters!$B$16</f>
-        <v>1.875E-4</v>
+        <f t="shared" si="5"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -13758,8 +13746,8 @@
         <v>30</v>
       </c>
       <c r="C114" s="4">
-        <f>C32*SimParameters!$B$16</f>
-        <v>1.875E-4</v>
+        <f t="shared" si="5"/>
+        <v>6.2500000000000001E-5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -13770,8 +13758,8 @@
         <v>31</v>
       </c>
       <c r="C115" s="4">
-        <f>C33*SimParameters!$B$16</f>
-        <v>1.1249999999999999E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.7499999999999995E-4</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -13782,8 +13770,8 @@
         <v>32</v>
       </c>
       <c r="C116" s="4">
-        <f>C34*SimParameters!$B$16</f>
-        <v>2.6250000000000002E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.7500000000000002E-4</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -13794,8 +13782,8 @@
         <v>33</v>
       </c>
       <c r="C117" s="4">
-        <f>C35*SimParameters!$B$16</f>
-        <v>4.1250000000000002E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.3750000000000001E-3</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -13806,8 +13794,8 @@
         <v>34</v>
       </c>
       <c r="C118" s="4">
-        <f>C36*SimParameters!$B$16</f>
-        <v>2.6250000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.7500000000000008E-3</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -13818,8 +13806,8 @@
         <v>35</v>
       </c>
       <c r="C119" s="4">
-        <f>C37*SimParameters!$B$16</f>
-        <v>1.125E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -13830,8 +13818,8 @@
         <v>36</v>
       </c>
       <c r="C120" s="4">
-        <f>C38*SimParameters!$B$16</f>
-        <v>1.2E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -13842,8 +13830,8 @@
         <v>37</v>
       </c>
       <c r="C121" s="4">
-        <f>C39*SimParameters!$B$16</f>
-        <v>4.4999999999999998E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -13854,8 +13842,8 @@
         <v>38</v>
       </c>
       <c r="C122" s="4">
-        <f>C40*SimParameters!$B$16</f>
-        <v>7.5000000000000011E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -13866,8 +13854,8 @@
         <v>39</v>
       </c>
       <c r="C123" s="4">
-        <f>C41*SimParameters!$B$16</f>
-        <v>1.5</v>
+        <f t="shared" si="5"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -13878,8 +13866,8 @@
         <v>40</v>
       </c>
       <c r="C124" s="4">
-        <f>C42*SimParameters!$B$16</f>
-        <v>1.5</v>
+        <f t="shared" si="5"/>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -13890,25 +13878,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B660230-52FE-B14B-96EF-BB7257C5F721}">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121:C124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -13917,13 +13905,10 @@
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -13933,11 +13918,11 @@
       <c r="C2" s="8">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -13948,7 +13933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -13959,7 +13944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -13973,7 +13958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -13987,7 +13972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -13995,10 +13980,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="8">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -14006,17 +13991,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="D8">
-        <v>0.2</v>
-      </c>
-      <c r="E8">
-        <f>1-((1-D8)^(1/COUNTA(C7:C8)))</f>
-        <v>0.10557280900008414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -14030,7 +14008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0</v>
       </c>
@@ -14038,10 +14016,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -14049,10 +14027,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -14060,10 +14038,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0</v>
       </c>
@@ -14071,17 +14049,14 @@
         <v>11</v>
       </c>
       <c r="C13" s="8">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="D13">
-        <v>0.9</v>
-      </c>
-      <c r="E13">
-        <f>1-((1-D13)^(1/COUNTA(C10:C13)))</f>
-        <v>0.43765867480965093</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1-(1-C13)^COUNT(C10:C13)</f>
+        <v>0.75990000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>0</v>
       </c>
@@ -14089,10 +14064,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>0</v>
       </c>
@@ -14100,10 +14075,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>0</v>
       </c>
@@ -14111,10 +14086,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>0</v>
       </c>
@@ -14122,13 +14097,14 @@
         <v>15</v>
       </c>
       <c r="C17" s="8">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="D17">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C17)^COUNT(C14:C17)</f>
+        <v>0.75990000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>0</v>
       </c>
@@ -14142,7 +14118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>0</v>
       </c>
@@ -14150,10 +14126,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>0</v>
       </c>
@@ -14161,10 +14137,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>0</v>
       </c>
@@ -14172,10 +14148,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="8">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>0</v>
       </c>
@@ -14183,17 +14159,14 @@
         <v>20</v>
       </c>
       <c r="C22" s="8">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="D22">
-        <v>0.9</v>
-      </c>
-      <c r="E22">
-        <f>1-((1-D22)^(1/COUNTA(C19:C22)))</f>
-        <v>0.43765867480965093</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C22)^COUNT(C19:C22)</f>
+        <v>0.75990000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>0</v>
       </c>
@@ -14201,10 +14174,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>0</v>
       </c>
@@ -14212,17 +14185,14 @@
         <v>22</v>
       </c>
       <c r="C24" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D24">
-        <v>0.9</v>
-      </c>
-      <c r="E24">
-        <f>1-((1-D24)^(1/COUNTA(C23:C24)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C24)^COUNT(C23:C24)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>0</v>
       </c>
@@ -14230,10 +14200,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>0</v>
       </c>
@@ -14241,17 +14211,14 @@
         <v>24</v>
       </c>
       <c r="C26" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D26">
-        <v>0.9</v>
-      </c>
-      <c r="E26">
-        <f>1-((1-D26)^(1/COUNTA(C25:C26)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C26)^COUNT(C25:C26)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>0</v>
       </c>
@@ -14259,10 +14226,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>0</v>
       </c>
@@ -14270,17 +14237,14 @@
         <v>26</v>
       </c>
       <c r="C28" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D28">
-        <v>0.9</v>
-      </c>
-      <c r="E28">
-        <f>1-((1-D28)^(1/COUNTA(C27:C28)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C28)^COUNT(C27:C28)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>0</v>
       </c>
@@ -14288,10 +14252,10 @@
         <v>27</v>
       </c>
       <c r="C29" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>0</v>
       </c>
@@ -14299,17 +14263,14 @@
         <v>28</v>
       </c>
       <c r="C30" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D30">
-        <v>0.9</v>
-      </c>
-      <c r="E30">
-        <f>1-((1-D30)^(1/COUNTA(C29:C30)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <f>1-(1-C30)^COUNT(C29:C30)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>0</v>
       </c>
@@ -14317,10 +14278,10 @@
         <v>29</v>
       </c>
       <c r="C31" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>0</v>
       </c>
@@ -14328,17 +14289,14 @@
         <v>30</v>
       </c>
       <c r="C32" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D32">
-        <v>0.9</v>
-      </c>
-      <c r="E32">
-        <f>1-((1-D32)^(1/COUNTA(C31:C32)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1-(1-C32)^COUNT(C31:C32)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>0</v>
       </c>
@@ -14346,10 +14304,10 @@
         <v>31</v>
       </c>
       <c r="C33" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>0</v>
       </c>
@@ -14357,17 +14315,14 @@
         <v>32</v>
       </c>
       <c r="C34" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D34">
-        <v>0.9</v>
-      </c>
-      <c r="E34">
-        <f>1-((1-D34)^(1/COUNTA(C33:C34)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1-(1-C34)^COUNT(C33:C34)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>0</v>
       </c>
@@ -14375,10 +14330,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>0</v>
       </c>
@@ -14386,17 +14341,14 @@
         <v>34</v>
       </c>
       <c r="C36" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D36">
-        <v>0.9</v>
-      </c>
-      <c r="E36">
-        <f>1-((1-D36)^(1/COUNTA(C35:C36)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1-(1-C36)^COUNT(C35:C36)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>0</v>
       </c>
@@ -14404,10 +14356,10 @@
         <v>35</v>
       </c>
       <c r="C37" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>0</v>
       </c>
@@ -14415,17 +14367,14 @@
         <v>36</v>
       </c>
       <c r="C38" s="8">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="D38">
-        <v>0.9</v>
-      </c>
-      <c r="E38">
-        <f>1-((1-D38)^(1/COUNTA(C37:C38)))</f>
-        <v>0.68377223398316211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <f>1-(1-C38)^COUNT(C37:C38)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>0</v>
       </c>
@@ -14438,11 +14387,8 @@
       <c r="D39">
         <v>0.9</v>
       </c>
-      <c r="E39">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>0</v>
       </c>
@@ -14455,11 +14401,8 @@
       <c r="D40">
         <v>0.9</v>
       </c>
-      <c r="E40">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>0</v>
       </c>
@@ -14472,11 +14415,8 @@
       <c r="D41">
         <v>0.9</v>
       </c>
-      <c r="E41">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>0</v>
       </c>
@@ -14489,11 +14429,8 @@
       <c r="D42">
         <v>0.9</v>
       </c>
-      <c r="E42">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -14501,14 +14438,14 @@
         <v>0</v>
       </c>
       <c r="C43" s="3">
-        <f>C2*$F$43</f>
-        <v>0</v>
-      </c>
-      <c r="F43" s="8">
+        <f>C2*$E$43</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="8">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1</v>
       </c>
@@ -14516,11 +14453,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" ref="C44:C46" si="0">C3*$F$43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C44:C46" si="0">C3*$E$43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>1</v>
       </c>
@@ -14532,7 +14469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>1</v>
       </c>
@@ -14544,7 +14481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -14556,7 +14493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -14564,8 +14501,8 @@
         <v>5</v>
       </c>
       <c r="C48" s="3">
-        <f>C7*$F$43</f>
-        <v>0.12100000000000001</v>
+        <f>C7*$E$43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -14576,8 +14513,8 @@
         <v>6</v>
       </c>
       <c r="C49" s="3">
-        <f>C8*$F$43</f>
-        <v>0.12100000000000001</v>
+        <f>C8*$E$43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -14600,8 +14537,8 @@
         <v>8</v>
       </c>
       <c r="C51" s="3">
-        <f>C10*$F$43</f>
-        <v>0.48400000000000004</v>
+        <f>C10*$E$43</f>
+        <v>0.33</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -14612,8 +14549,8 @@
         <v>9</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" ref="C52:C82" si="2">C11*$F$43</f>
-        <v>0.48400000000000004</v>
+        <f t="shared" ref="C52:C79" si="2">C11*$E$43</f>
+        <v>0.33</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -14625,7 +14562,7 @@
       </c>
       <c r="C53" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -14637,7 +14574,7 @@
       </c>
       <c r="C54" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -14649,7 +14586,7 @@
       </c>
       <c r="C55" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -14661,7 +14598,7 @@
       </c>
       <c r="C56" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -14673,7 +14610,7 @@
       </c>
       <c r="C57" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -14685,7 +14622,7 @@
       </c>
       <c r="C58" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -14709,7 +14646,7 @@
       </c>
       <c r="C60" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -14721,7 +14658,7 @@
       </c>
       <c r="C61" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -14733,7 +14670,7 @@
       </c>
       <c r="C62" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -14745,7 +14682,7 @@
       </c>
       <c r="C63" s="3">
         <f t="shared" si="2"/>
-        <v>0.48400000000000004</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -14757,7 +14694,7 @@
       </c>
       <c r="C64" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -14769,7 +14706,7 @@
       </c>
       <c r="C65" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -14781,7 +14718,7 @@
       </c>
       <c r="C66" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -14793,7 +14730,7 @@
       </c>
       <c r="C67" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -14805,7 +14742,7 @@
       </c>
       <c r="C68" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -14817,7 +14754,7 @@
       </c>
       <c r="C69" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -14829,7 +14766,7 @@
       </c>
       <c r="C70" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -14841,7 +14778,7 @@
       </c>
       <c r="C71" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -14853,7 +14790,7 @@
       </c>
       <c r="C72" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -14865,7 +14802,7 @@
       </c>
       <c r="C73" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -14877,7 +14814,7 @@
       </c>
       <c r="C74" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -14889,7 +14826,7 @@
       </c>
       <c r="C75" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -14901,7 +14838,7 @@
       </c>
       <c r="C76" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -14913,7 +14850,7 @@
       </c>
       <c r="C77" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -14925,7 +14862,7 @@
       </c>
       <c r="C78" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -14937,7 +14874,7 @@
       </c>
       <c r="C79" s="3">
         <f t="shared" si="2"/>
-        <v>0.74800000000000011</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -14952,7 +14889,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>1</v>
       </c>
@@ -14964,7 +14901,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>1</v>
       </c>
@@ -14976,7 +14913,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>1</v>
       </c>
@@ -14988,7 +14925,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>2</v>
       </c>
@@ -14996,14 +14933,14 @@
         <v>0</v>
       </c>
       <c r="C84" s="4">
-        <f>C2*$F$84</f>
-        <v>0</v>
-      </c>
-      <c r="F84" s="8">
+        <f>C2*$E$84</f>
+        <v>0</v>
+      </c>
+      <c r="E84" s="8">
         <v>1.2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>2</v>
       </c>
@@ -15011,11 +14948,11 @@
         <v>1</v>
       </c>
       <c r="C85" s="4">
-        <f t="shared" ref="C85:C87" si="5">C3*$F$84</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C85:C87" si="5">C3*$E$84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>2</v>
       </c>
@@ -15027,7 +14964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>2</v>
       </c>
@@ -15039,7 +14976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>2</v>
       </c>
@@ -15051,7 +14988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>2</v>
       </c>
@@ -15059,11 +14996,11 @@
         <v>5</v>
       </c>
       <c r="C89" s="4">
-        <f>C7*$F$84</f>
-        <v>0.13200000000000001</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <f>C7*$E$84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>2</v>
       </c>
@@ -15071,11 +15008,11 @@
         <v>6</v>
       </c>
       <c r="C90" s="4">
-        <f>C8*$F$84</f>
-        <v>0.13200000000000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <f>C8*$E$84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>2</v>
       </c>
@@ -15087,7 +15024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>2</v>
       </c>
@@ -15095,11 +15032,11 @@
         <v>8</v>
       </c>
       <c r="C92" s="4">
-        <f>C10*$F$84</f>
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+        <f>C10*$E$84</f>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>2</v>
       </c>
@@ -15107,11 +15044,11 @@
         <v>9</v>
       </c>
       <c r="C93" s="4">
-        <f t="shared" ref="C93:C123" si="8">C11*$F$84</f>
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="C93:C120" si="8">C11*$E$84</f>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>2</v>
       </c>
@@ -15120,10 +15057,10 @@
       </c>
       <c r="C94" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>2</v>
       </c>
@@ -15132,10 +15069,10 @@
       </c>
       <c r="C95" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>2</v>
       </c>
@@ -15144,7 +15081,7 @@
       </c>
       <c r="C96" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -15156,7 +15093,7 @@
       </c>
       <c r="C97" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -15168,7 +15105,7 @@
       </c>
       <c r="C98" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -15180,7 +15117,7 @@
       </c>
       <c r="C99" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -15204,7 +15141,7 @@
       </c>
       <c r="C101" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -15216,7 +15153,7 @@
       </c>
       <c r="C102" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -15228,7 +15165,7 @@
       </c>
       <c r="C103" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -15240,7 +15177,7 @@
       </c>
       <c r="C104" s="4">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -15252,7 +15189,7 @@
       </c>
       <c r="C105" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -15264,7 +15201,7 @@
       </c>
       <c r="C106" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -15276,7 +15213,7 @@
       </c>
       <c r="C107" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -15288,7 +15225,7 @@
       </c>
       <c r="C108" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -15300,7 +15237,7 @@
       </c>
       <c r="C109" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -15312,7 +15249,7 @@
       </c>
       <c r="C110" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -15324,7 +15261,7 @@
       </c>
       <c r="C111" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -15336,7 +15273,7 @@
       </c>
       <c r="C112" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -15348,7 +15285,7 @@
       </c>
       <c r="C113" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -15360,7 +15297,7 @@
       </c>
       <c r="C114" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -15372,7 +15309,7 @@
       </c>
       <c r="C115" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -15384,7 +15321,7 @@
       </c>
       <c r="C116" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -15396,7 +15333,7 @@
       </c>
       <c r="C117" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -15408,7 +15345,7 @@
       </c>
       <c r="C118" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -15420,7 +15357,7 @@
       </c>
       <c r="C119" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -15432,7 +15369,7 @@
       </c>
       <c r="C120" s="4">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Cleaning up files and uploading revised data generation parameters.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
+++ b/Parameters_Abortion0_8_Preeclampsia0_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E358ED3-2EE4-7F4D-B194-4EA59AB7A172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEB9305-F928-7F41-9262-EDE3FC19F097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="-20500" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="7" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -1089,7 +1089,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1140,12 +1140,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -13146,7 +13140,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" ref="C61:C66" si="1">C23</f>
+        <f t="shared" ref="C64:C66" si="1">C23</f>
         <v>0.5</v>
       </c>
     </row>
@@ -13638,7 +13632,7 @@
         <v>21</v>
       </c>
       <c r="C105" s="4">
-        <f t="shared" ref="C102:C107" si="4">C23</f>
+        <f t="shared" ref="C105:C107" si="4">C23</f>
         <v>0.5</v>
       </c>
     </row>

</xml_diff>